<commit_message>
Adding URI for dano
</commit_message>
<xml_diff>
--- a/data/Ontologies_forRepo.xlsx
+++ b/data/Ontologies_forRepo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbosche\Documents\GitHub\BE-OLS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C504A9CC-FCAD-4EAD-82C0-257046B09A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68D0DFE-0F65-485E-B2B9-402E0FF3396B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="2" xr2:uid="{C460B36E-D875-4E13-ACEB-9CF2004FB6B5}"/>
   </bookViews>
@@ -1607,7 +1607,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6579" uniqueCount="1134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6579" uniqueCount="1135">
   <si>
     <t>Count of Name</t>
   </si>
@@ -5058,13 +5058,16 @@
     <t>https://doi.org/10.1016/j.aei.2025.103761</t>
   </si>
   <si>
-    <t>geosparql</t>
-  </si>
-  <si>
     <t>DAnO is designed to standardize the representation of technical drawing data extracted through computer vision techniques. Focusing on floor plans, DAnO enables the aggregation, integration, and validation of extracted elements by defining key concepts, such as DrawingElement, DisplayElement, and DescriptionElement, and their relationships.</t>
   </si>
   <si>
     <t xml:space="preserve">beo, bot, sbeo, seas </t>
+  </si>
+  <si>
+    <t>https://w3id.org/dano</t>
+  </si>
+  <si>
+    <t>dc, schema, vann, foaf, skos, geosparql</t>
   </si>
 </sst>
 </file>
@@ -25031,10 +25034,10 @@
   <dimension ref="A1:AH126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="L17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q28" sqref="Q28"/>
+      <selection pane="bottomRight" activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -27502,8 +27505,8 @@
       <c r="B28" s="205" t="s">
         <v>1125</v>
       </c>
-      <c r="C28" s="196" t="s">
-        <v>80</v>
+      <c r="C28" s="196">
+        <v>0.2</v>
       </c>
       <c r="D28" s="205">
         <v>2025</v>
@@ -27511,20 +27514,23 @@
       <c r="F28" s="205" t="s">
         <v>13</v>
       </c>
+      <c r="K28" s="205" t="s">
+        <v>198</v>
+      </c>
       <c r="M28" s="205" t="s">
-        <v>1132</v>
-      </c>
-      <c r="N28" s="38" t="s">
-        <v>80</v>
+        <v>1131</v>
+      </c>
+      <c r="N28" s="191" t="s">
+        <v>1133</v>
       </c>
       <c r="O28" s="191" t="s">
         <v>1130</v>
       </c>
       <c r="P28" s="12" t="s">
-        <v>1133</v>
-      </c>
-      <c r="Q28" s="202" t="s">
-        <v>1131</v>
+        <v>1132</v>
+      </c>
+      <c r="Q28" s="201" t="s">
+        <v>1134</v>
       </c>
       <c r="R28" s="184" t="s">
         <v>67</v>
@@ -27542,12 +27548,14 @@
         <v>68</v>
       </c>
       <c r="W28" s="184" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="X28" s="184" t="s">
         <v>67</v>
       </c>
-      <c r="Y28" s="184"/>
+      <c r="Y28" s="184" t="s">
+        <v>67</v>
+      </c>
       <c r="Z28" s="199" t="s">
         <v>68</v>
       </c>
@@ -27558,11 +27566,11 @@
       </c>
       <c r="AC28" s="194">
         <f>COUNTIF(U28:W28, "yes")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD28" s="194">
         <f>COUNTIF(X28:Z28, "yes")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE28" s="194" t="s">
         <v>68</v>
@@ -32995,9 +33003,7 @@
       <c r="M90" t="s">
         <v>508</v>
       </c>
-      <c r="N90" s="198" t="s">
-        <v>80</v>
-      </c>
+      <c r="N90" s="191"/>
       <c r="O90" s="191" t="s">
         <v>509</v>
       </c>
@@ -36477,12 +36483,13 @@
     <hyperlink ref="O69" r:id="rId207" xr:uid="{8F6CA822-1BD4-4EE0-B1E1-9F4149E95A51}"/>
     <hyperlink ref="N69" r:id="rId208" xr:uid="{6C55BAE3-AC52-4A54-ADFB-4C03AECDF46E}"/>
     <hyperlink ref="O28" r:id="rId209" xr:uid="{C4B9ED1E-BBE3-49BD-842E-4772F661899A}"/>
+    <hyperlink ref="N28" r:id="rId210" xr:uid="{8E2664D8-B1A3-4730-A93D-55B9FD57EEDA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId210"/>
-  <legacyDrawing r:id="rId211"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId211"/>
+  <legacyDrawing r:id="rId212"/>
   <tableParts count="1">
-    <tablePart r:id="rId212"/>
+    <tablePart r:id="rId213"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -42268,6 +42275,16 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7e06419a-bc24-4bca-aaf1-3b90bf7d837a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100617EB9F8E3ABAA489A6191778AAEABC8" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ca410b711d7e1dbb3b8812b94cae59a8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7e06419a-bc24-4bca-aaf1-3b90bf7d837a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c5d67c1cae84893d945a781f540d5af9" ns2:_="">
     <xsd:import namespace="7e06419a-bc24-4bca-aaf1-3b90bf7d837a"/>
@@ -42471,16 +42488,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7e06419a-bc24-4bca-aaf1-3b90bf7d837a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -42491,6 +42498,16 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CBC734A-37E0-4A55-B328-89CFAE297459}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7e06419a-bc24-4bca-aaf1-3b90bf7d837a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3977A69D-27CD-4AC0-B4CF-1D599E9E2EF4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -42508,16 +42525,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CBC734A-37E0-4A55-B328-89CFAE297459}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7e06419a-bc24-4bca-aaf1-3b90bf7d837a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1E73802-DE0F-482B-8B75-044CD712CFB1}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Added aic, eco, hmo and fmo
</commit_message>
<xml_diff>
--- a/data/Ontologies_forRepo.xlsx
+++ b/data/Ontologies_forRepo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac.sharepoint.com/sites/EC3-1.ModellingandStandards/Shared Documents/1. Modelling and Standards/Material/Project D_Ontologies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbosche\Documents\GitHub\BE-OLS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{7F8D0847-A4D5-4BFA-BA6D-F8E91FF0BBBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FED8B562-A7C5-461C-A17A-7209D92E1A4A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08029F5A-362F-4634-BB39-1DA1CDDA21F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C460B36E-D875-4E13-ACEB-9CF2004FB6B5}"/>
+    <workbookView xWindow="12495" yWindow="3780" windowWidth="20820" windowHeight="11295" xr2:uid="{C460B36E-D875-4E13-ACEB-9CF2004FB6B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="14" r:id="rId1"/>
@@ -32,6 +32,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -109,32 +112,67 @@
     </comment>
     <comment ref="Z1" authorId="1" shapeId="0" xr:uid="{15ACBA56-A77C-4283-BBC4-F67788C8E63D}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     @Arghavan: one issue we have I think is that there is a difference between explicitly reuse concepts from another ontology and providing some alignment information. I think we need to keep our lives easy and only consider explicit reuse, i.e. explicitly referred to within the owl file</t>
+        </r>
       </text>
     </comment>
     <comment ref="O2" authorId="2" shapeId="0" xr:uid="{FE4BDE30-982D-4AEE-9FF1-D227ED2BE257}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     See also https://www.auto.tuwien.ac.at/downloads/thinkhome/ontology/BuildingOntology.owl</t>
+        </r>
       </text>
     </comment>
     <comment ref="P9" authorId="3" shapeId="0" xr:uid="{885FB683-17A8-485A-8691-53C79CD2DF41}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.freeclass.eu/download
 The Free Class (FC) ontology requires me to give my details to get access. But, it is otherwise an AECO ontology. Should I add it?</t>
+        </r>
       </text>
     </comment>
     <comment ref="Q21" authorId="4" shapeId="0" xr:uid="{973D48F1-79B3-4920-8BDA-8C16C92B26F0}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     This may need to include quantity kind (qk) and unit (unit), that are both from qudt.
@@ -142,19 +180,37 @@
     New list: bacnet, bsh, qudt, qudtqk, rec, ref, s223, sdo, sh, skos, sosa, tag, unit, vcard
 Reply:
     That seems better. Where did you find that list?</t>
+        </r>
       </text>
     </comment>
     <comment ref="O30" authorId="5" shapeId="0" xr:uid="{69563DD9-E157-466B-B7C0-685744C5F29A}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     See also https://www.auto.tuwien.ac.at/downloads/thinkhome/ontology/BuildingOntology.owl</t>
+        </r>
       </text>
     </comment>
     <comment ref="R32" authorId="6" shapeId="0" xr:uid="{4B8EE336-FBE0-47A3-9930-259BDD87F0E2}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Place Reference Theory (PRT) ontology
@@ -167,19 +223,37 @@
     Good question. Either PRT is UPPER, or we consider it AECO (we should change that columns to BE :) ). Please, ask Arghavan for her opinion.
 Reply:
     @Arghavan</t>
+        </r>
       </text>
     </comment>
     <comment ref="O34" authorId="7" shapeId="0" xr:uid="{79AF74C8-61FA-441F-B37E-08E57B208671}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     See also https://cui.unige.ch/isi/onto/citygml2.0.owl</t>
+        </r>
       </text>
     </comment>
     <comment ref="A49" authorId="8" shapeId="0" xr:uid="{F8B9D496-3A44-41C2-9AF2-0758B48A9DD7}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Probably doesn't exist
@@ -195,51 +269,105 @@
     I agree. looks like developers named it as ontology in paper, but in the end its not. Also, Section 5 of paper Conclusions and Future Work "Furthermore, it is recommended to use DOT as a modular core ontology in combination with additional web ontologies as extensions when adding more specific information, e.g. taxonomies for various damage types or national assessment standards. In this regard, three example ontologies have been developed that extend DOT with a taxonomy for damages in reinforced concrete (CDO), mechanical parameters for damaged areas (DMO) and properties based on the German inspection standard DIN 1076" . So maybe it cannot be considered as a separate ontology.
 Reply:
     So, I think we are fine. Because we put "no" to everything on the right. But, maybe we should ask our colleagues for their opinion whether or not to keep it.</t>
+        </r>
       </text>
     </comment>
     <comment ref="A76" authorId="9" shapeId="0" xr:uid="{23BF3BDA-5DFC-4776-A2D7-8F9ADF115349}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     This ontology seems to have 6 sub-modules. Should we add them to our database?</t>
+        </r>
       </text>
     </comment>
     <comment ref="Q76" authorId="10" shapeId="0" xr:uid="{F740CA61-96DA-4774-9A8A-ED9440FE2098}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Should we add the AffectedBy ontology (aff; https://w3id.org/affectedBy#) and the epp ontology (https://w3id.org/eep# ) to our database?</t>
+        </r>
       </text>
     </comment>
     <comment ref="O77" authorId="11" shapeId="0" xr:uid="{62695919-9F9A-40CF-9011-F3B8FA1114C9}">
       <text>
-        <t xml:space="preserve">[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     See also http://semantic.eurobau.com/eurobau-utility.owl </t>
+        </r>
       </text>
     </comment>
     <comment ref="O90" authorId="12" shapeId="0" xr:uid="{9A5C529B-FA1E-4373-8A74-C3F792561B4A}">
       <text>
-        <t xml:space="preserve">[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     See also  http://p-comp.di.uoa.gr/projects/ontonav/INOdoc/index.html </t>
+        </r>
       </text>
     </comment>
     <comment ref="A94" authorId="13" shapeId="0" xr:uid="{0BE7EF65-0D94-4F3A-8D1B-9B7F0932BB6B}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Note: used to be ontology iddo.</t>
+        </r>
       </text>
     </comment>
     <comment ref="Z101" authorId="14" shapeId="0" xr:uid="{51CFF48A-CD78-4902-8B0C-DC9E113097CA}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Occupant Property Taxonomy (2024). DOI: 10.3233/SW-223254
@@ -247,22 +375,41 @@
     If we miss an ontology in our database, just add it :) 
 Reply:
     We don't :) The ontology is extended by developers with this taxonomy in 2024</t>
+        </r>
       </text>
     </comment>
     <comment ref="P110" authorId="15" shapeId="0" xr:uid="{9B4FF538-E0FF-4ED4-A111-F93178D73F43}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     @Arghavan: I notice it refers to brickpatches and geojson. These are not in our database just now. Should we add them?</t>
+        </r>
       </text>
     </comment>
     <comment ref="O116" authorId="16" shapeId="0" xr:uid="{C1CFE5A4-62BC-4FCA-B09F-944B8ACAFADF}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     See also http://www.semanticbim.com/ontologies/residentialBuilding.owl</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -270,7 +417,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3272" uniqueCount="911">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3363" uniqueCount="936">
   <si>
     <t>BE Product (Building)</t>
   </si>
@@ -3006,6 +3153,82 @@
   </si>
   <si>
     <t>Year Issued</t>
+  </si>
+  <si>
+    <t>aic</t>
+  </si>
+  <si>
+    <t>The Agents in Construction (AiC) ontology is a lightweight semantic model for coordinating on-site production in construction. It represents construction agents (human workers, robots, and other autonomous hardware) as they operate on a site: the processes they carry out, the elements they modify, the resources they handle, and the operational modes and metrics used to assess their performance and impact. To express how agent activities evolve over time, AiC introduces meta-properties that specify when a statement holds (at an instant or over an interval), what dimension of information it represents (planned, simulated, or performed), and who generated it. The ontology emphasizes generic, trade-agnostic concepts to ensure broad applicability across project types and delivery methods.</t>
+  </si>
+  <si>
+    <t>https://w3id.org/aic#</t>
+  </si>
+  <si>
+    <t>https://digiconstructlab-tu-delft.github.io/AiC-Ontology/</t>
+  </si>
+  <si>
+    <t>Agents in Construction (AiC) Ontology</t>
+  </si>
+  <si>
+    <t>eco</t>
+  </si>
+  <si>
+    <t>ECO - Eurocode Core Ontology</t>
+  </si>
+  <si>
+    <t>The Eurocode Core Ontology (ECO) provides a formal semantic representation of foundational concepts from the Eurocodes, the European standards for structural design. It enables machine-readable interpretation of regulatory knowledge, supporting automated reasoning, semantic interoperability, and integration with engineering workflows. ECO is designed as a modular, extensible framework for use in intelligent, standards-compliant design tools within the AECO industry.</t>
+  </si>
+  <si>
+    <t>https://mlaura1996.github.io/EC1990/; https://doi.org/10.1016/j.aei.2025.104218</t>
+  </si>
+  <si>
+    <t>bot, omg, beo</t>
+  </si>
+  <si>
+    <t>dct, skos</t>
+  </si>
+  <si>
+    <t>Failure Mechanism Ontology</t>
+  </si>
+  <si>
+    <t>fmo</t>
+  </si>
+  <si>
+    <t>hmo</t>
+  </si>
+  <si>
+    <t>Historic Masonry Ontology</t>
+  </si>
+  <si>
+    <t>https://w3id.org/hmo#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Historic Masonry Ontology (HMO) aims to represent the historic masonry material by considering its heterogeneous nature and defining the configuration of units and joints in the wall. The proposed namespace is , with the preferred prefix hmo.
+The ontology includes reference masonry types and their mechanical parameters, together with a set of SWRL rules to deduce masonry quality and mechanical parameters for any other masonry type. The ontology is designed to be used with other existing ontologies and as a semantic enrichment of Building Information Modeling models, offering a wide range of applications in the field of construction and historic preservation. </t>
+  </si>
+  <si>
+    <t>The primary objective of the Failure Mechanism Ontology (FMO) is to represent masonry walls taking into account features and vulnerabilities that leads to a specific type of failure mechanism. This ontology is complementary to the Historic Masonry Ontology (HMO), of which represents an extension. The recommended prefix for this ontology is FMO, and its proposed namespace is https://w3id.org/fmo#. By utilizing the FMO ontology, it becomes possible to determine whether the structure is more susceptible to out-of-plane collapse or if in-plane failures are more likely. The scope is to facilitate the definition of the modeling assmptions, while employing global models for the structural analysis of unreinforced masonry constructions.</t>
+  </si>
+  <si>
+    <t>https://w3id.org/fmo#</t>
+  </si>
+  <si>
+    <t>https://www.w3id.org/eurocodes/ec1990#</t>
+  </si>
+  <si>
+    <t>https://mlaura1996.github.io/HistoricMasonryOntology/</t>
+  </si>
+  <si>
+    <t>https://mlaura1996.github.io/FailureMechanismOntology/</t>
+  </si>
+  <si>
+    <t>dot, beo, saref, mat</t>
+  </si>
+  <si>
+    <t>dct, vann, foaf, ombibo2</t>
+  </si>
+  <si>
+    <t>dot, beo, hmo</t>
   </si>
 </sst>
 </file>
@@ -3133,7 +3356,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -3175,6 +3398,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -3279,8 +3508,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EFE1469B-541D-4DB3-969C-63DB4F642030}" name="Table2" displayName="Table2" ref="A1:AH140" totalsRowShown="0">
-  <autoFilter ref="A1:AH140" xr:uid="{EFE1469B-541D-4DB3-969C-63DB4F642030}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EFE1469B-541D-4DB3-969C-63DB4F642030}" name="Table2" displayName="Table2" ref="A1:AH144" totalsRowShown="0">
+  <autoFilter ref="A1:AH144" xr:uid="{EFE1469B-541D-4DB3-969C-63DB4F642030}">
     <filterColumn colId="10">
       <filters>
         <filter val="n/d"/>
@@ -3721,47 +3950,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6484B993-682B-477D-B31E-A58D58B7BF22}">
-  <dimension ref="A1:AH140"/>
+  <dimension ref="A1:AH144"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="61" zoomScaleNormal="61" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C133" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomRight" activeCell="A144" sqref="A144"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="126.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="50.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
     <col min="3" max="3" width="10" style="17" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
     <col min="5" max="5" width="22" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" customWidth="1"/>
-    <col min="7" max="7" width="19.5546875" customWidth="1"/>
-    <col min="8" max="8" width="13.44140625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="22.109375" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" customWidth="1"/>
-    <col min="12" max="12" width="16.5546875" customWidth="1"/>
-    <col min="13" max="13" width="18.44140625" customWidth="1"/>
-    <col min="14" max="14" width="21.5546875" customWidth="1"/>
-    <col min="15" max="15" width="12.44140625" customWidth="1"/>
-    <col min="16" max="16" width="26.5546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" customWidth="1"/>
+    <col min="14" max="14" width="21.5703125" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" customWidth="1"/>
+    <col min="16" max="16" width="26.5703125" style="3" customWidth="1"/>
     <col min="17" max="17" width="46" style="3" customWidth="1"/>
-    <col min="18" max="18" width="27.5546875" style="9" customWidth="1"/>
-    <col min="19" max="19" width="34.5546875" style="9" customWidth="1"/>
-    <col min="20" max="20" width="34.109375" style="9" customWidth="1"/>
-    <col min="21" max="21" width="32.109375" style="9" customWidth="1"/>
-    <col min="22" max="22" width="26.109375" style="9" customWidth="1"/>
+    <col min="18" max="18" width="27.5703125" style="9" customWidth="1"/>
+    <col min="19" max="19" width="34.5703125" style="9" customWidth="1"/>
+    <col min="20" max="20" width="34.140625" style="9" customWidth="1"/>
+    <col min="21" max="21" width="32.140625" style="9" customWidth="1"/>
+    <col min="22" max="22" width="26.140625" style="9" customWidth="1"/>
     <col min="23" max="23" width="20" style="9" customWidth="1"/>
-    <col min="24" max="24" width="21.44140625" style="9" customWidth="1"/>
-    <col min="25" max="25" width="19.5546875" style="9" customWidth="1"/>
+    <col min="24" max="24" width="21.42578125" style="9" customWidth="1"/>
+    <col min="25" max="25" width="19.5703125" style="9" customWidth="1"/>
     <col min="26" max="26" width="19" style="9" customWidth="1"/>
-    <col min="27" max="27" width="13.44140625" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="13.42578125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -3865,7 +4094,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>608</v>
       </c>
@@ -3954,7 +4183,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>909</v>
       </c>
@@ -4038,7 +4267,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -4124,7 +4353,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -4219,7 +4448,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>359</v>
       </c>
@@ -4317,7 +4546,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>96</v>
       </c>
@@ -4409,7 +4638,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>87</v>
       </c>
@@ -4504,7 +4733,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>108</v>
       </c>
@@ -4590,7 +4819,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>114</v>
       </c>
@@ -4676,7 +4905,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -4768,7 +4997,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>158</v>
       </c>
@@ -4860,7 +5089,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>382</v>
       </c>
@@ -4952,7 +5181,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>402</v>
       </c>
@@ -5041,7 +5270,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>415</v>
       </c>
@@ -5103,7 +5332,7 @@
         <v>57</v>
       </c>
       <c r="Z15" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA15" s="8" t="s">
         <v>59</v>
@@ -5118,7 +5347,7 @@
       </c>
       <c r="AD15">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AE15" t="s">
         <v>57</v>
@@ -5130,7 +5359,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>118</v>
       </c>
@@ -5222,7 +5451,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>467</v>
       </c>
@@ -5311,7 +5540,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>501</v>
       </c>
@@ -5400,7 +5629,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>576</v>
       </c>
@@ -5489,7 +5718,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>633</v>
       </c>
@@ -5581,7 +5810,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>145</v>
       </c>
@@ -5676,7 +5905,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>153</v>
       </c>
@@ -5765,7 +5994,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -5851,7 +6080,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -5943,7 +6172,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>102</v>
       </c>
@@ -6032,7 +6261,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>659</v>
       </c>
@@ -6113,7 +6342,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>123</v>
       </c>
@@ -6205,7 +6434,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>137</v>
       </c>
@@ -6294,7 +6523,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>129</v>
       </c>
@@ -6386,7 +6615,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>727</v>
       </c>
@@ -6464,7 +6693,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>320</v>
       </c>
@@ -6556,7 +6785,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>178</v>
       </c>
@@ -6651,7 +6880,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>165</v>
       </c>
@@ -6746,7 +6975,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>457</v>
       </c>
@@ -6835,7 +7064,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>333</v>
       </c>
@@ -6924,7 +7153,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>392</v>
       </c>
@@ -7013,7 +7242,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>477</v>
       </c>
@@ -7102,7 +7331,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>484</v>
       </c>
@@ -7191,7 +7420,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>508</v>
       </c>
@@ -7280,7 +7509,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>545</v>
       </c>
@@ -7369,7 +7598,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>171</v>
       </c>
@@ -7461,7 +7690,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>724</v>
       </c>
@@ -7542,7 +7771,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>816</v>
       </c>
@@ -7623,7 +7852,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>725</v>
       </c>
@@ -7707,7 +7936,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>186</v>
       </c>
@@ -7790,7 +8019,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>811</v>
       </c>
@@ -7871,7 +8100,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="47" spans="1:34" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>181</v>
       </c>
@@ -7957,7 +8186,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>822</v>
       </c>
@@ -8038,7 +8267,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="49" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>270</v>
       </c>
@@ -8130,7 +8359,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>284</v>
       </c>
@@ -8222,7 +8451,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>295</v>
       </c>
@@ -8308,7 +8537,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>278</v>
       </c>
@@ -8400,7 +8629,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="53" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>852</v>
       </c>
@@ -8484,7 +8713,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>194</v>
       </c>
@@ -8573,7 +8802,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>201</v>
       </c>
@@ -8662,7 +8891,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="56" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>209</v>
       </c>
@@ -8748,7 +8977,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>221</v>
       </c>
@@ -8837,7 +9066,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>214</v>
       </c>
@@ -8929,7 +9158,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>228</v>
       </c>
@@ -9018,7 +9247,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>198</v>
       </c>
@@ -9099,7 +9328,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>234</v>
       </c>
@@ -9191,7 +9420,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>241</v>
       </c>
@@ -9280,7 +9509,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:34" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>247</v>
       </c>
@@ -9372,7 +9601,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="64" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>253</v>
       </c>
@@ -9461,7 +9690,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="65" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>259</v>
       </c>
@@ -9536,7 +9765,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>262</v>
       </c>
@@ -9617,7 +9846,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="67" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>265</v>
       </c>
@@ -9706,7 +9935,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="68" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>302</v>
       </c>
@@ -9795,7 +10024,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="69" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>426</v>
       </c>
@@ -9884,7 +10113,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="70" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>795</v>
       </c>
@@ -9965,7 +10194,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>289</v>
       </c>
@@ -10057,7 +10286,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="72" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>313</v>
       </c>
@@ -10143,7 +10372,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="73" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>698</v>
       </c>
@@ -10233,7 +10462,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="74" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>697</v>
       </c>
@@ -10323,7 +10552,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="75" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>613</v>
       </c>
@@ -10409,7 +10638,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="76" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>307</v>
       </c>
@@ -10498,7 +10727,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="77" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>327</v>
       </c>
@@ -10587,7 +10816,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="78" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>639</v>
       </c>
@@ -10679,7 +10908,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="79" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>353</v>
       </c>
@@ -10768,7 +10997,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="80" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>348</v>
       </c>
@@ -10857,7 +11086,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="81" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>340</v>
       </c>
@@ -10946,7 +11175,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="82" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>901</v>
       </c>
@@ -11026,7 +11255,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="83" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>665</v>
       </c>
@@ -11113,7 +11342,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="84" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>806</v>
       </c>
@@ -11189,7 +11418,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="85" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>644</v>
       </c>
@@ -11276,7 +11505,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="86" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>845</v>
       </c>
@@ -11360,7 +11589,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="87" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>847</v>
       </c>
@@ -11444,7 +11673,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="88" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>682</v>
       </c>
@@ -11528,7 +11757,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="89" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>371</v>
       </c>
@@ -11626,7 +11855,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="90" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>463</v>
       </c>
@@ -11712,7 +11941,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="91" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>366</v>
       </c>
@@ -11801,7 +12030,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="92" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>378</v>
       </c>
@@ -11887,7 +12116,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="93" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>387</v>
       </c>
@@ -11973,7 +12202,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="94" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>398</v>
       </c>
@@ -12050,7 +12279,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="95" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>407</v>
       </c>
@@ -12142,7 +12371,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="96" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>411</v>
       </c>
@@ -12231,7 +12460,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="97" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>430</v>
       </c>
@@ -12320,7 +12549,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="98" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>421</v>
       </c>
@@ -12409,7 +12638,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="99" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>704</v>
       </c>
@@ -12499,7 +12728,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="100" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>703</v>
       </c>
@@ -12589,7 +12818,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="101" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>440</v>
       </c>
@@ -12678,7 +12907,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="102" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>451</v>
       </c>
@@ -12770,7 +12999,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="103" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>436</v>
       </c>
@@ -12853,7 +13082,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="104" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>676</v>
       </c>
@@ -12937,7 +13166,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="105" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>446</v>
       </c>
@@ -13026,7 +13255,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="106" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>472</v>
       </c>
@@ -13115,7 +13344,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="107" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>273</v>
       </c>
@@ -13198,7 +13427,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="108" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>652</v>
       </c>
@@ -13248,7 +13477,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="109" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>572</v>
       </c>
@@ -13337,7 +13566,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="110" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>490</v>
       </c>
@@ -13424,7 +13653,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="111" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>828</v>
       </c>
@@ -13499,7 +13728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>497</v>
       </c>
@@ -13588,7 +13817,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="113" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>595</v>
       </c>
@@ -13677,7 +13906,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="114" spans="1:34" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>587</v>
       </c>
@@ -13763,7 +13992,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="115" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>590</v>
       </c>
@@ -13852,7 +14081,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="116" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>567</v>
       </c>
@@ -13936,7 +14165,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="117" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>878</v>
       </c>
@@ -14019,7 +14248,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="118" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>856</v>
       </c>
@@ -14114,7 +14343,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="119" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>557</v>
       </c>
@@ -14203,7 +14432,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="120" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>884</v>
       </c>
@@ -14283,7 +14512,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="121" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>857</v>
       </c>
@@ -14375,7 +14604,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="122" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>862</v>
       </c>
@@ -14467,7 +14696,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="123" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>889</v>
       </c>
@@ -14550,7 +14779,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="124" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>872</v>
       </c>
@@ -14630,7 +14859,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="125" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>858</v>
       </c>
@@ -14722,7 +14951,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="126" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>861</v>
       </c>
@@ -14814,7 +15043,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="127" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>860</v>
       </c>
@@ -14906,7 +15135,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="128" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>864</v>
       </c>
@@ -14995,7 +15224,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="129" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>859</v>
       </c>
@@ -15087,7 +15316,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="130" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>895</v>
       </c>
@@ -15167,7 +15396,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="131" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>560</v>
       </c>
@@ -15259,7 +15488,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="132" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>580</v>
       </c>
@@ -15348,7 +15577,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="133" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>583</v>
       </c>
@@ -15437,7 +15666,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="134" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>551</v>
       </c>
@@ -15523,7 +15752,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="135" spans="1:34" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:34" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
         <v>669</v>
       </c>
@@ -15614,7 +15843,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="136" spans="1:34" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:34" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>617</v>
       </c>
@@ -15707,7 +15936,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="137" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>625</v>
       </c>
@@ -15793,7 +16022,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="138" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>629</v>
       </c>
@@ -15851,7 +16080,9 @@
       <c r="Y138" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="Z138" s="18"/>
+      <c r="Z138" s="18" t="s">
+        <v>58</v>
+      </c>
       <c r="AA138" s="8" t="s">
         <v>95</v>
       </c>
@@ -15877,7 +16108,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="139" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>602</v>
       </c>
@@ -15963,7 +16194,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="140" spans="1:34" s="25" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:34" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>621</v>
       </c>
@@ -16053,6 +16284,352 @@
       </c>
       <c r="AG140"/>
       <c r="AH140" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="141" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>915</v>
+      </c>
+      <c r="B141" t="s">
+        <v>911</v>
+      </c>
+      <c r="C141" s="26" t="s">
+        <v>322</v>
+      </c>
+      <c r="D141">
+        <v>2025</v>
+      </c>
+      <c r="F141" t="s">
+        <v>14</v>
+      </c>
+      <c r="K141" t="s">
+        <v>188</v>
+      </c>
+      <c r="M141" s="28" t="s">
+        <v>912</v>
+      </c>
+      <c r="N141" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="O141" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="P141" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q141" s="29" t="s">
+        <v>734</v>
+      </c>
+      <c r="R141" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="S141" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="T141" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="U141" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="V141" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="W141" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="X141" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y141" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z141" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA141" s="8"/>
+      <c r="AB141" s="27">
+        <f t="shared" ref="AB141:AB143" si="15">COUNTIF(R141:T141, "yes")</f>
+        <v>1</v>
+      </c>
+      <c r="AC141" s="27">
+        <f t="shared" ref="AC141:AC143" si="16">COUNTIF(U141:W141, "yes")</f>
+        <v>3</v>
+      </c>
+      <c r="AD141" s="27">
+        <f t="shared" ref="AD141:AD143" si="17">COUNTIF(X141:Z141, "yes")</f>
+        <v>2</v>
+      </c>
+      <c r="AE141" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF141" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG141" s="27"/>
+      <c r="AH141" s="27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="142" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>917</v>
+      </c>
+      <c r="B142" t="s">
+        <v>916</v>
+      </c>
+      <c r="C142" s="17" t="s">
+        <v>315</v>
+      </c>
+      <c r="D142">
+        <v>2025</v>
+      </c>
+      <c r="F142" t="s">
+        <v>838</v>
+      </c>
+      <c r="K142" t="s">
+        <v>329</v>
+      </c>
+      <c r="M142" t="s">
+        <v>918</v>
+      </c>
+      <c r="N142" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="O142" t="s">
+        <v>919</v>
+      </c>
+      <c r="P142" s="3" t="s">
+        <v>920</v>
+      </c>
+      <c r="Q142" s="29" t="s">
+        <v>921</v>
+      </c>
+      <c r="R142" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="S142" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="T142" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="U142" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="V142" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="W142" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="X142" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y142" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z142" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA142" s="8"/>
+      <c r="AB142" s="27">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+      <c r="AC142" s="27">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="AD142" s="27">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="AE142" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF142" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG142" s="27"/>
+      <c r="AH142" s="27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="143" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>922</v>
+      </c>
+      <c r="B143" t="s">
+        <v>923</v>
+      </c>
+      <c r="C143" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D143">
+        <v>2024</v>
+      </c>
+      <c r="F143" t="s">
+        <v>15</v>
+      </c>
+      <c r="G143" t="s">
+        <v>838</v>
+      </c>
+      <c r="K143" t="s">
+        <v>64</v>
+      </c>
+      <c r="M143" t="s">
+        <v>928</v>
+      </c>
+      <c r="N143" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="O143" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="P143" s="3" t="s">
+        <v>935</v>
+      </c>
+      <c r="Q143" s="29" t="s">
+        <v>734</v>
+      </c>
+      <c r="R143" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="S143" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="T143" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="U143" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="V143" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="W143" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="X143" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y143" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z143" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA143" s="8"/>
+      <c r="AB143" s="27">
+        <f t="shared" si="15"/>
+        <v>2</v>
+      </c>
+      <c r="AC143" s="27">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="AD143" s="27">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="AE143" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF143" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG143" s="27"/>
+      <c r="AH143" s="27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="144" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>925</v>
+      </c>
+      <c r="B144" t="s">
+        <v>924</v>
+      </c>
+      <c r="C144" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D144">
+        <v>2024</v>
+      </c>
+      <c r="F144" t="s">
+        <v>0</v>
+      </c>
+      <c r="G144" t="s">
+        <v>1</v>
+      </c>
+      <c r="K144" t="s">
+        <v>64</v>
+      </c>
+      <c r="M144" s="30" t="s">
+        <v>927</v>
+      </c>
+      <c r="N144" s="1" t="s">
+        <v>926</v>
+      </c>
+      <c r="O144" s="1" t="s">
+        <v>931</v>
+      </c>
+      <c r="P144" s="3" t="s">
+        <v>933</v>
+      </c>
+      <c r="Q144" s="29" t="s">
+        <v>934</v>
+      </c>
+      <c r="R144" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="S144" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="T144" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="U144" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="V144" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="W144" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="X144" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y144" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z144" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA144" s="8"/>
+      <c r="AB144" s="27">
+        <f>COUNTIF(R144:T144, "yes")</f>
+        <v>3</v>
+      </c>
+      <c r="AC144" s="27">
+        <f>COUNTIF(U144:W144, "yes")</f>
+        <v>3</v>
+      </c>
+      <c r="AD144" s="27">
+        <f>COUNTIF(X144:Z144, "yes")</f>
+        <v>3</v>
+      </c>
+      <c r="AE144" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF144" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG144" s="27"/>
+      <c r="AH144" s="27" t="s">
         <v>58</v>
       </c>
     </row>
@@ -16293,12 +16870,19 @@
     <hyperlink ref="N130" r:id="rId232" xr:uid="{CF1F8098-F930-45E0-80E5-4564F180CF5A}"/>
     <hyperlink ref="O130" r:id="rId233" xr:uid="{85C86255-2EFE-412B-8C7A-5093F2959238}"/>
     <hyperlink ref="O82" r:id="rId234" xr:uid="{F40C8C8B-C3B0-4FA4-825C-82BC99AA456D}"/>
+    <hyperlink ref="N141" r:id="rId235" xr:uid="{7ADFBE34-97FF-4F43-908A-001BF3B2781E}"/>
+    <hyperlink ref="O141" r:id="rId236" xr:uid="{94710006-BA26-43E2-A645-55FCE25D4FB9}"/>
+    <hyperlink ref="N142" r:id="rId237" xr:uid="{6B27BBF5-6A3F-464E-884F-09439291A1D8}"/>
+    <hyperlink ref="N144" r:id="rId238" display="https://w3id.org/hmo" xr:uid="{7F86E95E-8F78-4306-BDB5-E42739A9F497}"/>
+    <hyperlink ref="N143" r:id="rId239" xr:uid="{D1049976-4189-4098-8B7A-A4FBB294F09E}"/>
+    <hyperlink ref="O144" r:id="rId240" xr:uid="{30C86014-BA17-46D9-869F-D0EB293E3CC6}"/>
+    <hyperlink ref="O143" r:id="rId241" xr:uid="{707EF97C-857E-4A6D-8457-A87CEB3939FC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId235"/>
-  <legacyDrawing r:id="rId236"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId242"/>
+  <legacyDrawing r:id="rId243"/>
   <tableParts count="1">
-    <tablePart r:id="rId237"/>
+    <tablePart r:id="rId244"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -16307,7 +16891,7 @@
           <x14:formula1>
             <xm:f>Domains!$A$2:$A$28</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:G140</xm:sqref>
+          <xm:sqref>F2:G144</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -16323,147 +16907,147 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>835</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>836</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>648</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>843</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>840</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>837</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>841</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>838</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -16482,25 +17066,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7e06419a-bc24-4bca-aaf1-3b90bf7d837a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100617EB9F8E3ABAA489A6191778AAEABC8" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9ff84ddffcc90b35ddafa68a8e3f57c5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7e06419a-bc24-4bca-aaf1-3b90bf7d837a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0aaa14ffaad9a81e002c763535d74184" ns2:_="">
     <xsd:import namespace="7e06419a-bc24-4bca-aaf1-3b90bf7d837a"/>
@@ -16704,25 +17269,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1E73802-DE0F-482B-8B75-044CD712CFB1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7e06419a-bc24-4bca-aaf1-3b90bf7d837a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CBC734A-37E0-4A55-B328-89CFAE297459}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7e06419a-bc24-4bca-aaf1-3b90bf7d837a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54B3783E-F272-4FB2-B0CD-BE7CB395B3FB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16740,6 +17306,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CBC734A-37E0-4A55-B328-89CFAE297459}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7e06419a-bc24-4bca-aaf1-3b90bf7d837a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1E73802-DE0F-482B-8B75-044CD712CFB1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{1faf88fe-a998-4c5b-93c9-210a11d9a5c2}" enabled="0" method="" siteId="{1faf88fe-a998-4c5b-93c9-210a11d9a5c2}" removed="1"/>

</xml_diff>

<commit_message>
Issues 42 and 44
</commit_message>
<xml_diff>
--- a/data/Ontologies_forRepo.xlsx
+++ b/data/Ontologies_forRepo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Іра\BE-OLS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ABDA2F3-AED3-47BC-AFB4-D193EFFF54CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658A5B22-EBB2-4F7C-A5BD-FD95C4CB5A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C460B36E-D875-4E13-ACEB-9CF2004FB6B5}"/>
   </bookViews>
@@ -3069,28 +3069,28 @@
     <t>voaf, foaf, vann, schema, skos, dbr, dbo</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Issued</t>
-  </si>
-  <si>
-    <t>License</t>
-  </si>
-  <si>
-    <t>Conforms To Standart</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Identifier</t>
-  </si>
-  <si>
-    <t>References</t>
-  </si>
-  <si>
     <t>https://saref.etsi.org/saref4city/</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Year Issued</t>
+  </si>
+  <si>
+    <t>Licensing</t>
+  </si>
+  <si>
+    <t>Use+L:Ld Standards</t>
+  </si>
+  <si>
+    <t>Short Description</t>
+  </si>
+  <si>
+    <t>URI</t>
+  </si>
+  <si>
+    <t>Reference</t>
   </si>
 </sst>
 </file>
@@ -3234,7 +3234,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -3276,14 +3276,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
@@ -3406,21 +3398,21 @@
     <sortCondition ref="A1:A140"/>
   </sortState>
   <tableColumns count="34">
-    <tableColumn id="1" xr3:uid="{9A74C9B8-D669-464E-AF30-98194DC54E48}" name="Title"/>
+    <tableColumn id="1" xr3:uid="{9A74C9B8-D669-464E-AF30-98194DC54E48}" name="Name"/>
     <tableColumn id="2" xr3:uid="{73BDDD59-2968-475D-8401-2BF3E8999200}" name="Acronym"/>
     <tableColumn id="3" xr3:uid="{5E6AD3D9-048B-4D2F-B847-6C1A6067C850}" name="Version" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{F5811825-18DF-4D53-8992-1DB0B4736D7E}" name="Issued"/>
+    <tableColumn id="4" xr3:uid="{F5811825-18DF-4D53-8992-1DB0B4736D7E}" name="Year Issued"/>
     <tableColumn id="5" xr3:uid="{8109B890-26AB-4E82-A593-277A5ACB9BEB}" name="Domain (deprecated)"/>
     <tableColumn id="6" xr3:uid="{FB87D2A8-5ECE-421B-BEEB-99CE3D46958C}" name="Primary Domain"/>
     <tableColumn id="7" xr3:uid="{881499B9-131D-4DE5-A339-98DFD60C9A69}" name="Secondary Domain"/>
     <tableColumn id="8" xr3:uid="{7DE7FAE7-F6AC-4DEB-B0A7-79E0910FD899}" name="FAIR - 5 star"/>
     <tableColumn id="9" xr3:uid="{04843D66-C3BB-4164-8392-A39781E8C45C}" name="Level of maintenance"/>
     <tableColumn id="10" xr3:uid="{31FD2BEC-7152-4DA6-ADFB-23A952D38D7D}" name="Level of use"/>
-    <tableColumn id="11" xr3:uid="{E1FC5A2F-8FAA-4353-A30F-F29A7749AB2B}" name="License"/>
-    <tableColumn id="12" xr3:uid="{50E2CFE4-419A-4D16-AEC4-D9C7962383EE}" name="Conforms To Standart"/>
-    <tableColumn id="13" xr3:uid="{5D297276-66F9-4459-BDF9-0A8DBD573003}" name="Description"/>
-    <tableColumn id="14" xr3:uid="{2B3CEEC7-8EDA-4CF0-86E7-B36012BB1130}" name="Identifier"/>
-    <tableColumn id="15" xr3:uid="{33DE9137-9047-46DC-B97D-FC9A03311E62}" name="References"/>
+    <tableColumn id="11" xr3:uid="{E1FC5A2F-8FAA-4353-A30F-F29A7749AB2B}" name="Licensing"/>
+    <tableColumn id="12" xr3:uid="{50E2CFE4-419A-4D16-AEC4-D9C7962383EE}" name="Use+L:Ld Standards"/>
+    <tableColumn id="13" xr3:uid="{5D297276-66F9-4459-BDF9-0A8DBD573003}" name="Short Description"/>
+    <tableColumn id="14" xr3:uid="{2B3CEEC7-8EDA-4CF0-86E7-B36012BB1130}" name="URI"/>
+    <tableColumn id="15" xr3:uid="{33DE9137-9047-46DC-B97D-FC9A03311E62}" name="Reference"/>
     <tableColumn id="16" xr3:uid="{B2A4823A-8123-4352-B2A2-6077AF9C5141}" name="Linked-to ontologies AECO" dataDxfId="18"/>
     <tableColumn id="17" xr3:uid="{22B21384-AC91-4BE5-9B73-D33D0CFF9782}" name="Linked-to ontologies UPPER" dataDxfId="17"/>
     <tableColumn id="19" xr3:uid="{08126F14-AB7C-40B4-B232-7308649DC55E}" name="Linkage to upper ontologies" dataDxfId="16"/>
@@ -3842,7 +3834,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomRight" activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3877,8 +3869,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
-        <v>930</v>
+      <c r="A1" s="27" t="s">
+        <v>931</v>
       </c>
       <c r="B1" t="s">
         <v>20</v>
@@ -3886,8 +3878,8 @@
       <c r="C1" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="32" t="s">
-        <v>931</v>
+      <c r="D1" s="28" t="s">
+        <v>932</v>
       </c>
       <c r="E1" t="s">
         <v>22</v>
@@ -3907,20 +3899,20 @@
       <c r="J1" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="32" t="s">
-        <v>932</v>
-      </c>
-      <c r="L1" s="32" t="s">
+      <c r="K1" s="28" t="s">
         <v>933</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="L1" s="28" t="s">
         <v>934</v>
       </c>
-      <c r="N1" s="31" t="s">
+      <c r="M1" s="28" t="s">
         <v>935</v>
       </c>
-      <c r="O1" s="31" t="s">
+      <c r="N1" s="27" t="s">
         <v>936</v>
+      </c>
+      <c r="O1" s="27" t="s">
+        <v>937</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>28</v>
@@ -5880,30 +5872,26 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:34" s="27" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="27" t="s">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" t="s">
         <v>73</v>
       </c>
-      <c r="C23" s="28">
+      <c r="C23" s="17">
         <v>0.2</v>
       </c>
-      <c r="D23" s="27">
+      <c r="D23">
         <v>2021</v>
       </c>
-      <c r="E23"/>
-      <c r="F23" s="27" t="s">
+      <c r="F23" t="s">
         <v>19</v>
       </c>
-      <c r="H23"/>
-      <c r="I23"/>
-      <c r="J23"/>
-      <c r="K23" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="M23" s="27" t="s">
+      <c r="K23" t="s">
+        <v>66</v>
+      </c>
+      <c r="M23" t="s">
         <v>74</v>
       </c>
       <c r="N23" s="4" t="s">
@@ -5912,61 +5900,61 @@
       <c r="O23" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P23" s="29" t="s">
+      <c r="P23" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="Q23" s="29" t="s">
+      <c r="Q23" s="3" t="s">
         <v>738</v>
       </c>
-      <c r="R23" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="S23" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="T23" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="U23" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="V23" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="W23" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="X23" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y23" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z23" s="30" t="s">
+      <c r="R23" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="S23" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="T23" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="U23" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="V23" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="W23" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="X23" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y23" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z23" s="9" t="s">
         <v>54</v>
       </c>
       <c r="AA23" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AB23" s="27">
+      <c r="AB23">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="AC23" s="27">
+      <c r="AC23">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="AD23" s="27">
+      <c r="AD23">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="AE23" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="AF23" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH23" s="27" t="s">
+      <c r="AE23" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH23" t="s">
         <v>54</v>
       </c>
     </row>
@@ -6232,35 +6220,32 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:34" s="27" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="27" t="s">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>119</v>
       </c>
-      <c r="B27" s="27" t="s">
+      <c r="B27" t="s">
         <v>120</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="D27" s="27">
+      <c r="D27">
         <v>2021</v>
       </c>
       <c r="E27" t="s">
         <v>122</v>
       </c>
-      <c r="F27" s="27" t="s">
+      <c r="F27" t="s">
         <v>10</v>
       </c>
-      <c r="G27" s="27" t="s">
+      <c r="G27" t="s">
         <v>4</v>
       </c>
-      <c r="H27"/>
-      <c r="I27"/>
-      <c r="J27"/>
-      <c r="K27" s="27" t="s">
+      <c r="K27" t="s">
         <v>47</v>
       </c>
-      <c r="M27" s="27" t="s">
+      <c r="M27" t="s">
         <v>123</v>
       </c>
       <c r="N27" s="4" t="s">
@@ -6269,61 +6254,61 @@
       <c r="O27" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="P27" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q27" s="29" t="s">
+      <c r="P27" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q27" s="3" t="s">
         <v>740</v>
       </c>
-      <c r="R27" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="S27" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="T27" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="U27" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="V27" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="W27" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="X27" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y27" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z27" s="30" t="s">
+      <c r="R27" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="S27" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="T27" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="U27" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="V27" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="W27" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="X27" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y27" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z27" s="9" t="s">
         <v>53</v>
       </c>
       <c r="AA27" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="AB27" s="27">
+      <c r="AB27">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="AC27" s="27">
+      <c r="AC27">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="AD27" s="27">
+      <c r="AD27">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="AE27" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="AF27" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH27" s="27" t="s">
+      <c r="AE27" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF27" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH27" t="s">
         <v>54</v>
       </c>
     </row>
@@ -6416,35 +6401,32 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:34" s="27" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="27" t="s">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>125</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" t="s">
         <v>126</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="D29" s="27">
+      <c r="D29">
         <v>2021</v>
       </c>
       <c r="E29" t="s">
         <v>101</v>
       </c>
-      <c r="F29" s="27" t="s">
+      <c r="F29" t="s">
         <v>0</v>
       </c>
-      <c r="H29"/>
-      <c r="I29"/>
-      <c r="J29"/>
-      <c r="K29" s="27" t="s">
+      <c r="K29" t="s">
         <v>128</v>
       </c>
-      <c r="L29" s="27" t="s">
+      <c r="L29" t="s">
         <v>129</v>
       </c>
-      <c r="M29" s="27" t="s">
+      <c r="M29" t="s">
         <v>130</v>
       </c>
       <c r="N29" s="4" t="s">
@@ -6453,61 +6435,61 @@
       <c r="O29" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="P29" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q29" s="29" t="s">
+      <c r="P29" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q29" s="3" t="s">
         <v>741</v>
       </c>
-      <c r="R29" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="S29" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="T29" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="U29" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="V29" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="W29" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="X29" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y29" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z29" s="30" t="s">
+      <c r="R29" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="S29" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="T29" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="U29" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="V29" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="W29" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="X29" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y29" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z29" s="9" t="s">
         <v>53</v>
       </c>
       <c r="AA29" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="AB29" s="27">
+      <c r="AB29">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AC29" s="27">
+      <c r="AC29">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="AD29" s="27">
+      <c r="AD29">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="AE29" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="AF29" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH29" s="27" t="s">
+      <c r="AE29" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF29" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH29" t="s">
         <v>54</v>
       </c>
     </row>
@@ -13323,30 +13305,26 @@
         <v>54</v>
       </c>
     </row>
-    <row r="108" spans="1:34" s="27" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="27" t="s">
+    <row r="108" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
         <v>648</v>
       </c>
-      <c r="B108" s="27" t="s">
+      <c r="B108" t="s">
         <v>649</v>
       </c>
-      <c r="C108" s="28">
+      <c r="C108" s="17">
         <v>2</v>
       </c>
-      <c r="D108" s="27">
+      <c r="D108">
         <v>2016</v>
       </c>
-      <c r="E108"/>
-      <c r="F108" s="27" t="s">
+      <c r="F108" t="s">
         <v>12</v>
       </c>
-      <c r="H108"/>
-      <c r="I108"/>
-      <c r="J108"/>
-      <c r="K108" s="27" t="s">
+      <c r="K108" t="s">
         <v>788</v>
       </c>
-      <c r="M108" s="27" t="s">
+      <c r="M108" t="s">
         <v>789</v>
       </c>
       <c r="N108" s="4" t="s">
@@ -13355,57 +13333,56 @@
       <c r="O108" s="4" t="s">
         <v>837</v>
       </c>
-      <c r="P108" s="29"/>
-      <c r="Q108" s="29" t="s">
+      <c r="Q108" s="3" t="s">
         <v>929</v>
       </c>
-      <c r="R108" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="S108" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="T108" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="U108" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="V108" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="W108" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="X108" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y108" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z108" s="30" t="s">
+      <c r="R108" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="S108" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="T108" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="U108" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="V108" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="W108" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="X108" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y108" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z108" s="9" t="s">
         <v>54</v>
       </c>
       <c r="AA108" s="8"/>
-      <c r="AB108" s="27">
+      <c r="AB108">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="AC108" s="27">
+      <c r="AC108">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="AD108" s="27">
+      <c r="AD108">
         <f t="shared" si="11"/>
         <v>2</v>
       </c>
-      <c r="AE108" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="AF108" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH108" s="27" t="s">
+      <c r="AE108" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF108" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH108" t="s">
         <v>54</v>
       </c>
     </row>
@@ -14819,8 +14796,8 @@
       <c r="M125" t="s">
         <v>518</v>
       </c>
-      <c r="N125" s="33" t="s">
-        <v>937</v>
+      <c r="N125" s="29" t="s">
+        <v>930</v>
       </c>
       <c r="O125" s="1" t="s">
         <v>519</v>

</xml_diff>

<commit_message>
Issue 53. DC columns alignment. Name/Title
</commit_message>
<xml_diff>
--- a/data/Ontologies_forRepo.xlsx
+++ b/data/Ontologies_forRepo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Іра\BE-OLS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3FC047-DD26-4B10-9129-C3B57BECA018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3E666E-9C3E-4D79-B387-830C096149B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C460B36E-D875-4E13-ACEB-9CF2004FB6B5}"/>
   </bookViews>
@@ -3081,9 +3081,6 @@
     <t>Issued</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
     <t>License</t>
   </si>
   <si>
@@ -3133,6 +3130,9 @@
   </si>
   <si>
     <t>https://w3id.org/obpi#</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -3140,7 +3140,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -3221,11 +3221,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -3286,7 +3287,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -3335,18 +3336,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -3465,7 +3463,7 @@
     <sortCondition ref="A1:A140"/>
   </sortState>
   <tableColumns count="34">
-    <tableColumn id="1" xr3:uid="{9A74C9B8-D669-464E-AF30-98194DC54E48}" name="Title"/>
+    <tableColumn id="1" xr3:uid="{9A74C9B8-D669-464E-AF30-98194DC54E48}" name="Name"/>
     <tableColumn id="2" xr3:uid="{73BDDD59-2968-475D-8401-2BF3E8999200}" name="Acronym"/>
     <tableColumn id="3" xr3:uid="{5E6AD3D9-048B-4D2F-B847-6C1A6067C850}" name="Version" dataDxfId="19"/>
     <tableColumn id="4" xr3:uid="{F5811825-18DF-4D53-8992-1DB0B4736D7E}" name="Issued"/>
@@ -3907,7 +3905,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M152" sqref="M152"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3942,8 +3940,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
-        <v>928</v>
+      <c r="A1" s="36" t="s">
+        <v>945</v>
       </c>
       <c r="B1" t="s">
         <v>20</v>
@@ -3973,19 +3971,19 @@
         <v>27</v>
       </c>
       <c r="K1" s="28" t="s">
+        <v>928</v>
+      </c>
+      <c r="L1" s="28" t="s">
         <v>929</v>
       </c>
-      <c r="L1" s="28" t="s">
+      <c r="M1" s="28" t="s">
         <v>930</v>
-      </c>
-      <c r="M1" s="28" t="s">
-        <v>931</v>
       </c>
       <c r="N1" s="27" t="s">
         <v>926</v>
       </c>
       <c r="O1" s="27" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>28</v>
@@ -7998,8 +7996,8 @@
       <c r="O46" s="1" t="s">
         <v>807</v>
       </c>
-      <c r="P46" s="32" t="s">
-        <v>935</v>
+      <c r="P46" s="3" t="s">
+        <v>934</v>
       </c>
       <c r="Q46" s="3" t="s">
         <v>811</v>
@@ -8165,8 +8163,8 @@
       <c r="O48" s="1" t="s">
         <v>807</v>
       </c>
-      <c r="P48" s="32" t="s">
-        <v>936</v>
+      <c r="P48" s="3" t="s">
+        <v>935</v>
       </c>
       <c r="Q48" s="3" t="s">
         <v>811</v>
@@ -10004,7 +10002,7 @@
         <v>422</v>
       </c>
       <c r="N69" s="30" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="P69" s="21" t="s">
         <v>643</v>
@@ -10802,7 +10800,7 @@
         <v>635</v>
       </c>
       <c r="P78" s="21" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="Q78" s="3" t="s">
         <v>636</v>
@@ -11715,7 +11713,7 @@
       <c r="B89" s="31" t="s">
         <v>642</v>
       </c>
-      <c r="C89" s="33" t="s">
+      <c r="C89" s="32" t="s">
         <v>66</v>
       </c>
       <c r="D89" s="31">
@@ -11743,11 +11741,11 @@
       <c r="M89" s="31" t="s">
         <v>370</v>
       </c>
-      <c r="N89" s="34" t="s">
-        <v>934</v>
-      </c>
-      <c r="O89" s="34" t="s">
-        <v>938</v>
+      <c r="N89" s="33" t="s">
+        <v>933</v>
+      </c>
+      <c r="O89" s="33" t="s">
+        <v>937</v>
       </c>
       <c r="P89" s="21" t="s">
         <v>66</v>
@@ -16614,12 +16612,12 @@
     </row>
     <row r="145" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
+        <v>938</v>
+      </c>
+      <c r="B145" s="34" t="s">
         <v>939</v>
       </c>
-      <c r="B145" s="36" t="s">
-        <v>940</v>
-      </c>
-      <c r="C145" s="37">
+      <c r="C145" s="35">
         <v>1</v>
       </c>
       <c r="D145">
@@ -16632,20 +16630,20 @@
         <v>184</v>
       </c>
       <c r="M145" t="s">
+        <v>940</v>
+      </c>
+      <c r="N145" s="30" t="s">
+        <v>944</v>
+      </c>
+      <c r="O145" s="30" t="s">
         <v>941</v>
       </c>
-      <c r="N145" s="30" t="s">
-        <v>945</v>
-      </c>
-      <c r="O145" s="30" t="s">
+      <c r="P145" s="21" t="s">
         <v>942</v>
       </c>
-      <c r="P145" s="21" t="s">
+      <c r="Q145" s="3" t="s">
         <v>943</v>
       </c>
-      <c r="Q145" s="32" t="s">
-        <v>944</v>
-      </c>
       <c r="R145" s="9" t="s">
         <v>53</v>
       </c>
@@ -16674,15 +16672,15 @@
         <v>53</v>
       </c>
       <c r="AA145" s="8"/>
-      <c r="AB145" s="35">
+      <c r="AB145">
         <f>COUNTIF(R145:T145, "yes")</f>
         <v>3</v>
       </c>
-      <c r="AC145" s="35">
+      <c r="AC145">
         <f>COUNTIF(U145:W145, "yes")</f>
         <v>3</v>
       </c>
-      <c r="AD145" s="35">
+      <c r="AD145">
         <f>COUNTIF(X145:Z145, "yes")</f>
         <v>3</v>
       </c>
@@ -16692,7 +16690,6 @@
       <c r="AF145" t="s">
         <v>66</v>
       </c>
-      <c r="AG145" s="35"/>
       <c r="AH145" t="s">
         <v>54</v>
       </c>
@@ -17132,25 +17129,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7e06419a-bc24-4bca-aaf1-3b90bf7d837a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100617EB9F8E3ABAA489A6191778AAEABC8" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9ff84ddffcc90b35ddafa68a8e3f57c5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7e06419a-bc24-4bca-aaf1-3b90bf7d837a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0aaa14ffaad9a81e002c763535d74184" ns2:_="">
     <xsd:import namespace="7e06419a-bc24-4bca-aaf1-3b90bf7d837a"/>
@@ -17354,25 +17332,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CBC734A-37E0-4A55-B328-89CFAE297459}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7e06419a-bc24-4bca-aaf1-3b90bf7d837a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1E73802-DE0F-482B-8B75-044CD712CFB1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7e06419a-bc24-4bca-aaf1-3b90bf7d837a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54B3783E-F272-4FB2-B0CD-BE7CB395B3FB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17390,6 +17369,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1E73802-DE0F-482B-8B75-044CD712CFB1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CBC734A-37E0-4A55-B328-89CFAE297459}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7e06419a-bc24-4bca-aaf1-3b90bf7d837a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{1faf88fe-a998-4c5b-93c9-210a11d9a5c2}" enabled="0" method="" siteId="{1faf88fe-a998-4c5b-93c9-210a11d9a5c2}" removed="1"/>

</xml_diff>

<commit_message>
Issue 53. No DC columns alignment
</commit_message>
<xml_diff>
--- a/data/Ontologies_forRepo.xlsx
+++ b/data/Ontologies_forRepo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Іра\BE-OLS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3E666E-9C3E-4D79-B387-830C096149B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2429B6F-9686-43FA-B3B1-093E78DBD0D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C460B36E-D875-4E13-ACEB-9CF2004FB6B5}"/>
   </bookViews>
@@ -43,6 +43,12 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={71B5F379-C086-4B92-983B-AFC244E3587F}</author>
+    <author>tc={989258E7-9F0B-4F05-8141-0D9109AC5F40}</author>
+    <author>tc={C6B5012E-44BF-4449-9E24-196A2D3017E4}</author>
+    <author>tc={074CC748-731F-4922-9404-3758D4569400}</author>
+    <author>tc={4C2AF009-BCC7-4140-953E-9EBC2CA18C13}</author>
+    <author>tc={A3277E1B-1B1D-452F-92F8-C600F866F5EF}</author>
     <author>Frederic Bosche</author>
     <author>tc={15ACBA56-A77C-4283-BBC4-F67788C8E63D}</author>
     <author>tc={FE4BDE30-982D-4AEE-9FF1-D227ED2BE257}</author>
@@ -64,7 +70,55 @@
     <author>tc={927B62E8-0FF6-4EF1-936E-463477F0E0BD}</author>
   </authors>
   <commentList>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{1FC545F3-2336-4BC5-91B8-D4A837C4557B}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{71B5F379-C086-4B92-983B-AFC244E3587F}">
+      <text>
+        <t>[Ланцюжок приміток]
+Ваша версія Excel дає змогу прочитати цей ланцюжок приміток, проте будь-які зміни в примітці буде вилучено, якщо відкрити цей файл у новішій версії Excel. Докладні відомості: https://go.microsoft.com/fwlink/?linkid=870924.
+Примітка:
+    Title</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="1" shapeId="0" xr:uid="{989258E7-9F0B-4F05-8141-0D9109AC5F40}">
+      <text>
+        <t>[Ланцюжок приміток]
+Ваша версія Excel дає змогу прочитати цей ланцюжок приміток, проте будь-які зміни в примітці буде вилучено, якщо відкрити цей файл у новішій версії Excel. Докладні відомості: https://go.microsoft.com/fwlink/?linkid=870924.
+Примітка:
+    Issued</t>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="2" shapeId="0" xr:uid="{C6B5012E-44BF-4449-9E24-196A2D3017E4}">
+      <text>
+        <t>[Ланцюжок приміток]
+Ваша версія Excel дає змогу прочитати цей ланцюжок приміток, проте будь-які зміни в примітці буде вилучено, якщо відкрити цей файл у новішій версії Excel. Докладні відомості: https://go.microsoft.com/fwlink/?linkid=870924.
+Примітка:
+    License</t>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="3" shapeId="0" xr:uid="{074CC748-731F-4922-9404-3758D4569400}">
+      <text>
+        <t>[Ланцюжок приміток]
+Ваша версія Excel дає змогу прочитати цей ланцюжок приміток, проте будь-які зміни в примітці буде вилучено, якщо відкрити цей файл у новішій версії Excel. Докладні відомості: https://go.microsoft.com/fwlink/?linkid=870924.
+Примітка:
+    Conforms To Standard</t>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="4" shapeId="0" xr:uid="{4C2AF009-BCC7-4140-953E-9EBC2CA18C13}">
+      <text>
+        <t>[Ланцюжок приміток]
+Ваша версія Excel дає змогу прочитати цей ланцюжок приміток, проте будь-які зміни в примітці буде вилучено, якщо відкрити цей файл у новішій версії Excel. Докладні відомості: https://go.microsoft.com/fwlink/?linkid=870924.
+Примітка:
+    Description</t>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="5" shapeId="0" xr:uid="{A3277E1B-1B1D-452F-92F8-C600F866F5EF}">
+      <text>
+        <t>[Ланцюжок приміток]
+Ваша версія Excel дає змогу прочитати цей ланцюжок приміток, проте будь-які зміни в примітці буде вилучено, якщо відкрити цей файл у новішій версії Excel. Докладні відомості: https://go.microsoft.com/fwlink/?linkid=870924.
+Примітка:
+    References</t>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="6" shapeId="0" xr:uid="{1FC545F3-2336-4BC5-91B8-D4A837C4557B}">
       <text>
         <r>
           <rPr>
@@ -88,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{DDC3F8C0-E372-4E58-9BFF-9363BC89A2D0}">
+    <comment ref="Y1" authorId="6" shapeId="0" xr:uid="{DDC3F8C0-E372-4E58-9BFF-9363BC89A2D0}">
       <text>
         <r>
           <rPr>
@@ -112,7 +166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="1" shapeId="0" xr:uid="{15ACBA56-A77C-4283-BBC4-F67788C8E63D}">
+    <comment ref="Z1" authorId="7" shapeId="0" xr:uid="{15ACBA56-A77C-4283-BBC4-F67788C8E63D}">
       <text>
         <t>[Ланцюжок приміток]
 Ваша версія Excel дає змогу прочитати цей ланцюжок приміток, проте будь-які зміни в примітці буде вилучено, якщо відкрити цей файл у новішій версії Excel. Докладні відомості: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -120,7 +174,7 @@
     @Arghavan: one issue we have I think is that there is a difference between explicitly reuse concepts from another ontology and providing some alignment information. I think we need to keep our lives easy and only consider explicit reuse, i.e. explicitly referred to within the owl file</t>
       </text>
     </comment>
-    <comment ref="O2" authorId="2" shapeId="0" xr:uid="{FE4BDE30-982D-4AEE-9FF1-D227ED2BE257}">
+    <comment ref="O2" authorId="8" shapeId="0" xr:uid="{FE4BDE30-982D-4AEE-9FF1-D227ED2BE257}">
       <text>
         <t>[Ланцюжок приміток]
 Ваша версія Excel дає змогу прочитати цей ланцюжок приміток, проте будь-які зміни в примітці буде вилучено, якщо відкрити цей файл у новішій версії Excel. Докладні відомості: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -128,7 +182,7 @@
     See also https://www.auto.tuwien.ac.at/downloads/thinkhome/ontology/BuildingOntology.owl</t>
       </text>
     </comment>
-    <comment ref="P9" authorId="3" shapeId="0" xr:uid="{885FB683-17A8-485A-8691-53C79CD2DF41}">
+    <comment ref="P9" authorId="9" shapeId="0" xr:uid="{885FB683-17A8-485A-8691-53C79CD2DF41}">
       <text>
         <t>[Ланцюжок приміток]
 Ваша версія Excel дає змогу прочитати цей ланцюжок приміток, проте будь-які зміни в примітці буде вилучено, якщо відкрити цей файл у новішій версії Excel. Докладні відомості: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -137,7 +191,7 @@
 The Free Class (FC) ontology requires me to give my details to get access. But, it is otherwise an AECO ontology. Should I add it?</t>
       </text>
     </comment>
-    <comment ref="Q21" authorId="4" shapeId="0" xr:uid="{973D48F1-79B3-4920-8BDA-8C16C92B26F0}">
+    <comment ref="Q21" authorId="10" shapeId="0" xr:uid="{973D48F1-79B3-4920-8BDA-8C16C92B26F0}">
       <text>
         <t>[Ланцюжок приміток]
 Ваша версія Excel дає змогу прочитати цей ланцюжок приміток, проте будь-які зміни в примітці буде вилучено, якщо відкрити цей файл у новішій версії Excel. Докладні відомості: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -149,7 +203,7 @@
     That seems better. Where did you find that list?</t>
       </text>
     </comment>
-    <comment ref="O30" authorId="5" shapeId="0" xr:uid="{69563DD9-E157-466B-B7C0-685744C5F29A}">
+    <comment ref="O30" authorId="11" shapeId="0" xr:uid="{69563DD9-E157-466B-B7C0-685744C5F29A}">
       <text>
         <t>[Ланцюжок приміток]
 Ваша версія Excel дає змогу прочитати цей ланцюжок приміток, проте будь-які зміни в примітці буде вилучено, якщо відкрити цей файл у новішій версії Excel. Докладні відомості: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -157,7 +211,7 @@
     See also https://www.auto.tuwien.ac.at/downloads/thinkhome/ontology/BuildingOntology.owl</t>
       </text>
     </comment>
-    <comment ref="R32" authorId="6" shapeId="0" xr:uid="{4B8EE336-FBE0-47A3-9930-259BDD87F0E2}">
+    <comment ref="R32" authorId="12" shapeId="0" xr:uid="{4B8EE336-FBE0-47A3-9930-259BDD87F0E2}">
       <text>
         <t>[Ланцюжок приміток]
 Ваша версія Excel дає змогу прочитати цей ланцюжок приміток, проте будь-які зміни в примітці буде вилучено, якщо відкрити цей файл у новішій версії Excel. Докладні відомості: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -174,7 +228,7 @@
     @Arghavan</t>
       </text>
     </comment>
-    <comment ref="O34" authorId="7" shapeId="0" xr:uid="{79AF74C8-61FA-441F-B37E-08E57B208671}">
+    <comment ref="O34" authorId="13" shapeId="0" xr:uid="{79AF74C8-61FA-441F-B37E-08E57B208671}">
       <text>
         <t>[Ланцюжок приміток]
 Ваша версія Excel дає змогу прочитати цей ланцюжок приміток, проте будь-які зміни в примітці буде вилучено, якщо відкрити цей файл у новішій версії Excel. Докладні відомості: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -182,7 +236,7 @@
     See also https://cui.unige.ch/isi/onto/citygml2.0.owl</t>
       </text>
     </comment>
-    <comment ref="A49" authorId="8" shapeId="0" xr:uid="{F8B9D496-3A44-41C2-9AF2-0758B48A9DD7}">
+    <comment ref="A49" authorId="14" shapeId="0" xr:uid="{F8B9D496-3A44-41C2-9AF2-0758B48A9DD7}">
       <text>
         <t>[Ланцюжок приміток]
 Ваша версія Excel дає змогу прочитати цей ланцюжок приміток, проте будь-які зміни в примітці буде вилучено, якщо відкрити цей файл у новішій версії Excel. Докладні відомості: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -202,7 +256,7 @@
     So, I think we are fine. Because we put "no" to everything on the right. But, maybe we should ask our colleagues for their opinion whether or not to keep it.</t>
       </text>
     </comment>
-    <comment ref="A76" authorId="9" shapeId="0" xr:uid="{23BF3BDA-5DFC-4776-A2D7-8F9ADF115349}">
+    <comment ref="A76" authorId="15" shapeId="0" xr:uid="{23BF3BDA-5DFC-4776-A2D7-8F9ADF115349}">
       <text>
         <t>[Ланцюжок приміток]
 Ваша версія Excel дає змогу прочитати цей ланцюжок приміток, проте будь-які зміни в примітці буде вилучено, якщо відкрити цей файл у новішій версії Excel. Докладні відомості: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -210,7 +264,7 @@
     This ontology seems to have 6 sub-modules. Should we add them to our database?</t>
       </text>
     </comment>
-    <comment ref="Q76" authorId="10" shapeId="0" xr:uid="{F740CA61-96DA-4774-9A8A-ED9440FE2098}">
+    <comment ref="Q76" authorId="16" shapeId="0" xr:uid="{F740CA61-96DA-4774-9A8A-ED9440FE2098}">
       <text>
         <t>[Ланцюжок приміток]
 Ваша версія Excel дає змогу прочитати цей ланцюжок приміток, проте будь-які зміни в примітці буде вилучено, якщо відкрити цей файл у новішій версії Excel. Докладні відомості: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -218,7 +272,7 @@
     Should we add the AffectedBy ontology (aff; https://w3id.org/affectedBy#) and the epp ontology (https://w3id.org/eep# ) to our database?</t>
       </text>
     </comment>
-    <comment ref="O77" authorId="11" shapeId="0" xr:uid="{62695919-9F9A-40CF-9011-F3B8FA1114C9}">
+    <comment ref="O77" authorId="17" shapeId="0" xr:uid="{62695919-9F9A-40CF-9011-F3B8FA1114C9}">
       <text>
         <t xml:space="preserve">[Ланцюжок приміток]
 Ваша версія Excel дає змогу прочитати цей ланцюжок приміток, проте будь-які зміни в примітці буде вилучено, якщо відкрити цей файл у новішій версії Excel. Докладні відомості: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -226,7 +280,7 @@
     See also http://semantic.eurobau.com/eurobau-utility.owl </t>
       </text>
     </comment>
-    <comment ref="P78" authorId="12" shapeId="0" xr:uid="{1E091BA1-9F74-4A1F-AB26-EF125F3AC8A3}">
+    <comment ref="P78" authorId="18" shapeId="0" xr:uid="{1E091BA1-9F74-4A1F-AB26-EF125F3AC8A3}">
       <text>
         <t>[Ланцюжок приміток]
 Ваша версія Excel дає змогу прочитати цей ланцюжок приміток, проте будь-які зміни в примітці буде вилучено, якщо відкрити цей файл у новішій версії Excel. Докладні відомості: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -234,7 +288,7 @@
     Retired version</t>
       </text>
     </comment>
-    <comment ref="O90" authorId="13" shapeId="0" xr:uid="{9A5C529B-FA1E-4373-8A74-C3F792561B4A}">
+    <comment ref="O90" authorId="19" shapeId="0" xr:uid="{9A5C529B-FA1E-4373-8A74-C3F792561B4A}">
       <text>
         <t xml:space="preserve">[Ланцюжок приміток]
 Ваша версія Excel дає змогу прочитати цей ланцюжок приміток, проте будь-які зміни в примітці буде вилучено, якщо відкрити цей файл у новішій версії Excel. Докладні відомості: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -242,7 +296,7 @@
     See also  http://p-comp.di.uoa.gr/projects/ontonav/INOdoc/index.html </t>
       </text>
     </comment>
-    <comment ref="A94" authorId="14" shapeId="0" xr:uid="{0BE7EF65-0D94-4F3A-8D1B-9B7F0932BB6B}">
+    <comment ref="A94" authorId="20" shapeId="0" xr:uid="{0BE7EF65-0D94-4F3A-8D1B-9B7F0932BB6B}">
       <text>
         <t>[Ланцюжок приміток]
 Ваша версія Excel дає змогу прочитати цей ланцюжок приміток, проте будь-які зміни в примітці буде вилучено, якщо відкрити цей файл у новішій версії Excel. Докладні відомості: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -250,7 +304,7 @@
     Note: used to be ontology iddo.</t>
       </text>
     </comment>
-    <comment ref="Z101" authorId="15" shapeId="0" xr:uid="{51CFF48A-CD78-4902-8B0C-DC9E113097CA}">
+    <comment ref="Z101" authorId="21" shapeId="0" xr:uid="{51CFF48A-CD78-4902-8B0C-DC9E113097CA}">
       <text>
         <t>[Ланцюжок приміток]
 Ваша версія Excel дає змогу прочитати цей ланцюжок приміток, проте будь-які зміни в примітці буде вилучено, якщо відкрити цей файл у новішій версії Excel. Докладні відомості: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -262,7 +316,7 @@
     We don't :) The ontology is extended by developers with this taxonomy in 2024</t>
       </text>
     </comment>
-    <comment ref="P110" authorId="16" shapeId="0" xr:uid="{9B4FF538-E0FF-4ED4-A111-F93178D73F43}">
+    <comment ref="P110" authorId="22" shapeId="0" xr:uid="{9B4FF538-E0FF-4ED4-A111-F93178D73F43}">
       <text>
         <t>[Ланцюжок приміток]
 Ваша версія Excel дає змогу прочитати цей ланцюжок приміток, проте будь-які зміни в примітці буде вилучено, якщо відкрити цей файл у новішій версії Excel. Докладні відомості: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -270,7 +324,7 @@
     @Arghavan: I notice it refers to brickpatches and geojson. These are not in our database just now. Should we add them?</t>
       </text>
     </comment>
-    <comment ref="O116" authorId="17" shapeId="0" xr:uid="{C1CFE5A4-62BC-4FCA-B09F-944B8ACAFADF}">
+    <comment ref="O116" authorId="23" shapeId="0" xr:uid="{C1CFE5A4-62BC-4FCA-B09F-944B8ACAFADF}">
       <text>
         <t>[Ланцюжок приміток]
 Ваша версія Excel дає змогу прочитати цей ланцюжок приміток, проте будь-які зміни в примітці буде вилучено, якщо відкрити цей файл у новішій версії Excel. Докладні відомості: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -278,7 +332,7 @@
     See also http://www.semanticbim.com/ontologies/residentialBuilding.owl</t>
       </text>
     </comment>
-    <comment ref="P145" authorId="18" shapeId="0" xr:uid="{927B62E8-0FF6-4EF1-936E-463477F0E0BD}">
+    <comment ref="P145" authorId="24" shapeId="0" xr:uid="{927B62E8-0FF6-4EF1-936E-463477F0E0BD}">
       <text>
         <t>[Ланцюжок приміток]
 Ваша версія Excel дає змогу прочитати цей ланцюжок приміток, проте будь-які зміни в примітці буде вилучено, якщо відкрити цей файл у новішій версії Excel. Докладні відомості: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -3078,21 +3132,6 @@
     <t>URI</t>
   </si>
   <si>
-    <t>Issued</t>
-  </si>
-  <si>
-    <t>License</t>
-  </si>
-  <si>
-    <t>Conforms To Standard</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>References</t>
-  </si>
-  <si>
     <t>https://pi.pauwel.be/voc/distributionelement</t>
   </si>
   <si>
@@ -3133,6 +3172,21 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Year Issued</t>
+  </si>
+  <si>
+    <t>Licensing</t>
+  </si>
+  <si>
+    <t>Use+L:Ld Standards</t>
+  </si>
+  <si>
+    <t>Short Description</t>
+  </si>
+  <si>
+    <t>Reference</t>
   </si>
 </sst>
 </file>
@@ -3142,7 +3196,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3227,6 +3281,19 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="8">
@@ -3466,18 +3533,18 @@
     <tableColumn id="1" xr3:uid="{9A74C9B8-D669-464E-AF30-98194DC54E48}" name="Name"/>
     <tableColumn id="2" xr3:uid="{73BDDD59-2968-475D-8401-2BF3E8999200}" name="Acronym"/>
     <tableColumn id="3" xr3:uid="{5E6AD3D9-048B-4D2F-B847-6C1A6067C850}" name="Version" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{F5811825-18DF-4D53-8992-1DB0B4736D7E}" name="Issued"/>
+    <tableColumn id="4" xr3:uid="{F5811825-18DF-4D53-8992-1DB0B4736D7E}" name="Year Issued"/>
     <tableColumn id="5" xr3:uid="{8109B890-26AB-4E82-A593-277A5ACB9BEB}" name="Domain (deprecated)"/>
     <tableColumn id="6" xr3:uid="{FB87D2A8-5ECE-421B-BEEB-99CE3D46958C}" name="Primary Domain"/>
     <tableColumn id="7" xr3:uid="{881499B9-131D-4DE5-A339-98DFD60C9A69}" name="Secondary Domain"/>
     <tableColumn id="8" xr3:uid="{7DE7FAE7-F6AC-4DEB-B0A7-79E0910FD899}" name="FAIR - 5 star"/>
     <tableColumn id="9" xr3:uid="{04843D66-C3BB-4164-8392-A39781E8C45C}" name="Level of maintenance"/>
     <tableColumn id="10" xr3:uid="{31FD2BEC-7152-4DA6-ADFB-23A952D38D7D}" name="Level of use"/>
-    <tableColumn id="11" xr3:uid="{E1FC5A2F-8FAA-4353-A30F-F29A7749AB2B}" name="License"/>
-    <tableColumn id="12" xr3:uid="{50E2CFE4-419A-4D16-AEC4-D9C7962383EE}" name="Conforms To Standard"/>
-    <tableColumn id="13" xr3:uid="{5D297276-66F9-4459-BDF9-0A8DBD573003}" name="Description"/>
+    <tableColumn id="11" xr3:uid="{E1FC5A2F-8FAA-4353-A30F-F29A7749AB2B}" name="Licensing"/>
+    <tableColumn id="12" xr3:uid="{50E2CFE4-419A-4D16-AEC4-D9C7962383EE}" name="Use+L:Ld Standards"/>
+    <tableColumn id="13" xr3:uid="{5D297276-66F9-4459-BDF9-0A8DBD573003}" name="Short Description"/>
     <tableColumn id="14" xr3:uid="{2B3CEEC7-8EDA-4CF0-86E7-B36012BB1130}" name="URI"/>
-    <tableColumn id="15" xr3:uid="{33DE9137-9047-46DC-B97D-FC9A03311E62}" name="References"/>
+    <tableColumn id="15" xr3:uid="{33DE9137-9047-46DC-B97D-FC9A03311E62}" name="Reference"/>
     <tableColumn id="16" xr3:uid="{B2A4823A-8123-4352-B2A2-6077AF9C5141}" name="Linked-to ontologies AECO" dataDxfId="18"/>
     <tableColumn id="17" xr3:uid="{22B21384-AC91-4BE5-9B73-D33D0CFF9782}" name="Linked-to ontologies UPPER" dataDxfId="17"/>
     <tableColumn id="19" xr3:uid="{08126F14-AB7C-40B4-B232-7308649DC55E}" name="Linkage to upper ontologies" dataDxfId="16"/>
@@ -3771,6 +3838,24 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2026-01-15T12:19:02.78" personId="{1897075C-2302-4D30-BAB3-34D253D1BE65}" id="{71B5F379-C086-4B92-983B-AFC244E3587F}">
+    <text>Title</text>
+  </threadedComment>
+  <threadedComment ref="D1" dT="2026-01-15T12:19:26.06" personId="{1897075C-2302-4D30-BAB3-34D253D1BE65}" id="{989258E7-9F0B-4F05-8141-0D9109AC5F40}">
+    <text>Issued</text>
+  </threadedComment>
+  <threadedComment ref="K1" dT="2026-01-15T12:20:11.84" personId="{1897075C-2302-4D30-BAB3-34D253D1BE65}" id="{C6B5012E-44BF-4449-9E24-196A2D3017E4}">
+    <text>License</text>
+  </threadedComment>
+  <threadedComment ref="L1" dT="2026-01-15T12:20:35.38" personId="{1897075C-2302-4D30-BAB3-34D253D1BE65}" id="{074CC748-731F-4922-9404-3758D4569400}">
+    <text>Conforms To Standard</text>
+  </threadedComment>
+  <threadedComment ref="M1" dT="2026-01-15T12:21:10.47" personId="{1897075C-2302-4D30-BAB3-34D253D1BE65}" id="{4C2AF009-BCC7-4140-953E-9EBC2CA18C13}">
+    <text>Description</text>
+  </threadedComment>
+  <threadedComment ref="O1" dT="2026-01-15T12:21:49.70" personId="{1897075C-2302-4D30-BAB3-34D253D1BE65}" id="{A3277E1B-1B1D-452F-92F8-C600F866F5EF}">
+    <text>References</text>
+  </threadedComment>
   <threadedComment ref="Z1" dT="2025-01-26T10:26:15.62" personId="{0EE3F1E9-506E-4FC5-A865-C5CF5A3B9A85}" id="{15ACBA56-A77C-4283-BBC4-F67788C8E63D}">
     <text>@Arghavan: one issue we have I think is that there is a difference between explicitly reuse concepts from another ontology and providing some alignment information. I think we need to keep our lives easy and only consider explicit reuse, i.e. explicitly referred to within the owl file</text>
   </threadedComment>
@@ -3905,7 +3990,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3940,8 +4025,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A1" s="36" t="s">
-        <v>945</v>
+      <c r="A1" s="27" t="s">
+        <v>940</v>
       </c>
       <c r="B1" t="s">
         <v>20</v>
@@ -3950,7 +4035,7 @@
         <v>21</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>927</v>
+        <v>941</v>
       </c>
       <c r="E1" t="s">
         <v>22</v>
@@ -3971,19 +4056,19 @@
         <v>27</v>
       </c>
       <c r="K1" s="28" t="s">
-        <v>928</v>
+        <v>942</v>
       </c>
       <c r="L1" s="28" t="s">
-        <v>929</v>
+        <v>943</v>
       </c>
       <c r="M1" s="28" t="s">
-        <v>930</v>
-      </c>
-      <c r="N1" s="27" t="s">
+        <v>944</v>
+      </c>
+      <c r="N1" s="36" t="s">
         <v>926</v>
       </c>
       <c r="O1" s="27" t="s">
-        <v>931</v>
+        <v>945</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>28</v>
@@ -7997,7 +8082,7 @@
         <v>807</v>
       </c>
       <c r="P46" s="3" t="s">
-        <v>934</v>
+        <v>929</v>
       </c>
       <c r="Q46" s="3" t="s">
         <v>811</v>
@@ -8164,7 +8249,7 @@
         <v>807</v>
       </c>
       <c r="P48" s="3" t="s">
-        <v>935</v>
+        <v>930</v>
       </c>
       <c r="Q48" s="3" t="s">
         <v>811</v>
@@ -10002,7 +10087,7 @@
         <v>422</v>
       </c>
       <c r="N69" s="30" t="s">
-        <v>932</v>
+        <v>927</v>
       </c>
       <c r="P69" s="21" t="s">
         <v>643</v>
@@ -10800,7 +10885,7 @@
         <v>635</v>
       </c>
       <c r="P78" s="21" t="s">
-        <v>936</v>
+        <v>931</v>
       </c>
       <c r="Q78" s="3" t="s">
         <v>636</v>
@@ -11742,10 +11827,10 @@
         <v>370</v>
       </c>
       <c r="N89" s="33" t="s">
-        <v>933</v>
+        <v>928</v>
       </c>
       <c r="O89" s="33" t="s">
-        <v>937</v>
+        <v>932</v>
       </c>
       <c r="P89" s="21" t="s">
         <v>66</v>
@@ -16612,10 +16697,10 @@
     </row>
     <row r="145" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>938</v>
+        <v>933</v>
       </c>
       <c r="B145" s="34" t="s">
-        <v>939</v>
+        <v>934</v>
       </c>
       <c r="C145" s="35">
         <v>1</v>
@@ -16630,19 +16715,19 @@
         <v>184</v>
       </c>
       <c r="M145" t="s">
-        <v>940</v>
+        <v>935</v>
       </c>
       <c r="N145" s="30" t="s">
-        <v>944</v>
+        <v>939</v>
       </c>
       <c r="O145" s="30" t="s">
-        <v>941</v>
+        <v>936</v>
       </c>
       <c r="P145" s="21" t="s">
-        <v>942</v>
+        <v>937</v>
       </c>
       <c r="Q145" s="3" t="s">
-        <v>943</v>
+        <v>938</v>
       </c>
       <c r="R145" s="9" t="s">
         <v>53</v>
@@ -17129,6 +17214,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7e06419a-bc24-4bca-aaf1-3b90bf7d837a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100617EB9F8E3ABAA489A6191778AAEABC8" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9ff84ddffcc90b35ddafa68a8e3f57c5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7e06419a-bc24-4bca-aaf1-3b90bf7d837a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0aaa14ffaad9a81e002c763535d74184" ns2:_="">
     <xsd:import namespace="7e06419a-bc24-4bca-aaf1-3b90bf7d837a"/>
@@ -17332,26 +17436,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CBC734A-37E0-4A55-B328-89CFAE297459}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7e06419a-bc24-4bca-aaf1-3b90bf7d837a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7e06419a-bc24-4bca-aaf1-3b90bf7d837a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1E73802-DE0F-482B-8B75-044CD712CFB1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54B3783E-F272-4FB2-B0CD-BE7CB395B3FB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17369,24 +17472,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1E73802-DE0F-482B-8B75-044CD712CFB1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CBC734A-37E0-4A55-B328-89CFAE297459}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7e06419a-bc24-4bca-aaf1-3b90bf7d837a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{1faf88fe-a998-4c5b-93c9-210a11d9a5c2}" enabled="0" method="" siteId="{1faf88fe-a998-4c5b-93c9-210a11d9a5c2}" removed="1"/>

</xml_diff>

<commit_message>
Error Fixes to Ontology Field Display
</commit_message>
<xml_diff>
--- a/data/Ontologies_forRepo.xlsx
+++ b/data/Ontologies_forRepo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbosche\Documents\GitHub\BE-OLS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0F534C-6E14-4C76-B760-B6E5DA40CF99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{317C2D0E-7B72-4308-AD07-27F4EDA35815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5460,7 +5460,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CD145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -28233,25 +28235,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7e06419a-bc24-4bca-aaf1-3b90bf7d837a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100617EB9F8E3ABAA489A6191778AAEABC8" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="be0c97903f599d62d21cd63252cde9aa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7e06419a-bc24-4bca-aaf1-3b90bf7d837a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="784cf5edc76b43144e46369ffdbd4f65" ns2:_="">
     <xsd:import namespace="7e06419a-bc24-4bca-aaf1-3b90bf7d837a"/>
@@ -28455,25 +28438,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57874B87-94C2-4EC8-911D-8271965282CB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7e06419a-bc24-4bca-aaf1-3b90bf7d837a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5798C2B9-ADF6-4B63-9E02-5C931B722A0C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7e06419a-bc24-4bca-aaf1-3b90bf7d837a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1130DA5C-7101-4542-A84A-ADC9A3A2005F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -28489,4 +28473,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5798C2B9-ADF6-4B63-9E02-5C931B722A0C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57874B87-94C2-4EC8-911D-8271965282CB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7e06419a-bc24-4bca-aaf1-3b90bf7d837a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
ADDED: FOOPs Query + Annotation Coverage Calculation
</commit_message>
<xml_diff>
--- a/data/Ontologies_forRepo.xlsx
+++ b/data/Ontologies_forRepo.xlsx
@@ -985,8 +985,12 @@
       <c r="AQ2" t="inlineStr"/>
       <c r="AR2" t="inlineStr"/>
       <c r="AS2" t="inlineStr"/>
-      <c r="AT2" t="inlineStr"/>
-      <c r="AU2" t="inlineStr"/>
+      <c r="AT2" t="n">
+        <v>0.6722222</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>0.6722222</v>
+      </c>
       <c r="AV2" t="inlineStr"/>
       <c r="AW2" t="inlineStr"/>
       <c r="AX2" t="inlineStr"/>
@@ -1223,8 +1227,12 @@
       <c r="AQ3" t="inlineStr"/>
       <c r="AR3" t="inlineStr"/>
       <c r="AS3" t="inlineStr"/>
-      <c r="AT3" t="inlineStr"/>
-      <c r="AU3" t="inlineStr"/>
+      <c r="AT3" t="n">
+        <v>0.14583333</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>0.14583333</v>
+      </c>
       <c r="AV3" t="inlineStr"/>
       <c r="AW3" t="inlineStr"/>
       <c r="AX3" t="inlineStr"/>
@@ -1477,9 +1485,11 @@
       <c r="AS4" t="n">
         <v>15</v>
       </c>
-      <c r="AT4" t="inlineStr"/>
+      <c r="AT4" t="n">
+        <v>0.104166664</v>
+      </c>
       <c r="AU4" t="n">
-        <v>15</v>
+        <v>0.104166664</v>
       </c>
       <c r="AV4" t="inlineStr"/>
       <c r="AW4" t="inlineStr"/>
@@ -1745,8 +1755,12 @@
       <c r="AQ5" t="inlineStr"/>
       <c r="AR5" t="inlineStr"/>
       <c r="AS5" t="inlineStr"/>
-      <c r="AT5" t="inlineStr"/>
-      <c r="AU5" t="inlineStr"/>
+      <c r="AT5" t="n">
+        <v>0.6979166999999999</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>0.6979166999999999</v>
+      </c>
       <c r="AV5" t="inlineStr"/>
       <c r="AW5" t="inlineStr"/>
       <c r="AX5" t="inlineStr"/>
@@ -1787,12 +1801,12 @@
       <c r="BM5" t="inlineStr"/>
       <c r="BN5" t="inlineStr">
         <is>
-          <t>n39bb303ddb28459489b3fd0a0fb4c73ab1</t>
+          <t>n3244b1251ee04b699f21ebdd1500db17b1</t>
         </is>
       </c>
       <c r="BO5" t="inlineStr">
         <is>
-          <t>['n39bb303ddb28459489b3fd0a0fb4c73ab1']</t>
+          <t>['n3244b1251ee04b699f21ebdd1500db17b1']</t>
         </is>
       </c>
       <c r="BP5" t="inlineStr"/>
@@ -1982,9 +1996,11 @@
       <c r="AS6" t="n">
         <v>15</v>
       </c>
-      <c r="AT6" t="inlineStr"/>
+      <c r="AT6" t="n">
+        <v>0.65871125</v>
+      </c>
       <c r="AU6" t="n">
-        <v>15</v>
+        <v>0.65871125</v>
       </c>
       <c r="AV6" t="inlineStr"/>
       <c r="AW6" t="inlineStr"/>
@@ -2034,12 +2050,12 @@
       </c>
       <c r="BN6" t="inlineStr">
         <is>
-          <t>n7bd07ab275dc4507a3c1fb54b401dc13b1</t>
+          <t>nae7ce59cd1c74adb908fa80b10955ab5b1</t>
         </is>
       </c>
       <c r="BO6" t="inlineStr">
         <is>
-          <t>['n7bd07ab275dc4507a3c1fb54b401dc13b1']</t>
+          <t>['nae7ce59cd1c74adb908fa80b10955ab5b1']</t>
         </is>
       </c>
       <c r="BP6" t="inlineStr"/>
@@ -2083,7 +2099,7 @@
         <v>3</v>
       </c>
       <c r="CD6" t="n">
-        <v>1</v>
+        <v>1.239</v>
       </c>
     </row>
     <row r="7">
@@ -2224,8 +2240,12 @@
       <c r="AQ7" t="inlineStr"/>
       <c r="AR7" t="inlineStr"/>
       <c r="AS7" t="inlineStr"/>
-      <c r="AT7" t="inlineStr"/>
-      <c r="AU7" t="inlineStr"/>
+      <c r="AT7" t="n">
+        <v>0.104166664</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>0.104166664</v>
+      </c>
       <c r="AV7" t="inlineStr"/>
       <c r="AW7" t="inlineStr"/>
       <c r="AX7" t="inlineStr"/>
@@ -2424,8 +2444,12 @@
       <c r="AQ8" t="inlineStr"/>
       <c r="AR8" t="inlineStr"/>
       <c r="AS8" t="inlineStr"/>
-      <c r="AT8" t="inlineStr"/>
-      <c r="AU8" t="inlineStr"/>
+      <c r="AT8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>0</v>
+      </c>
       <c r="AV8" t="inlineStr">
         <is>
           <t>ISO/CEN 23386, ISO/CEN 23387</t>
@@ -2674,9 +2698,11 @@
       <c r="AS9" t="n">
         <v>22</v>
       </c>
-      <c r="AT9" t="inlineStr"/>
+      <c r="AT9" t="n">
+        <v>0</v>
+      </c>
       <c r="AU9" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="AV9" t="inlineStr">
         <is>
@@ -2918,9 +2944,11 @@
       <c r="AS10" t="n">
         <v>15</v>
       </c>
-      <c r="AT10" t="inlineStr"/>
+      <c r="AT10" t="n">
+        <v>0</v>
+      </c>
       <c r="AU10" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AV10" t="inlineStr"/>
       <c r="AW10" t="inlineStr"/>
@@ -3182,8 +3210,12 @@
         </is>
       </c>
       <c r="AS11" t="inlineStr"/>
-      <c r="AT11" t="inlineStr"/>
-      <c r="AU11" t="inlineStr"/>
+      <c r="AT11" t="n">
+        <v>0.6666666999999999</v>
+      </c>
+      <c r="AU11" t="n">
+        <v>0.6666666999999999</v>
+      </c>
       <c r="AV11" t="inlineStr"/>
       <c r="AW11" t="inlineStr"/>
       <c r="AX11" t="inlineStr"/>
@@ -3224,12 +3256,12 @@
       <c r="BM11" t="inlineStr"/>
       <c r="BN11" t="inlineStr">
         <is>
-          <t>nd4d092c0bb0b4b53a9bd515673ed020cb1</t>
+          <t>n34c3ada48c28465f83ed8415f038363bb1</t>
         </is>
       </c>
       <c r="BO11" t="inlineStr">
         <is>
-          <t>['nd4d092c0bb0b4b53a9bd515673ed020cb1']</t>
+          <t>['n34c3ada48c28465f83ed8415f038363bb1']</t>
         </is>
       </c>
       <c r="BP11" t="inlineStr"/>
@@ -3388,8 +3420,12 @@
       <c r="AQ12" t="inlineStr"/>
       <c r="AR12" t="inlineStr"/>
       <c r="AS12" t="inlineStr"/>
-      <c r="AT12" t="inlineStr"/>
-      <c r="AU12" t="inlineStr"/>
+      <c r="AT12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU12" t="n">
+        <v>0</v>
+      </c>
       <c r="AV12" t="inlineStr"/>
       <c r="AW12" t="inlineStr"/>
       <c r="AX12" t="inlineStr"/>
@@ -3576,9 +3612,11 @@
       <c r="AS13" t="n">
         <v>15</v>
       </c>
-      <c r="AT13" t="inlineStr"/>
+      <c r="AT13" t="n">
+        <v>0</v>
+      </c>
       <c r="AU13" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AV13" t="inlineStr"/>
       <c r="AW13" t="inlineStr"/>
@@ -3766,9 +3804,11 @@
       <c r="AS14" t="n">
         <v>15</v>
       </c>
-      <c r="AT14" t="inlineStr"/>
+      <c r="AT14" t="n">
+        <v>0</v>
+      </c>
       <c r="AU14" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AV14" t="inlineStr"/>
       <c r="AW14" t="inlineStr"/>
@@ -3994,9 +4034,11 @@
       <c r="AS15" t="n">
         <v>15</v>
       </c>
-      <c r="AT15" t="inlineStr"/>
+      <c r="AT15" t="n">
+        <v>0.104166664</v>
+      </c>
       <c r="AU15" t="n">
-        <v>15</v>
+        <v>0.104166664</v>
       </c>
       <c r="AV15" t="inlineStr"/>
       <c r="AW15" t="inlineStr"/>
@@ -4253,8 +4295,12 @@
       <c r="AQ16" t="inlineStr"/>
       <c r="AR16" t="inlineStr"/>
       <c r="AS16" t="inlineStr"/>
-      <c r="AT16" t="inlineStr"/>
-      <c r="AU16" t="inlineStr"/>
+      <c r="AT16" t="n">
+        <v>0.104166664</v>
+      </c>
+      <c r="AU16" t="n">
+        <v>0.104166664</v>
+      </c>
       <c r="AV16" t="inlineStr"/>
       <c r="AW16" t="inlineStr"/>
       <c r="AX16" t="inlineStr"/>
@@ -4352,7 +4398,7 @@
         <v>3</v>
       </c>
       <c r="CD16" t="n">
-        <v>2</v>
+        <v>1.986</v>
       </c>
     </row>
     <row r="17">
@@ -4530,8 +4576,12 @@
         </is>
       </c>
       <c r="AS17" t="inlineStr"/>
-      <c r="AT17" t="inlineStr"/>
-      <c r="AU17" t="inlineStr"/>
+      <c r="AT17" t="n">
+        <v>0.8611111</v>
+      </c>
+      <c r="AU17" t="n">
+        <v>0.8611111</v>
+      </c>
       <c r="AV17" t="inlineStr">
         <is>
           <t>ISO-12006</t>
@@ -4792,8 +4842,12 @@
         </is>
       </c>
       <c r="AS18" t="inlineStr"/>
-      <c r="AT18" t="inlineStr"/>
-      <c r="AU18" t="inlineStr"/>
+      <c r="AT18" t="n">
+        <v>0.6597222700000001</v>
+      </c>
+      <c r="AU18" t="n">
+        <v>0.6597222700000001</v>
+      </c>
       <c r="AV18" t="inlineStr"/>
       <c r="AW18" t="inlineStr"/>
       <c r="AX18" t="inlineStr"/>
@@ -4834,12 +4888,12 @@
       <c r="BM18" t="inlineStr"/>
       <c r="BN18" t="inlineStr">
         <is>
-          <t>nebe1d6eb1f264cada3404dcc572dbf92b8, nebe1d6eb1f264cada3404dcc572dbf92b9, nebe1d6eb1f264cada3404dcc572dbf92b10, nebe1d6eb1f264cada3404dcc572dbf92b11</t>
+          <t>n31739d9d92ad40e59072f273b243dbe2b8, n31739d9d92ad40e59072f273b243dbe2b9, n31739d9d92ad40e59072f273b243dbe2b10, n31739d9d92ad40e59072f273b243dbe2b11</t>
         </is>
       </c>
       <c r="BO18" t="inlineStr">
         <is>
-          <t>['nebe1d6eb1f264cada3404dcc572dbf92b8', 'nebe1d6eb1f264cada3404dcc572dbf92b9', 'nebe1d6eb1f264cada3404dcc572dbf92b10', 'nebe1d6eb1f264cada3404dcc572dbf92b11']</t>
+          <t>['n31739d9d92ad40e59072f273b243dbe2b8', 'n31739d9d92ad40e59072f273b243dbe2b9', 'n31739d9d92ad40e59072f273b243dbe2b10', 'n31739d9d92ad40e59072f273b243dbe2b11']</t>
         </is>
       </c>
       <c r="BP18" t="inlineStr"/>
@@ -5048,9 +5102,11 @@
       <c r="AS19" t="n">
         <v>78</v>
       </c>
-      <c r="AT19" t="inlineStr"/>
+      <c r="AT19" t="n">
+        <v>0</v>
+      </c>
       <c r="AU19" t="n">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="AV19" t="inlineStr"/>
       <c r="AW19" t="inlineStr"/>
@@ -5100,22 +5156,22 @@
       </c>
       <c r="BN19" t="inlineStr">
         <is>
-          <t>n498e4b99ddfa490d9a3f8c55fabe4319b7274</t>
+          <t>n44744923c071402ebde9a58be3d12dd6b7274</t>
         </is>
       </c>
       <c r="BO19" t="inlineStr">
         <is>
-          <t>['n498e4b99ddfa490d9a3f8c55fabe4319b7274']</t>
+          <t>['n44744923c071402ebde9a58be3d12dd6b7274']</t>
         </is>
       </c>
       <c r="BP19" t="inlineStr">
         <is>
-          <t>n498e4b99ddfa490d9a3f8c55fabe4319b7276</t>
+          <t>n44744923c071402ebde9a58be3d12dd6b7276</t>
         </is>
       </c>
       <c r="BQ19" t="inlineStr">
         <is>
-          <t>n498e4b99ddfa490d9a3f8c55fabe4319b7276</t>
+          <t>n44744923c071402ebde9a58be3d12dd6b7276</t>
         </is>
       </c>
       <c r="BR19" t="inlineStr">
@@ -5308,8 +5364,12 @@
       <c r="AQ20" t="inlineStr"/>
       <c r="AR20" t="inlineStr"/>
       <c r="AS20" t="inlineStr"/>
-      <c r="AT20" t="inlineStr"/>
-      <c r="AU20" t="inlineStr"/>
+      <c r="AT20" t="n">
+        <v>0.7395833000000001</v>
+      </c>
+      <c r="AU20" t="n">
+        <v>0.7395833000000001</v>
+      </c>
       <c r="AV20" t="inlineStr"/>
       <c r="AW20" t="inlineStr"/>
       <c r="AX20" t="inlineStr"/>
@@ -5350,12 +5410,12 @@
       <c r="BM20" t="inlineStr"/>
       <c r="BN20" t="inlineStr">
         <is>
-          <t>nc2ea097a19674b2995408b1e809df9d8b1, nc2ea097a19674b2995408b1e809df9d8b2</t>
+          <t>n4a99d86e00f44609a5555bb477f0c721b1, n4a99d86e00f44609a5555bb477f0c721b2</t>
         </is>
       </c>
       <c r="BO20" t="inlineStr">
         <is>
-          <t>['nc2ea097a19674b2995408b1e809df9d8b1', 'nc2ea097a19674b2995408b1e809df9d8b2']</t>
+          <t>['n4a99d86e00f44609a5555bb477f0c721b1', 'n4a99d86e00f44609a5555bb477f0c721b2']</t>
         </is>
       </c>
       <c r="BP20" t="inlineStr"/>
@@ -5566,9 +5626,11 @@
       <c r="AS21" t="n">
         <v>15</v>
       </c>
-      <c r="AT21" t="inlineStr"/>
+      <c r="AT21" t="n">
+        <v>0.104166664</v>
+      </c>
       <c r="AU21" t="n">
-        <v>15</v>
+        <v>0.104166664</v>
       </c>
       <c r="AV21" t="inlineStr"/>
       <c r="AW21" t="inlineStr"/>
@@ -5675,7 +5737,7 @@
         <v>3</v>
       </c>
       <c r="CD21" t="n">
-        <v>2</v>
+        <v>1.833</v>
       </c>
     </row>
     <row r="22">
@@ -5782,8 +5844,12 @@
       <c r="AQ22" t="inlineStr"/>
       <c r="AR22" t="inlineStr"/>
       <c r="AS22" t="inlineStr"/>
-      <c r="AT22" t="inlineStr"/>
-      <c r="AU22" t="inlineStr"/>
+      <c r="AT22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU22" t="n">
+        <v>0</v>
+      </c>
       <c r="AV22" t="inlineStr"/>
       <c r="AW22" t="inlineStr"/>
       <c r="AX22" t="inlineStr"/>
@@ -6020,8 +6086,12 @@
       <c r="AQ23" t="inlineStr"/>
       <c r="AR23" t="inlineStr"/>
       <c r="AS23" t="inlineStr"/>
-      <c r="AT23" t="inlineStr"/>
-      <c r="AU23" t="inlineStr"/>
+      <c r="AT23" t="n">
+        <v>0.8125</v>
+      </c>
+      <c r="AU23" t="n">
+        <v>0.8125</v>
+      </c>
       <c r="AV23" t="inlineStr"/>
       <c r="AW23" t="inlineStr"/>
       <c r="AX23" t="inlineStr"/>
@@ -6054,12 +6124,12 @@
       <c r="BM23" t="inlineStr"/>
       <c r="BN23" t="inlineStr">
         <is>
-          <t>n6842406de79b4da889bba858396c12bbb1</t>
+          <t>n67c76c94e3a14b7098d050656db422d8b1</t>
         </is>
       </c>
       <c r="BO23" t="inlineStr">
         <is>
-          <t>['n6842406de79b4da889bba858396c12bbb1']</t>
+          <t>['n67c76c94e3a14b7098d050656db422d8b1']</t>
         </is>
       </c>
       <c r="BP23" t="inlineStr"/>
@@ -6210,8 +6280,12 @@
       <c r="AQ24" t="inlineStr"/>
       <c r="AR24" t="inlineStr"/>
       <c r="AS24" t="inlineStr"/>
-      <c r="AT24" t="inlineStr"/>
-      <c r="AU24" t="inlineStr"/>
+      <c r="AT24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU24" t="n">
+        <v>0</v>
+      </c>
       <c r="AV24" t="inlineStr"/>
       <c r="AW24" t="inlineStr"/>
       <c r="AX24" t="inlineStr"/>
@@ -6404,8 +6478,12 @@
       <c r="AQ25" t="inlineStr"/>
       <c r="AR25" t="inlineStr"/>
       <c r="AS25" t="inlineStr"/>
-      <c r="AT25" t="inlineStr"/>
-      <c r="AU25" t="inlineStr"/>
+      <c r="AT25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU25" t="n">
+        <v>0</v>
+      </c>
       <c r="AV25" t="inlineStr"/>
       <c r="AW25" t="inlineStr"/>
       <c r="AX25" t="inlineStr"/>
@@ -6664,8 +6742,12 @@
         </is>
       </c>
       <c r="AS26" t="inlineStr"/>
-      <c r="AT26" t="inlineStr"/>
-      <c r="AU26" t="inlineStr"/>
+      <c r="AT26" t="n">
+        <v>0.14583333</v>
+      </c>
+      <c r="AU26" t="n">
+        <v>0.14583333</v>
+      </c>
       <c r="AV26" t="inlineStr"/>
       <c r="AW26" t="inlineStr"/>
       <c r="AX26" t="inlineStr"/>
@@ -6714,12 +6796,12 @@
       <c r="BM26" t="inlineStr"/>
       <c r="BN26" t="inlineStr">
         <is>
-          <t>n0e130e84f70548209e41d06d5be35fa2b3, n0e130e84f70548209e41d06d5be35fa2b4</t>
+          <t>nca51b53ad14c4384a9ecd0358baa5e8eb3, nca51b53ad14c4384a9ecd0358baa5e8eb4</t>
         </is>
       </c>
       <c r="BO26" t="inlineStr">
         <is>
-          <t>['n0e130e84f70548209e41d06d5be35fa2b3', 'n0e130e84f70548209e41d06d5be35fa2b4']</t>
+          <t>['nca51b53ad14c4384a9ecd0358baa5e8eb3', 'nca51b53ad14c4384a9ecd0358baa5e8eb4']</t>
         </is>
       </c>
       <c r="BP26" t="inlineStr"/>
@@ -6878,8 +6960,12 @@
       <c r="AQ27" t="inlineStr"/>
       <c r="AR27" t="inlineStr"/>
       <c r="AS27" t="inlineStr"/>
-      <c r="AT27" t="inlineStr"/>
-      <c r="AU27" t="inlineStr"/>
+      <c r="AT27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU27" t="n">
+        <v>0</v>
+      </c>
       <c r="AV27" t="inlineStr"/>
       <c r="AW27" t="inlineStr"/>
       <c r="AX27" t="inlineStr"/>
@@ -6949,7 +7035,7 @@
         <v>1</v>
       </c>
       <c r="CD27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -7114,8 +7200,12 @@
       <c r="AQ28" t="inlineStr"/>
       <c r="AR28" t="inlineStr"/>
       <c r="AS28" t="inlineStr"/>
-      <c r="AT28" t="inlineStr"/>
-      <c r="AU28" t="inlineStr"/>
+      <c r="AT28" t="n">
+        <v>0.7973485</v>
+      </c>
+      <c r="AU28" t="n">
+        <v>0.7973485</v>
+      </c>
       <c r="AV28" t="inlineStr"/>
       <c r="AW28" t="inlineStr"/>
       <c r="AX28" t="inlineStr"/>
@@ -7164,12 +7254,12 @@
       </c>
       <c r="BN28" t="inlineStr">
         <is>
-          <t>n28ffd50793024d5b865e9a978242f20ab1</t>
+          <t>ne92fefd39a694cb3a94846113a8ffc30b1</t>
         </is>
       </c>
       <c r="BO28" t="inlineStr">
         <is>
-          <t>['n28ffd50793024d5b865e9a978242f20ab1']</t>
+          <t>['ne92fefd39a694cb3a94846113a8ffc30b1']</t>
         </is>
       </c>
       <c r="BP28" t="inlineStr"/>
@@ -7213,7 +7303,7 @@
         <v>2</v>
       </c>
       <c r="CD28" t="n">
-        <v>1</v>
+        <v>1.389</v>
       </c>
     </row>
     <row r="29">
@@ -7394,8 +7484,12 @@
         </is>
       </c>
       <c r="AS29" t="inlineStr"/>
-      <c r="AT29" t="inlineStr"/>
-      <c r="AU29" t="inlineStr"/>
+      <c r="AT29" t="n">
+        <v>0.14583333</v>
+      </c>
+      <c r="AU29" t="n">
+        <v>0.14583333</v>
+      </c>
       <c r="AV29" t="inlineStr"/>
       <c r="AW29" t="inlineStr"/>
       <c r="AX29" t="inlineStr"/>
@@ -7444,12 +7538,12 @@
       <c r="BM29" t="inlineStr"/>
       <c r="BN29" t="inlineStr">
         <is>
-          <t>n21b9e2b265b346888941d4adfa85e4dab3, n21b9e2b265b346888941d4adfa85e4dab4</t>
+          <t>n3a56e66f2729490cbc26c23fa43dc5edb3, n3a56e66f2729490cbc26c23fa43dc5edb4</t>
         </is>
       </c>
       <c r="BO29" t="inlineStr">
         <is>
-          <t>['n21b9e2b265b346888941d4adfa85e4dab3', 'n21b9e2b265b346888941d4adfa85e4dab4']</t>
+          <t>['n3a56e66f2729490cbc26c23fa43dc5edb3', 'n3a56e66f2729490cbc26c23fa43dc5edb4']</t>
         </is>
       </c>
       <c r="BP29" t="inlineStr"/>
@@ -7674,8 +7768,12 @@
         </is>
       </c>
       <c r="AS30" t="inlineStr"/>
-      <c r="AT30" t="inlineStr"/>
-      <c r="AU30" t="inlineStr"/>
+      <c r="AT30" t="n">
+        <v>0.14583333</v>
+      </c>
+      <c r="AU30" t="n">
+        <v>0.14583333</v>
+      </c>
       <c r="AV30" t="inlineStr"/>
       <c r="AW30" t="inlineStr"/>
       <c r="AX30" t="inlineStr"/>
@@ -7724,12 +7822,12 @@
       <c r="BM30" t="inlineStr"/>
       <c r="BN30" t="inlineStr">
         <is>
-          <t>n6390b2ebfd974b50b08f99b1ef23cb6ab3, n6390b2ebfd974b50b08f99b1ef23cb6ab4</t>
+          <t>ne1dc41f433d441dc934dee8f4f0a064cb3, ne1dc41f433d441dc934dee8f4f0a064cb4</t>
         </is>
       </c>
       <c r="BO30" t="inlineStr">
         <is>
-          <t>['n6390b2ebfd974b50b08f99b1ef23cb6ab3', 'n6390b2ebfd974b50b08f99b1ef23cb6ab4']</t>
+          <t>['ne1dc41f433d441dc934dee8f4f0a064cb3', 'ne1dc41f433d441dc934dee8f4f0a064cb4']</t>
         </is>
       </c>
       <c r="BP30" t="inlineStr"/>
@@ -7947,8 +8045,12 @@
         </is>
       </c>
       <c r="AS31" t="inlineStr"/>
-      <c r="AT31" t="inlineStr"/>
-      <c r="AU31" t="inlineStr"/>
+      <c r="AT31" t="n">
+        <v>0.8125</v>
+      </c>
+      <c r="AU31" t="n">
+        <v>0.8125</v>
+      </c>
       <c r="AV31" t="inlineStr"/>
       <c r="AW31" t="inlineStr"/>
       <c r="AX31" t="inlineStr"/>
@@ -7997,12 +8099,12 @@
       <c r="BM31" t="inlineStr"/>
       <c r="BN31" t="inlineStr">
         <is>
-          <t>n2f7b303cdbea4cca9d230706edde4e4bb1</t>
+          <t>n44185ebbc4be42fd9f9a9a3b6c3a5c5eb1</t>
         </is>
       </c>
       <c r="BO31" t="inlineStr">
         <is>
-          <t>['n2f7b303cdbea4cca9d230706edde4e4bb1']</t>
+          <t>['n44185ebbc4be42fd9f9a9a3b6c3a5c5eb1']</t>
         </is>
       </c>
       <c r="BP31" t="inlineStr"/>
@@ -8046,7 +8148,7 @@
         <v>3</v>
       </c>
       <c r="CD31" t="n">
-        <v>2</v>
+        <v>1.81</v>
       </c>
     </row>
     <row r="32">
@@ -8220,8 +8322,12 @@
       <c r="AQ32" t="inlineStr"/>
       <c r="AR32" t="inlineStr"/>
       <c r="AS32" t="inlineStr"/>
-      <c r="AT32" t="inlineStr"/>
-      <c r="AU32" t="inlineStr"/>
+      <c r="AT32" t="n">
+        <v>0.7892157400000001</v>
+      </c>
+      <c r="AU32" t="n">
+        <v>0.7892157400000001</v>
+      </c>
       <c r="AV32" t="inlineStr"/>
       <c r="AW32" t="inlineStr"/>
       <c r="AX32" t="inlineStr"/>
@@ -8262,22 +8368,22 @@
       <c r="BM32" t="inlineStr"/>
       <c r="BN32" t="inlineStr">
         <is>
-          <t>naec60fa6a2b14b379b49c030147b49f9b1</t>
+          <t>n02a4f2f658e84a55bfe7e389fc80fb4bb1</t>
         </is>
       </c>
       <c r="BO32" t="inlineStr">
         <is>
-          <t>['naec60fa6a2b14b379b49c030147b49f9b1']</t>
+          <t>['n02a4f2f658e84a55bfe7e389fc80fb4bb1']</t>
         </is>
       </c>
       <c r="BP32" t="inlineStr">
         <is>
-          <t>naec60fa6a2b14b379b49c030147b49f9b3</t>
+          <t>n02a4f2f658e84a55bfe7e389fc80fb4bb3</t>
         </is>
       </c>
       <c r="BQ32" t="inlineStr">
         <is>
-          <t>naec60fa6a2b14b379b49c030147b49f9b3</t>
+          <t>n02a4f2f658e84a55bfe7e389fc80fb4bb3</t>
         </is>
       </c>
       <c r="BR32" t="inlineStr">
@@ -8319,7 +8425,7 @@
         <v>3</v>
       </c>
       <c r="CD32" t="n">
-        <v>2</v>
+        <v>1.941</v>
       </c>
     </row>
     <row r="33">
@@ -8434,8 +8540,12 @@
       <c r="AQ33" t="inlineStr"/>
       <c r="AR33" t="inlineStr"/>
       <c r="AS33" t="inlineStr"/>
-      <c r="AT33" t="inlineStr"/>
-      <c r="AU33" t="inlineStr"/>
+      <c r="AT33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU33" t="n">
+        <v>0</v>
+      </c>
       <c r="AV33" t="inlineStr"/>
       <c r="AW33" t="inlineStr"/>
       <c r="AX33" t="inlineStr"/>
@@ -8684,8 +8794,12 @@
         </is>
       </c>
       <c r="AS34" t="inlineStr"/>
-      <c r="AT34" t="inlineStr"/>
-      <c r="AU34" t="inlineStr"/>
+      <c r="AT34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU34" t="n">
+        <v>0</v>
+      </c>
       <c r="AV34" t="inlineStr"/>
       <c r="AW34" t="inlineStr"/>
       <c r="AX34" t="inlineStr"/>
@@ -8783,7 +8897,7 @@
         <v>3</v>
       </c>
       <c r="CD34" t="n">
-        <v>1</v>
+        <v>1.492</v>
       </c>
     </row>
     <row r="35">
@@ -8942,8 +9056,12 @@
         </is>
       </c>
       <c r="AS35" t="inlineStr"/>
-      <c r="AT35" t="inlineStr"/>
-      <c r="AU35" t="inlineStr"/>
+      <c r="AT35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU35" t="n">
+        <v>0</v>
+      </c>
       <c r="AV35" t="inlineStr"/>
       <c r="AW35" t="inlineStr"/>
       <c r="AX35" t="inlineStr"/>
@@ -9041,7 +9159,7 @@
         <v>3</v>
       </c>
       <c r="CD35" t="n">
-        <v>1</v>
+        <v>1.458</v>
       </c>
     </row>
     <row r="36">
@@ -9212,8 +9330,12 @@
         </is>
       </c>
       <c r="AS36" t="inlineStr"/>
-      <c r="AT36" t="inlineStr"/>
-      <c r="AU36" t="inlineStr"/>
+      <c r="AT36" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU36" t="n">
+        <v>0</v>
+      </c>
       <c r="AV36" t="inlineStr">
         <is>
           <t>ISO/IEC 21838-2</t>
@@ -9319,7 +9441,7 @@
         <v>3</v>
       </c>
       <c r="CD36" t="n">
-        <v>2</v>
+        <v>1.647</v>
       </c>
     </row>
     <row r="37">
@@ -9476,8 +9598,12 @@
       <c r="AQ37" t="inlineStr"/>
       <c r="AR37" t="inlineStr"/>
       <c r="AS37" t="inlineStr"/>
-      <c r="AT37" t="inlineStr"/>
-      <c r="AU37" t="inlineStr"/>
+      <c r="AT37" t="n">
+        <v>0.14583333</v>
+      </c>
+      <c r="AU37" t="n">
+        <v>0.14583333</v>
+      </c>
       <c r="AV37" t="inlineStr"/>
       <c r="AW37" t="inlineStr"/>
       <c r="AX37" t="inlineStr"/>
@@ -9583,7 +9709,7 @@
         <v>3</v>
       </c>
       <c r="CD37" t="n">
-        <v>1</v>
+        <v>1.497</v>
       </c>
     </row>
     <row r="38">
@@ -9754,8 +9880,12 @@
         </is>
       </c>
       <c r="AS38" t="inlineStr"/>
-      <c r="AT38" t="inlineStr"/>
-      <c r="AU38" t="inlineStr"/>
+      <c r="AT38" t="n">
+        <v>0.14583333</v>
+      </c>
+      <c r="AU38" t="n">
+        <v>0.14583333</v>
+      </c>
       <c r="AV38" t="inlineStr"/>
       <c r="AW38" t="inlineStr"/>
       <c r="AX38" t="inlineStr"/>
@@ -9853,7 +9983,7 @@
         <v>3</v>
       </c>
       <c r="CD38" t="n">
-        <v>1</v>
+        <v>1.428</v>
       </c>
     </row>
     <row r="39">
@@ -10024,8 +10154,12 @@
         </is>
       </c>
       <c r="AS39" t="inlineStr"/>
-      <c r="AT39" t="inlineStr"/>
-      <c r="AU39" t="inlineStr"/>
+      <c r="AT39" t="n">
+        <v>0.14583333</v>
+      </c>
+      <c r="AU39" t="n">
+        <v>0.14583333</v>
+      </c>
       <c r="AV39" t="inlineStr">
         <is>
           <t>BS EN 16310:2013, HOAI, RIBA, ISO 22263</t>
@@ -10131,7 +10265,7 @@
         <v>3</v>
       </c>
       <c r="CD39" t="n">
-        <v>1</v>
+        <v>1.333</v>
       </c>
     </row>
     <row r="40">
@@ -10272,8 +10406,12 @@
       <c r="AQ40" t="inlineStr"/>
       <c r="AR40" t="inlineStr"/>
       <c r="AS40" t="inlineStr"/>
-      <c r="AT40" t="inlineStr"/>
-      <c r="AU40" t="inlineStr"/>
+      <c r="AT40" t="n">
+        <v>0.14583333</v>
+      </c>
+      <c r="AU40" t="n">
+        <v>0.14583333</v>
+      </c>
       <c r="AV40" t="inlineStr"/>
       <c r="AW40" t="inlineStr"/>
       <c r="AX40" t="inlineStr"/>
@@ -10544,8 +10682,12 @@
         </is>
       </c>
       <c r="AS41" t="inlineStr"/>
-      <c r="AT41" t="inlineStr"/>
-      <c r="AU41" t="inlineStr"/>
+      <c r="AT41" t="n">
+        <v>0.14583333</v>
+      </c>
+      <c r="AU41" t="n">
+        <v>0.14583333</v>
+      </c>
       <c r="AV41" t="inlineStr"/>
       <c r="AW41" t="inlineStr"/>
       <c r="AX41" t="inlineStr"/>
@@ -10643,7 +10785,7 @@
         <v>3</v>
       </c>
       <c r="CD41" t="n">
-        <v>2</v>
+        <v>1.525</v>
       </c>
     </row>
     <row r="42">
@@ -10806,8 +10948,12 @@
       <c r="AQ42" t="inlineStr"/>
       <c r="AR42" t="inlineStr"/>
       <c r="AS42" t="inlineStr"/>
-      <c r="AT42" t="inlineStr"/>
-      <c r="AU42" t="inlineStr"/>
+      <c r="AT42" t="n">
+        <v>0.14583333</v>
+      </c>
+      <c r="AU42" t="n">
+        <v>0.14583333</v>
+      </c>
       <c r="AV42" t="inlineStr"/>
       <c r="AW42" t="inlineStr"/>
       <c r="AX42" t="inlineStr"/>
@@ -10913,7 +11059,7 @@
         <v>3</v>
       </c>
       <c r="CD42" t="n">
-        <v>1</v>
+        <v>1.067</v>
       </c>
     </row>
     <row r="43">
@@ -11084,8 +11230,12 @@
         </is>
       </c>
       <c r="AS43" t="inlineStr"/>
-      <c r="AT43" t="inlineStr"/>
-      <c r="AU43" t="inlineStr"/>
+      <c r="AT43" t="n">
+        <v>0.14583333</v>
+      </c>
+      <c r="AU43" t="n">
+        <v>0.14583333</v>
+      </c>
       <c r="AV43" t="inlineStr"/>
       <c r="AW43" t="inlineStr"/>
       <c r="AX43" t="inlineStr"/>
@@ -11183,7 +11333,7 @@
         <v>3</v>
       </c>
       <c r="CD43" t="n">
-        <v>2</v>
+        <v>1.524</v>
       </c>
     </row>
     <row r="44">
@@ -11316,8 +11466,12 @@
       <c r="AQ44" t="inlineStr"/>
       <c r="AR44" t="inlineStr"/>
       <c r="AS44" t="inlineStr"/>
-      <c r="AT44" t="inlineStr"/>
-      <c r="AU44" t="inlineStr"/>
+      <c r="AT44" t="n">
+        <v>0.14583333</v>
+      </c>
+      <c r="AU44" t="n">
+        <v>0.14583333</v>
+      </c>
       <c r="AV44" t="inlineStr"/>
       <c r="AW44" t="inlineStr"/>
       <c r="AX44" t="inlineStr"/>
@@ -11552,8 +11706,12 @@
         </is>
       </c>
       <c r="AS45" t="inlineStr"/>
-      <c r="AT45" t="inlineStr"/>
-      <c r="AU45" t="inlineStr"/>
+      <c r="AT45" t="n">
+        <v>0.14583333</v>
+      </c>
+      <c r="AU45" t="n">
+        <v>0.14583333</v>
+      </c>
       <c r="AV45" t="inlineStr"/>
       <c r="AW45" t="inlineStr"/>
       <c r="AX45" t="inlineStr"/>
@@ -11802,8 +11960,12 @@
         </is>
       </c>
       <c r="AS46" t="inlineStr"/>
-      <c r="AT46" t="inlineStr"/>
-      <c r="AU46" t="inlineStr"/>
+      <c r="AT46" t="n">
+        <v>0.14583333</v>
+      </c>
+      <c r="AU46" t="n">
+        <v>0.14583333</v>
+      </c>
       <c r="AV46" t="inlineStr"/>
       <c r="AW46" t="inlineStr"/>
       <c r="AX46" t="inlineStr"/>
@@ -11901,7 +12063,7 @@
         <v>3</v>
       </c>
       <c r="CD46" t="n">
-        <v>2</v>
+        <v>1.782</v>
       </c>
     </row>
     <row r="47">
@@ -12000,8 +12162,12 @@
       <c r="AQ47" t="inlineStr"/>
       <c r="AR47" t="inlineStr"/>
       <c r="AS47" t="inlineStr"/>
-      <c r="AT47" t="inlineStr"/>
-      <c r="AU47" t="inlineStr"/>
+      <c r="AT47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU47" t="n">
+        <v>0</v>
+      </c>
       <c r="AV47" t="inlineStr"/>
       <c r="AW47" t="inlineStr"/>
       <c r="AX47" t="inlineStr"/>
@@ -12178,8 +12344,12 @@
       <c r="AQ48" t="inlineStr"/>
       <c r="AR48" t="inlineStr"/>
       <c r="AS48" t="inlineStr"/>
-      <c r="AT48" t="inlineStr"/>
-      <c r="AU48" t="inlineStr"/>
+      <c r="AT48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU48" t="n">
+        <v>0</v>
+      </c>
       <c r="AV48" t="inlineStr"/>
       <c r="AW48" t="inlineStr"/>
       <c r="AX48" t="inlineStr"/>
@@ -12423,8 +12593,12 @@
       <c r="AQ49" t="inlineStr"/>
       <c r="AR49" t="inlineStr"/>
       <c r="AS49" t="inlineStr"/>
-      <c r="AT49" t="inlineStr"/>
-      <c r="AU49" t="inlineStr"/>
+      <c r="AT49" t="n">
+        <v>0.104166664</v>
+      </c>
+      <c r="AU49" t="n">
+        <v>0.104166664</v>
+      </c>
       <c r="AV49" t="inlineStr"/>
       <c r="AW49" t="inlineStr"/>
       <c r="AX49" t="inlineStr"/>
@@ -12514,7 +12688,7 @@
         <v>3</v>
       </c>
       <c r="CD49" t="n">
-        <v>1</v>
+        <v>1.226</v>
       </c>
     </row>
     <row r="50">
@@ -12679,8 +12853,12 @@
       <c r="AQ50" t="inlineStr"/>
       <c r="AR50" t="inlineStr"/>
       <c r="AS50" t="inlineStr"/>
-      <c r="AT50" t="inlineStr"/>
-      <c r="AU50" t="inlineStr"/>
+      <c r="AT50" t="n">
+        <v>0.104166664</v>
+      </c>
+      <c r="AU50" t="n">
+        <v>0.104166664</v>
+      </c>
       <c r="AV50" t="inlineStr">
         <is>
           <t>ISO/DIS 59004</t>
@@ -12778,7 +12956,7 @@
         <v>3</v>
       </c>
       <c r="CD50" t="n">
-        <v>2</v>
+        <v>1.986</v>
       </c>
     </row>
     <row r="51">
@@ -12959,8 +13137,12 @@
         </is>
       </c>
       <c r="AS51" t="inlineStr"/>
-      <c r="AT51" t="inlineStr"/>
-      <c r="AU51" t="inlineStr"/>
+      <c r="AT51" t="n">
+        <v>0.8611111</v>
+      </c>
+      <c r="AU51" t="n">
+        <v>0.8611111</v>
+      </c>
       <c r="AV51" t="inlineStr"/>
       <c r="AW51" t="inlineStr"/>
       <c r="AX51" t="inlineStr"/>
@@ -13009,12 +13191,12 @@
       </c>
       <c r="BN51" t="inlineStr">
         <is>
-          <t>n47034cc08ce84de68f53454e9bddbf83b1, https://www.researchgate.net/profile/Mathias_Bonduel</t>
+          <t>n0f5122232f024f6f987d3ad335536392b1, https://www.researchgate.net/profile/Mathias_Bonduel</t>
         </is>
       </c>
       <c r="BO51" t="inlineStr">
         <is>
-          <t>['n47034cc08ce84de68f53454e9bddbf83b1', 'https://www.researchgate.net/profile/Mathias_Bonduel']</t>
+          <t>['n0f5122232f024f6f987d3ad335536392b1', 'https://www.researchgate.net/profile/Mathias_Bonduel']</t>
         </is>
       </c>
       <c r="BP51" t="inlineStr"/>
@@ -13217,8 +13399,12 @@
       <c r="AQ52" t="inlineStr"/>
       <c r="AR52" t="inlineStr"/>
       <c r="AS52" t="inlineStr"/>
-      <c r="AT52" t="inlineStr"/>
-      <c r="AU52" t="inlineStr"/>
+      <c r="AT52" t="n">
+        <v>0.72222215</v>
+      </c>
+      <c r="AU52" t="n">
+        <v>0.72222215</v>
+      </c>
       <c r="AV52" t="inlineStr"/>
       <c r="AW52" t="inlineStr"/>
       <c r="AX52" t="inlineStr"/>
@@ -13475,8 +13661,12 @@
         </is>
       </c>
       <c r="AS53" t="inlineStr"/>
-      <c r="AT53" t="inlineStr"/>
-      <c r="AU53" t="inlineStr"/>
+      <c r="AT53" t="n">
+        <v>0.1875</v>
+      </c>
+      <c r="AU53" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="AV53" t="inlineStr"/>
       <c r="AW53" t="inlineStr"/>
       <c r="AX53" t="inlineStr"/>
@@ -13725,8 +13915,12 @@
       <c r="AQ54" t="inlineStr"/>
       <c r="AR54" t="inlineStr"/>
       <c r="AS54" t="inlineStr"/>
-      <c r="AT54" t="inlineStr"/>
-      <c r="AU54" t="inlineStr"/>
+      <c r="AT54" t="n">
+        <v>0.6388889</v>
+      </c>
+      <c r="AU54" t="n">
+        <v>0.6388889</v>
+      </c>
       <c r="AV54" t="inlineStr"/>
       <c r="AW54" t="inlineStr"/>
       <c r="AX54" t="inlineStr"/>
@@ -13973,8 +14167,12 @@
       <c r="AQ55" t="inlineStr"/>
       <c r="AR55" t="inlineStr"/>
       <c r="AS55" t="inlineStr"/>
-      <c r="AT55" t="inlineStr"/>
-      <c r="AU55" t="inlineStr"/>
+      <c r="AT55" t="n">
+        <v>0.68402785</v>
+      </c>
+      <c r="AU55" t="n">
+        <v>0.68402785</v>
+      </c>
       <c r="AV55" t="inlineStr"/>
       <c r="AW55" t="inlineStr"/>
       <c r="AX55" t="inlineStr"/>
@@ -14230,8 +14428,12 @@
       <c r="AQ56" t="inlineStr"/>
       <c r="AR56" t="inlineStr"/>
       <c r="AS56" t="inlineStr"/>
-      <c r="AT56" t="inlineStr"/>
-      <c r="AU56" t="inlineStr"/>
+      <c r="AT56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU56" t="n">
+        <v>0</v>
+      </c>
       <c r="AV56" t="inlineStr"/>
       <c r="AW56" t="inlineStr"/>
       <c r="AX56" t="inlineStr"/>
@@ -14496,8 +14698,12 @@
       <c r="AQ57" t="inlineStr"/>
       <c r="AR57" t="inlineStr"/>
       <c r="AS57" t="inlineStr"/>
-      <c r="AT57" t="inlineStr"/>
-      <c r="AU57" t="inlineStr"/>
+      <c r="AT57" t="n">
+        <v>0.6770833000000001</v>
+      </c>
+      <c r="AU57" t="n">
+        <v>0.6770833000000001</v>
+      </c>
       <c r="AV57" t="inlineStr"/>
       <c r="AW57" t="inlineStr"/>
       <c r="AX57" t="inlineStr"/>
@@ -14714,8 +14920,12 @@
       <c r="AQ58" t="inlineStr"/>
       <c r="AR58" t="inlineStr"/>
       <c r="AS58" t="inlineStr"/>
-      <c r="AT58" t="inlineStr"/>
-      <c r="AU58" t="inlineStr"/>
+      <c r="AT58" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU58" t="n">
+        <v>0</v>
+      </c>
       <c r="AV58" t="inlineStr">
         <is>
           <t xml:space="preserve"> ISO 3166-2</t>
@@ -14793,7 +15003,7 @@
         <v>2</v>
       </c>
       <c r="CD58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -14962,8 +15172,12 @@
         </is>
       </c>
       <c r="AS59" t="inlineStr"/>
-      <c r="AT59" t="inlineStr"/>
-      <c r="AU59" t="inlineStr"/>
+      <c r="AT59" t="n">
+        <v>0.104166664</v>
+      </c>
+      <c r="AU59" t="n">
+        <v>0.104166664</v>
+      </c>
       <c r="AV59" t="inlineStr"/>
       <c r="AW59" t="inlineStr"/>
       <c r="AX59" t="inlineStr"/>
@@ -15213,8 +15427,12 @@
       <c r="AQ60" t="inlineStr"/>
       <c r="AR60" t="inlineStr"/>
       <c r="AS60" t="inlineStr"/>
-      <c r="AT60" t="inlineStr"/>
-      <c r="AU60" t="inlineStr"/>
+      <c r="AT60" t="n">
+        <v>0.14583333</v>
+      </c>
+      <c r="AU60" t="n">
+        <v>0.14583333</v>
+      </c>
       <c r="AV60" t="inlineStr"/>
       <c r="AW60" t="inlineStr"/>
       <c r="AX60" t="inlineStr"/>
@@ -15308,7 +15526,7 @@
         <v>3</v>
       </c>
       <c r="CD60" t="n">
-        <v>2</v>
+        <v>1.932</v>
       </c>
     </row>
     <row r="61">
@@ -15431,8 +15649,12 @@
       <c r="AQ61" t="inlineStr"/>
       <c r="AR61" t="inlineStr"/>
       <c r="AS61" t="inlineStr"/>
-      <c r="AT61" t="inlineStr"/>
-      <c r="AU61" t="inlineStr"/>
+      <c r="AT61" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU61" t="n">
+        <v>0</v>
+      </c>
       <c r="AV61" t="inlineStr"/>
       <c r="AW61" t="inlineStr"/>
       <c r="AX61" t="inlineStr"/>
@@ -15645,8 +15867,12 @@
       <c r="AQ62" t="inlineStr"/>
       <c r="AR62" t="inlineStr"/>
       <c r="AS62" t="inlineStr"/>
-      <c r="AT62" t="inlineStr"/>
-      <c r="AU62" t="inlineStr"/>
+      <c r="AT62" t="n">
+        <v>0.14583333</v>
+      </c>
+      <c r="AU62" t="n">
+        <v>0.14583333</v>
+      </c>
       <c r="AV62" t="inlineStr"/>
       <c r="AW62" t="inlineStr"/>
       <c r="AX62" t="inlineStr"/>
@@ -15716,7 +15942,7 @@
         <v>3</v>
       </c>
       <c r="CD62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63">
@@ -15839,8 +16065,12 @@
       <c r="AQ63" t="inlineStr"/>
       <c r="AR63" t="inlineStr"/>
       <c r="AS63" t="inlineStr"/>
-      <c r="AT63" t="inlineStr"/>
-      <c r="AU63" t="inlineStr"/>
+      <c r="AT63" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU63" t="n">
+        <v>0</v>
+      </c>
       <c r="AV63" t="inlineStr"/>
       <c r="AW63" t="inlineStr"/>
       <c r="AX63" t="inlineStr"/>
@@ -16089,8 +16319,12 @@
       <c r="AQ64" t="inlineStr"/>
       <c r="AR64" t="inlineStr"/>
       <c r="AS64" t="inlineStr"/>
-      <c r="AT64" t="inlineStr"/>
-      <c r="AU64" t="inlineStr"/>
+      <c r="AT64" t="n">
+        <v>0.3784722</v>
+      </c>
+      <c r="AU64" t="n">
+        <v>0.3784722</v>
+      </c>
       <c r="AV64" t="inlineStr"/>
       <c r="AW64" t="inlineStr"/>
       <c r="AX64" t="inlineStr"/>
@@ -16188,7 +16422,7 @@
         <v>3</v>
       </c>
       <c r="CD64" t="n">
-        <v>2</v>
+        <v>1.913</v>
       </c>
     </row>
     <row r="65">
@@ -16369,8 +16603,12 @@
         </is>
       </c>
       <c r="AS65" t="inlineStr"/>
-      <c r="AT65" t="inlineStr"/>
-      <c r="AU65" t="inlineStr"/>
+      <c r="AT65" t="n">
+        <v>0.81218195</v>
+      </c>
+      <c r="AU65" t="n">
+        <v>0.81218195</v>
+      </c>
       <c r="AV65" t="inlineStr"/>
       <c r="AW65" t="inlineStr"/>
       <c r="AX65" t="inlineStr"/>
@@ -16460,7 +16698,7 @@
         <v>3</v>
       </c>
       <c r="CD65" t="n">
-        <v>2</v>
+        <v>1.992</v>
       </c>
     </row>
     <row r="66">
@@ -16627,8 +16865,12 @@
       <c r="AQ66" t="inlineStr"/>
       <c r="AR66" t="inlineStr"/>
       <c r="AS66" t="inlineStr"/>
-      <c r="AT66" t="inlineStr"/>
-      <c r="AU66" t="inlineStr"/>
+      <c r="AT66" t="n">
+        <v>0.14583333</v>
+      </c>
+      <c r="AU66" t="n">
+        <v>0.14583333</v>
+      </c>
       <c r="AV66" t="inlineStr"/>
       <c r="AW66" t="inlineStr"/>
       <c r="AX66" t="inlineStr"/>
@@ -16726,7 +16968,7 @@
         <v>3</v>
       </c>
       <c r="CD66" t="n">
-        <v>2</v>
+        <v>1.886</v>
       </c>
     </row>
     <row r="67">
@@ -16825,8 +17067,12 @@
       <c r="AQ67" t="inlineStr"/>
       <c r="AR67" t="inlineStr"/>
       <c r="AS67" t="inlineStr"/>
-      <c r="AT67" t="inlineStr"/>
-      <c r="AU67" t="inlineStr"/>
+      <c r="AT67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU67" t="n">
+        <v>0</v>
+      </c>
       <c r="AV67" t="inlineStr"/>
       <c r="AW67" t="inlineStr"/>
       <c r="AX67" t="inlineStr"/>
@@ -17003,8 +17249,12 @@
       <c r="AQ68" t="inlineStr"/>
       <c r="AR68" t="inlineStr"/>
       <c r="AS68" t="inlineStr"/>
-      <c r="AT68" t="inlineStr"/>
-      <c r="AU68" t="inlineStr"/>
+      <c r="AT68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU68" t="n">
+        <v>0</v>
+      </c>
       <c r="AV68" t="inlineStr"/>
       <c r="AW68" t="inlineStr"/>
       <c r="AX68" t="inlineStr"/>
@@ -17239,8 +17489,12 @@
         </is>
       </c>
       <c r="AS69" t="inlineStr"/>
-      <c r="AT69" t="inlineStr"/>
-      <c r="AU69" t="inlineStr"/>
+      <c r="AT69" t="n">
+        <v>0.8993056</v>
+      </c>
+      <c r="AU69" t="n">
+        <v>0.8993056</v>
+      </c>
       <c r="AV69" t="inlineStr">
         <is>
           <t>OGC</t>
@@ -17299,12 +17553,12 @@
       </c>
       <c r="BP69" t="inlineStr">
         <is>
-          <t>n3f19c6bc39b74ecbb3ec1a1f90f91af6b1</t>
+          <t>nd6e9bf97cccd469d9294e6da77b119e5b1</t>
         </is>
       </c>
       <c r="BQ69" t="inlineStr">
         <is>
-          <t>n3f19c6bc39b74ecbb3ec1a1f90f91af6b1</t>
+          <t>nd6e9bf97cccd469d9294e6da77b119e5b1</t>
         </is>
       </c>
       <c r="BR69" t="inlineStr">
@@ -17461,8 +17715,12 @@
       <c r="AQ70" t="inlineStr"/>
       <c r="AR70" t="inlineStr"/>
       <c r="AS70" t="inlineStr"/>
-      <c r="AT70" t="inlineStr"/>
-      <c r="AU70" t="inlineStr"/>
+      <c r="AT70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU70" t="n">
+        <v>0</v>
+      </c>
       <c r="AV70" t="inlineStr"/>
       <c r="AW70" t="inlineStr"/>
       <c r="AX70" t="inlineStr"/>
@@ -17717,8 +17975,12 @@
         </is>
       </c>
       <c r="AS71" t="inlineStr"/>
-      <c r="AT71" t="inlineStr"/>
-      <c r="AU71" t="inlineStr"/>
+      <c r="AT71" t="n">
+        <v>0.7361111</v>
+      </c>
+      <c r="AU71" t="n">
+        <v>0.7361111</v>
+      </c>
       <c r="AV71" t="inlineStr"/>
       <c r="AW71" t="inlineStr"/>
       <c r="AX71" t="inlineStr"/>
@@ -17977,9 +18239,11 @@
       <c r="AS72" t="n">
         <v>0</v>
       </c>
-      <c r="AT72" t="inlineStr"/>
+      <c r="AT72" t="n">
+        <v>0.0625</v>
+      </c>
       <c r="AU72" t="n">
-        <v>0</v>
+        <v>0.0625</v>
       </c>
       <c r="AV72" t="inlineStr">
         <is>
@@ -18243,8 +18507,12 @@
       <c r="AQ73" t="inlineStr"/>
       <c r="AR73" t="inlineStr"/>
       <c r="AS73" t="inlineStr"/>
-      <c r="AT73" t="inlineStr"/>
-      <c r="AU73" t="inlineStr"/>
+      <c r="AT73" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="AU73" t="n">
+        <v>0.0625</v>
+      </c>
       <c r="AV73" t="inlineStr">
         <is>
           <t>ISO 19650</t>
@@ -18293,22 +18561,22 @@
       <c r="BM73" t="inlineStr"/>
       <c r="BN73" t="inlineStr">
         <is>
-          <t>n29e328aba23c4bd78a5a1ee8e7855805b1</t>
+          <t>nc4d210c79b634f7a8f62a48a3e1bbf56b1</t>
         </is>
       </c>
       <c r="BO73" t="inlineStr">
         <is>
-          <t>['n29e328aba23c4bd78a5a1ee8e7855805b1']</t>
+          <t>['nc4d210c79b634f7a8f62a48a3e1bbf56b1']</t>
         </is>
       </c>
       <c r="BP73" t="inlineStr">
         <is>
-          <t>n29e328aba23c4bd78a5a1ee8e7855805b3</t>
+          <t>nc4d210c79b634f7a8f62a48a3e1bbf56b3</t>
         </is>
       </c>
       <c r="BQ73" t="inlineStr">
         <is>
-          <t>n29e328aba23c4bd78a5a1ee8e7855805b3</t>
+          <t>nc4d210c79b634f7a8f62a48a3e1bbf56b3</t>
         </is>
       </c>
       <c r="BR73" t="inlineStr">
@@ -18350,7 +18618,7 @@
         <v>3</v>
       </c>
       <c r="CD73" t="n">
-        <v>2</v>
+        <v>1.933</v>
       </c>
     </row>
     <row r="74">
@@ -18495,8 +18763,12 @@
         </is>
       </c>
       <c r="AS74" t="inlineStr"/>
-      <c r="AT74" t="inlineStr"/>
-      <c r="AU74" t="inlineStr"/>
+      <c r="AT74" t="n">
+        <v>0.56815</v>
+      </c>
+      <c r="AU74" t="n">
+        <v>0.56815</v>
+      </c>
       <c r="AV74" t="inlineStr"/>
       <c r="AW74" t="inlineStr"/>
       <c r="AX74" t="inlineStr"/>
@@ -18747,8 +19019,12 @@
       <c r="AQ75" t="inlineStr"/>
       <c r="AR75" t="inlineStr"/>
       <c r="AS75" t="inlineStr"/>
-      <c r="AT75" t="inlineStr"/>
-      <c r="AU75" t="inlineStr"/>
+      <c r="AT75" t="n">
+        <v>0.104166664</v>
+      </c>
+      <c r="AU75" t="n">
+        <v>0.104166664</v>
+      </c>
       <c r="AV75" t="inlineStr"/>
       <c r="AW75" t="inlineStr"/>
       <c r="AX75" t="inlineStr"/>
@@ -18789,12 +19065,12 @@
       <c r="BM75" t="inlineStr"/>
       <c r="BN75" t="inlineStr">
         <is>
-          <t>n5ddeeb3fa28b40c08b500efc110dd98fb1, n5ddeeb3fa28b40c08b500efc110dd98fb2</t>
+          <t>n3d430423b1914c95b9a573defad90fbcb1, n3d430423b1914c95b9a573defad90fbcb2</t>
         </is>
       </c>
       <c r="BO75" t="inlineStr">
         <is>
-          <t>['n5ddeeb3fa28b40c08b500efc110dd98fb1', 'n5ddeeb3fa28b40c08b500efc110dd98fb2']</t>
+          <t>['n3d430423b1914c95b9a573defad90fbcb1', 'n3d430423b1914c95b9a573defad90fbcb2']</t>
         </is>
       </c>
       <c r="BP75" t="inlineStr"/>
@@ -18993,9 +19269,11 @@
       <c r="AS76" t="n">
         <v>15</v>
       </c>
-      <c r="AT76" t="inlineStr"/>
+      <c r="AT76" t="n">
+        <v>0.104166664</v>
+      </c>
       <c r="AU76" t="n">
-        <v>15</v>
+        <v>0.104166664</v>
       </c>
       <c r="AV76" t="inlineStr"/>
       <c r="AW76" t="inlineStr"/>
@@ -19102,7 +19380,7 @@
         <v>3</v>
       </c>
       <c r="CD76" t="n">
-        <v>2</v>
+        <v>1.556</v>
       </c>
     </row>
     <row r="77">
@@ -19273,8 +19551,12 @@
         </is>
       </c>
       <c r="AS77" t="inlineStr"/>
-      <c r="AT77" t="inlineStr"/>
-      <c r="AU77" t="inlineStr"/>
+      <c r="AT77" t="n">
+        <v>0.72023803</v>
+      </c>
+      <c r="AU77" t="n">
+        <v>0.72023803</v>
+      </c>
       <c r="AV77" t="inlineStr"/>
       <c r="AW77" t="inlineStr"/>
       <c r="AX77" t="inlineStr"/>
@@ -19372,7 +19654,7 @@
         <v>3</v>
       </c>
       <c r="CD77" t="n">
-        <v>2</v>
+        <v>1.984</v>
       </c>
     </row>
     <row r="78">
@@ -19541,8 +19823,12 @@
         </is>
       </c>
       <c r="AS78" t="inlineStr"/>
-      <c r="AT78" t="inlineStr"/>
-      <c r="AU78" t="inlineStr"/>
+      <c r="AT78" t="n">
+        <v>0.104166664</v>
+      </c>
+      <c r="AU78" t="n">
+        <v>0.104166664</v>
+      </c>
       <c r="AV78" t="inlineStr"/>
       <c r="AW78" t="inlineStr"/>
       <c r="AX78" t="inlineStr"/>
@@ -19810,8 +20096,12 @@
       <c r="AQ79" t="inlineStr"/>
       <c r="AR79" t="inlineStr"/>
       <c r="AS79" t="inlineStr"/>
-      <c r="AT79" t="inlineStr"/>
-      <c r="AU79" t="inlineStr"/>
+      <c r="AT79" t="n">
+        <v>0.104166664</v>
+      </c>
+      <c r="AU79" t="n">
+        <v>0.104166664</v>
+      </c>
       <c r="AV79" t="inlineStr"/>
       <c r="AW79" t="inlineStr"/>
       <c r="AX79" t="inlineStr"/>
@@ -19844,22 +20134,22 @@
       <c r="BM79" t="inlineStr"/>
       <c r="BN79" t="inlineStr">
         <is>
-          <t>n36ffb28c8eac416b8b80b55bd7694105b3, n36ffb28c8eac416b8b80b55bd7694105b5</t>
+          <t>n1855b57938dd4b1e92b12a25be7ea42bb3, n1855b57938dd4b1e92b12a25be7ea42bb5</t>
         </is>
       </c>
       <c r="BO79" t="inlineStr">
         <is>
-          <t>['n36ffb28c8eac416b8b80b55bd7694105b3', 'n36ffb28c8eac416b8b80b55bd7694105b5']</t>
+          <t>['n1855b57938dd4b1e92b12a25be7ea42bb3', 'n1855b57938dd4b1e92b12a25be7ea42bb5']</t>
         </is>
       </c>
       <c r="BP79" t="inlineStr">
         <is>
-          <t>n36ffb28c8eac416b8b80b55bd7694105b7</t>
+          <t>n1855b57938dd4b1e92b12a25be7ea42bb7</t>
         </is>
       </c>
       <c r="BQ79" t="inlineStr">
         <is>
-          <t>n36ffb28c8eac416b8b80b55bd7694105b7</t>
+          <t>n1855b57938dd4b1e92b12a25be7ea42bb7</t>
         </is>
       </c>
       <c r="BR79" t="inlineStr">
@@ -19901,7 +20191,7 @@
         <v>3</v>
       </c>
       <c r="CD79" t="n">
-        <v>2</v>
+        <v>1.896</v>
       </c>
     </row>
     <row r="80">
@@ -20004,8 +20294,12 @@
       <c r="AQ80" t="inlineStr"/>
       <c r="AR80" t="inlineStr"/>
       <c r="AS80" t="inlineStr"/>
-      <c r="AT80" t="inlineStr"/>
-      <c r="AU80" t="inlineStr"/>
+      <c r="AT80" t="n">
+        <v>0.041666668</v>
+      </c>
+      <c r="AU80" t="n">
+        <v>0.041666668</v>
+      </c>
       <c r="AV80" t="inlineStr"/>
       <c r="AW80" t="inlineStr"/>
       <c r="AX80" t="inlineStr"/>
@@ -20244,8 +20538,12 @@
         </is>
       </c>
       <c r="AS81" t="inlineStr"/>
-      <c r="AT81" t="inlineStr"/>
-      <c r="AU81" t="inlineStr"/>
+      <c r="AT81" t="n">
+        <v>0.104166664</v>
+      </c>
+      <c r="AU81" t="n">
+        <v>0.104166664</v>
+      </c>
       <c r="AV81" t="inlineStr"/>
       <c r="AW81" t="inlineStr"/>
       <c r="AX81" t="inlineStr"/>
@@ -20343,7 +20641,7 @@
         <v>3</v>
       </c>
       <c r="CD81" t="n">
-        <v>2</v>
+        <v>1.865</v>
       </c>
     </row>
     <row r="82">
@@ -20462,8 +20760,12 @@
       <c r="AQ82" t="inlineStr"/>
       <c r="AR82" t="inlineStr"/>
       <c r="AS82" t="inlineStr"/>
-      <c r="AT82" t="inlineStr"/>
-      <c r="AU82" t="inlineStr"/>
+      <c r="AT82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU82" t="n">
+        <v>0</v>
+      </c>
       <c r="AV82" t="inlineStr"/>
       <c r="AW82" t="inlineStr"/>
       <c r="AX82" t="inlineStr"/>
@@ -20711,8 +21013,12 @@
       <c r="AQ83" t="inlineStr"/>
       <c r="AR83" t="inlineStr"/>
       <c r="AS83" t="inlineStr"/>
-      <c r="AT83" t="inlineStr"/>
-      <c r="AU83" t="inlineStr"/>
+      <c r="AT83" t="n">
+        <v>0.87082696</v>
+      </c>
+      <c r="AU83" t="n">
+        <v>0.87082696</v>
+      </c>
       <c r="AV83" t="inlineStr">
         <is>
           <t>LOIN</t>
@@ -20761,22 +21067,22 @@
       <c r="BM83" t="inlineStr"/>
       <c r="BN83" t="inlineStr">
         <is>
-          <t>nc11c0815d0b748b4a3f5be276dcfcea3b3, nc11c0815d0b748b4a3f5be276dcfcea3b5</t>
+          <t>ne269ecf3bfd34bc89e28c40f8506748cb3, ne269ecf3bfd34bc89e28c40f8506748cb5</t>
         </is>
       </c>
       <c r="BO83" t="inlineStr">
         <is>
-          <t>['nc11c0815d0b748b4a3f5be276dcfcea3b3', 'nc11c0815d0b748b4a3f5be276dcfcea3b5']</t>
+          <t>['ne269ecf3bfd34bc89e28c40f8506748cb3', 'ne269ecf3bfd34bc89e28c40f8506748cb5']</t>
         </is>
       </c>
       <c r="BP83" t="inlineStr">
         <is>
-          <t>nc11c0815d0b748b4a3f5be276dcfcea3b7</t>
+          <t>ne269ecf3bfd34bc89e28c40f8506748cb7</t>
         </is>
       </c>
       <c r="BQ83" t="inlineStr">
         <is>
-          <t>nc11c0815d0b748b4a3f5be276dcfcea3b7</t>
+          <t>ne269ecf3bfd34bc89e28c40f8506748cb7</t>
         </is>
       </c>
       <c r="BR83" t="inlineStr">
@@ -20818,7 +21124,7 @@
         <v>3</v>
       </c>
       <c r="CD83" t="n">
-        <v>2</v>
+        <v>1.815</v>
       </c>
     </row>
     <row r="84">
@@ -20987,8 +21293,12 @@
         </is>
       </c>
       <c r="AS84" t="inlineStr"/>
-      <c r="AT84" t="inlineStr"/>
-      <c r="AU84" t="inlineStr"/>
+      <c r="AT84" t="n">
+        <v>0.104166664</v>
+      </c>
+      <c r="AU84" t="n">
+        <v>0.104166664</v>
+      </c>
       <c r="AV84" t="inlineStr"/>
       <c r="AW84" t="inlineStr"/>
       <c r="AX84" t="inlineStr"/>
@@ -21094,7 +21404,7 @@
         <v>3</v>
       </c>
       <c r="CD84" t="n">
-        <v>1</v>
+        <v>1.179</v>
       </c>
     </row>
     <row r="85">
@@ -21251,8 +21561,12 @@
       <c r="AQ85" t="inlineStr"/>
       <c r="AR85" t="inlineStr"/>
       <c r="AS85" t="inlineStr"/>
-      <c r="AT85" t="inlineStr"/>
-      <c r="AU85" t="inlineStr"/>
+      <c r="AT85" t="n">
+        <v>0.14583333</v>
+      </c>
+      <c r="AU85" t="n">
+        <v>0.14583333</v>
+      </c>
       <c r="AV85" t="inlineStr"/>
       <c r="AW85" t="inlineStr"/>
       <c r="AX85" t="inlineStr"/>
@@ -21342,7 +21656,7 @@
         <v>3</v>
       </c>
       <c r="CD85" t="n">
-        <v>2</v>
+        <v>1.933</v>
       </c>
     </row>
     <row r="86">
@@ -21505,8 +21819,12 @@
       <c r="AQ86" t="inlineStr"/>
       <c r="AR86" t="inlineStr"/>
       <c r="AS86" t="inlineStr"/>
-      <c r="AT86" t="inlineStr"/>
-      <c r="AU86" t="inlineStr"/>
+      <c r="AT86" t="n">
+        <v>0.104166664</v>
+      </c>
+      <c r="AU86" t="n">
+        <v>0.104166664</v>
+      </c>
       <c r="AV86" t="inlineStr"/>
       <c r="AW86" t="inlineStr"/>
       <c r="AX86" t="inlineStr"/>
@@ -21547,12 +21865,12 @@
       </c>
       <c r="BN86" t="inlineStr">
         <is>
-          <t>nfd8ded3ccf0b4104a6a57ac23c99ccf8b1</t>
+          <t>na3f8de111d8a4b30abd84e3c819094bfb1</t>
         </is>
       </c>
       <c r="BO86" t="inlineStr">
         <is>
-          <t>['nfd8ded3ccf0b4104a6a57ac23c99ccf8b1']</t>
+          <t>['na3f8de111d8a4b30abd84e3c819094bfb1']</t>
         </is>
       </c>
       <c r="BP86" t="inlineStr"/>
@@ -21596,7 +21914,7 @@
         <v>3</v>
       </c>
       <c r="CD86" t="n">
-        <v>2</v>
+        <v>1.994</v>
       </c>
     </row>
     <row r="87">
@@ -21719,8 +22037,12 @@
       <c r="AQ87" t="inlineStr"/>
       <c r="AR87" t="inlineStr"/>
       <c r="AS87" t="inlineStr"/>
-      <c r="AT87" t="inlineStr"/>
-      <c r="AU87" t="inlineStr"/>
+      <c r="AT87" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU87" t="n">
+        <v>0</v>
+      </c>
       <c r="AV87" t="inlineStr"/>
       <c r="AW87" t="inlineStr"/>
       <c r="AX87" t="inlineStr"/>
@@ -21915,8 +22237,12 @@
       <c r="AQ88" t="inlineStr"/>
       <c r="AR88" t="inlineStr"/>
       <c r="AS88" t="inlineStr"/>
-      <c r="AT88" t="inlineStr"/>
-      <c r="AU88" t="inlineStr"/>
+      <c r="AT88" t="n">
+        <v>0.20833333</v>
+      </c>
+      <c r="AU88" t="n">
+        <v>0.20833333</v>
+      </c>
       <c r="AV88" t="inlineStr">
         <is>
           <t>NEN 2660-2:2022 nl</t>
@@ -22141,8 +22467,12 @@
         </is>
       </c>
       <c r="AS89" t="inlineStr"/>
-      <c r="AT89" t="inlineStr"/>
-      <c r="AU89" t="inlineStr"/>
+      <c r="AT89" t="n">
+        <v>0.20833333</v>
+      </c>
+      <c r="AU89" t="n">
+        <v>0.20833333</v>
+      </c>
       <c r="AV89" t="inlineStr">
         <is>
           <t>NEN 2660-2:2022 nl</t>
@@ -22236,7 +22566,7 @@
         <v>3</v>
       </c>
       <c r="CD89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90">
@@ -22351,8 +22681,12 @@
       <c r="AQ90" t="inlineStr"/>
       <c r="AR90" t="inlineStr"/>
       <c r="AS90" t="inlineStr"/>
-      <c r="AT90" t="inlineStr"/>
-      <c r="AU90" t="inlineStr"/>
+      <c r="AT90" t="n">
+        <v>0.104166664</v>
+      </c>
+      <c r="AU90" t="n">
+        <v>0.104166664</v>
+      </c>
       <c r="AV90" t="inlineStr"/>
       <c r="AW90" t="inlineStr"/>
       <c r="AX90" t="inlineStr"/>
@@ -22422,7 +22756,7 @@
         <v>3</v>
       </c>
       <c r="CD90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91">
@@ -22603,8 +22937,12 @@
         </is>
       </c>
       <c r="AS91" t="inlineStr"/>
-      <c r="AT91" t="inlineStr"/>
-      <c r="AU91" t="inlineStr"/>
+      <c r="AT91" t="n">
+        <v>0.14583333</v>
+      </c>
+      <c r="AU91" t="n">
+        <v>0.14583333</v>
+      </c>
       <c r="AV91" t="inlineStr"/>
       <c r="AW91" t="inlineStr"/>
       <c r="AX91" t="inlineStr"/>
@@ -22694,7 +23032,7 @@
         <v>3</v>
       </c>
       <c r="CD91" t="n">
-        <v>1</v>
+        <v>1.257</v>
       </c>
     </row>
     <row r="92">
@@ -22841,8 +23179,12 @@
       <c r="AQ92" t="inlineStr"/>
       <c r="AR92" t="inlineStr"/>
       <c r="AS92" t="inlineStr"/>
-      <c r="AT92" t="inlineStr"/>
-      <c r="AU92" t="inlineStr"/>
+      <c r="AT92" t="n">
+        <v>0.6527777299999999</v>
+      </c>
+      <c r="AU92" t="n">
+        <v>0.6527777299999999</v>
+      </c>
       <c r="AV92" t="inlineStr"/>
       <c r="AW92" t="inlineStr"/>
       <c r="AX92" t="inlineStr"/>
@@ -23100,8 +23442,12 @@
         </is>
       </c>
       <c r="AS93" t="inlineStr"/>
-      <c r="AT93" t="inlineStr"/>
-      <c r="AU93" t="inlineStr"/>
+      <c r="AT93" t="n">
+        <v>0.7708333000000001</v>
+      </c>
+      <c r="AU93" t="n">
+        <v>0.7708333000000001</v>
+      </c>
       <c r="AV93" t="inlineStr"/>
       <c r="AW93" t="inlineStr"/>
       <c r="AX93" t="inlineStr"/>
@@ -23191,7 +23537,7 @@
         <v>3</v>
       </c>
       <c r="CD93" t="n">
-        <v>2</v>
+        <v>1.833</v>
       </c>
     </row>
     <row r="94">
@@ -23300,8 +23646,12 @@
       <c r="AQ94" t="inlineStr"/>
       <c r="AR94" t="inlineStr"/>
       <c r="AS94" t="inlineStr"/>
-      <c r="AT94" t="inlineStr"/>
-      <c r="AU94" t="inlineStr"/>
+      <c r="AT94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU94" t="n">
+        <v>0</v>
+      </c>
       <c r="AV94" t="inlineStr">
         <is>
           <t>TS-0012</t>
@@ -23379,7 +23729,7 @@
         <v>2</v>
       </c>
       <c r="CD94" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95">
@@ -23486,8 +23836,12 @@
       <c r="AQ95" t="inlineStr"/>
       <c r="AR95" t="inlineStr"/>
       <c r="AS95" t="inlineStr"/>
-      <c r="AT95" t="inlineStr"/>
-      <c r="AU95" t="inlineStr"/>
+      <c r="AT95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU95" t="n">
+        <v>0</v>
+      </c>
       <c r="AV95" t="inlineStr"/>
       <c r="AW95" t="inlineStr"/>
       <c r="AX95" t="inlineStr"/>
@@ -23668,8 +24022,12 @@
       <c r="AQ96" t="inlineStr"/>
       <c r="AR96" t="inlineStr"/>
       <c r="AS96" t="inlineStr"/>
-      <c r="AT96" t="inlineStr"/>
-      <c r="AU96" t="inlineStr"/>
+      <c r="AT96" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU96" t="n">
+        <v>0</v>
+      </c>
       <c r="AV96" t="inlineStr"/>
       <c r="AW96" t="inlineStr"/>
       <c r="AX96" t="inlineStr"/>
@@ -23739,7 +24097,7 @@
         <v>2</v>
       </c>
       <c r="CD96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97">
@@ -23904,8 +24262,12 @@
       <c r="AQ97" t="inlineStr"/>
       <c r="AR97" t="inlineStr"/>
       <c r="AS97" t="inlineStr"/>
-      <c r="AT97" t="inlineStr"/>
-      <c r="AU97" t="inlineStr"/>
+      <c r="AT97" t="n">
+        <v>0.104166664</v>
+      </c>
+      <c r="AU97" t="n">
+        <v>0.104166664</v>
+      </c>
       <c r="AV97" t="inlineStr"/>
       <c r="AW97" t="inlineStr"/>
       <c r="AX97" t="inlineStr"/>
@@ -24011,7 +24373,7 @@
         <v>3</v>
       </c>
       <c r="CD97" t="n">
-        <v>2</v>
+        <v>1.963</v>
       </c>
     </row>
     <row r="98">
@@ -24170,8 +24532,12 @@
       <c r="AQ98" t="inlineStr"/>
       <c r="AR98" t="inlineStr"/>
       <c r="AS98" t="inlineStr"/>
-      <c r="AT98" t="inlineStr"/>
-      <c r="AU98" t="inlineStr"/>
+      <c r="AT98" t="n">
+        <v>0.14583333</v>
+      </c>
+      <c r="AU98" t="n">
+        <v>0.14583333</v>
+      </c>
       <c r="AV98" t="inlineStr"/>
       <c r="AW98" t="inlineStr"/>
       <c r="AX98" t="inlineStr"/>
@@ -24212,12 +24578,12 @@
       <c r="BM98" t="inlineStr"/>
       <c r="BN98" t="inlineStr">
         <is>
-          <t>n3aad4e1c1f00417297e72becc1c7650bb1, n3aad4e1c1f00417297e72becc1c7650bb2</t>
+          <t>n7907b3fb6d6c4be287c978cb92b27cabb1, n7907b3fb6d6c4be287c978cb92b27cabb2</t>
         </is>
       </c>
       <c r="BO98" t="inlineStr">
         <is>
-          <t>['n3aad4e1c1f00417297e72becc1c7650bb1', 'n3aad4e1c1f00417297e72becc1c7650bb2']</t>
+          <t>['n7907b3fb6d6c4be287c978cb92b27cabb1', 'n7907b3fb6d6c4be287c978cb92b27cabb2']</t>
         </is>
       </c>
       <c r="BP98" t="inlineStr"/>
@@ -24261,7 +24627,7 @@
         <v>3</v>
       </c>
       <c r="CD98" t="n">
-        <v>2</v>
+        <v>1.947</v>
       </c>
     </row>
     <row r="99">
@@ -24422,8 +24788,12 @@
       <c r="AQ99" t="inlineStr"/>
       <c r="AR99" t="inlineStr"/>
       <c r="AS99" t="inlineStr"/>
-      <c r="AT99" t="inlineStr"/>
-      <c r="AU99" t="inlineStr"/>
+      <c r="AT99" t="n">
+        <v>0.104166664</v>
+      </c>
+      <c r="AU99" t="n">
+        <v>0.104166664</v>
+      </c>
       <c r="AV99" t="inlineStr"/>
       <c r="AW99" t="inlineStr"/>
       <c r="AX99" t="inlineStr"/>
@@ -24682,8 +25052,12 @@
       <c r="AQ100" t="inlineStr"/>
       <c r="AR100" t="inlineStr"/>
       <c r="AS100" t="inlineStr"/>
-      <c r="AT100" t="inlineStr"/>
-      <c r="AU100" t="inlineStr"/>
+      <c r="AT100" t="n">
+        <v>0.104166664</v>
+      </c>
+      <c r="AU100" t="n">
+        <v>0.104166664</v>
+      </c>
       <c r="AV100" t="inlineStr"/>
       <c r="AW100" t="inlineStr"/>
       <c r="AX100" t="inlineStr"/>
@@ -24908,8 +25282,12 @@
       <c r="AQ101" t="inlineStr"/>
       <c r="AR101" t="inlineStr"/>
       <c r="AS101" t="inlineStr"/>
-      <c r="AT101" t="inlineStr"/>
-      <c r="AU101" t="inlineStr"/>
+      <c r="AT101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU101" t="n">
+        <v>0</v>
+      </c>
       <c r="AV101" t="inlineStr"/>
       <c r="AW101" t="inlineStr"/>
       <c r="AX101" t="inlineStr"/>
@@ -25134,8 +25512,12 @@
       <c r="AQ102" t="inlineStr"/>
       <c r="AR102" t="inlineStr"/>
       <c r="AS102" t="inlineStr"/>
-      <c r="AT102" t="inlineStr"/>
-      <c r="AU102" t="inlineStr"/>
+      <c r="AT102" t="n">
+        <v>0.14583333</v>
+      </c>
+      <c r="AU102" t="n">
+        <v>0.14583333</v>
+      </c>
       <c r="AV102" t="inlineStr"/>
       <c r="AW102" t="inlineStr"/>
       <c r="AX102" t="inlineStr"/>
@@ -25336,8 +25718,12 @@
       <c r="AQ103" t="inlineStr"/>
       <c r="AR103" t="inlineStr"/>
       <c r="AS103" t="inlineStr"/>
-      <c r="AT103" t="inlineStr"/>
-      <c r="AU103" t="inlineStr"/>
+      <c r="AT103" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU103" t="n">
+        <v>0</v>
+      </c>
       <c r="AV103" t="inlineStr"/>
       <c r="AW103" t="inlineStr"/>
       <c r="AX103" t="inlineStr"/>
@@ -25568,8 +25954,12 @@
       <c r="AQ104" t="inlineStr"/>
       <c r="AR104" t="inlineStr"/>
       <c r="AS104" t="inlineStr"/>
-      <c r="AT104" t="inlineStr"/>
-      <c r="AU104" t="inlineStr"/>
+      <c r="AT104" t="n">
+        <v>0.104166664</v>
+      </c>
+      <c r="AU104" t="n">
+        <v>0.104166664</v>
+      </c>
       <c r="AV104" t="inlineStr"/>
       <c r="AW104" t="inlineStr"/>
       <c r="AX104" t="inlineStr"/>
@@ -25675,7 +26065,7 @@
         <v>3</v>
       </c>
       <c r="CD104" t="n">
-        <v>1</v>
+        <v>1.462</v>
       </c>
     </row>
     <row r="105">
@@ -25844,8 +26234,12 @@
         </is>
       </c>
       <c r="AS105" t="inlineStr"/>
-      <c r="AT105" t="inlineStr"/>
-      <c r="AU105" t="inlineStr"/>
+      <c r="AT105" t="n">
+        <v>0.104166664</v>
+      </c>
+      <c r="AU105" t="n">
+        <v>0.104166664</v>
+      </c>
       <c r="AV105" t="inlineStr"/>
       <c r="AW105" t="inlineStr"/>
       <c r="AX105" t="inlineStr"/>
@@ -26122,8 +26516,12 @@
       <c r="AQ106" t="inlineStr"/>
       <c r="AR106" t="inlineStr"/>
       <c r="AS106" t="inlineStr"/>
-      <c r="AT106" t="inlineStr"/>
-      <c r="AU106" t="inlineStr"/>
+      <c r="AT106" t="n">
+        <v>0.9270833000000001</v>
+      </c>
+      <c r="AU106" t="n">
+        <v>0.9270833000000001</v>
+      </c>
       <c r="AV106" t="inlineStr"/>
       <c r="AW106" t="inlineStr"/>
       <c r="AX106" t="inlineStr"/>
@@ -26404,8 +26802,12 @@
       <c r="AQ107" t="inlineStr"/>
       <c r="AR107" t="inlineStr"/>
       <c r="AS107" t="inlineStr"/>
-      <c r="AT107" t="inlineStr"/>
-      <c r="AU107" t="inlineStr"/>
+      <c r="AT107" t="n">
+        <v>0.7708333000000001</v>
+      </c>
+      <c r="AU107" t="n">
+        <v>0.7708333000000001</v>
+      </c>
       <c r="AV107" t="inlineStr"/>
       <c r="AW107" t="inlineStr"/>
       <c r="AX107" t="inlineStr"/>
@@ -26702,8 +27104,12 @@
         </is>
       </c>
       <c r="AS108" t="inlineStr"/>
-      <c r="AT108" t="inlineStr"/>
-      <c r="AU108" t="inlineStr"/>
+      <c r="AT108" t="n">
+        <v>0.8541666999999999</v>
+      </c>
+      <c r="AU108" t="n">
+        <v>0.8541666999999999</v>
+      </c>
       <c r="AV108" t="inlineStr">
         <is>
           <t xml:space="preserve">ISO 16739 </t>
@@ -27008,8 +27414,12 @@
         </is>
       </c>
       <c r="AS109" t="inlineStr"/>
-      <c r="AT109" t="inlineStr"/>
-      <c r="AU109" t="inlineStr"/>
+      <c r="AT109" t="n">
+        <v>0.8958333000000001</v>
+      </c>
+      <c r="AU109" t="n">
+        <v>0.8958333000000001</v>
+      </c>
       <c r="AV109" t="inlineStr"/>
       <c r="AW109" t="inlineStr"/>
       <c r="AX109" t="inlineStr"/>
@@ -27308,8 +27718,12 @@
       <c r="AQ110" t="inlineStr"/>
       <c r="AR110" t="inlineStr"/>
       <c r="AS110" t="inlineStr"/>
-      <c r="AT110" t="inlineStr"/>
-      <c r="AU110" t="inlineStr"/>
+      <c r="AT110" t="n">
+        <v>0.8958333000000001</v>
+      </c>
+      <c r="AU110" t="n">
+        <v>0.8958333000000001</v>
+      </c>
       <c r="AV110" t="inlineStr"/>
       <c r="AW110" t="inlineStr"/>
       <c r="AX110" t="inlineStr"/>
@@ -27605,8 +28019,12 @@
       <c r="AQ111" t="inlineStr"/>
       <c r="AR111" t="inlineStr"/>
       <c r="AS111" t="inlineStr"/>
-      <c r="AT111" t="inlineStr"/>
-      <c r="AU111" t="inlineStr"/>
+      <c r="AT111" t="n">
+        <v>0.8958333000000001</v>
+      </c>
+      <c r="AU111" t="n">
+        <v>0.8958333000000001</v>
+      </c>
       <c r="AV111" t="inlineStr"/>
       <c r="AW111" t="inlineStr"/>
       <c r="AX111" t="inlineStr"/>
@@ -27895,8 +28313,12 @@
       <c r="AQ112" t="inlineStr"/>
       <c r="AR112" t="inlineStr"/>
       <c r="AS112" t="inlineStr"/>
-      <c r="AT112" t="inlineStr"/>
-      <c r="AU112" t="inlineStr"/>
+      <c r="AT112" t="n">
+        <v>0.8958333000000001</v>
+      </c>
+      <c r="AU112" t="n">
+        <v>0.8958333000000001</v>
+      </c>
       <c r="AV112" t="inlineStr"/>
       <c r="AW112" t="inlineStr"/>
       <c r="AX112" t="inlineStr"/>
@@ -28185,8 +28607,12 @@
       <c r="AQ113" t="inlineStr"/>
       <c r="AR113" t="inlineStr"/>
       <c r="AS113" t="inlineStr"/>
-      <c r="AT113" t="inlineStr"/>
-      <c r="AU113" t="inlineStr"/>
+      <c r="AT113" t="n">
+        <v>0.7708333000000001</v>
+      </c>
+      <c r="AU113" t="n">
+        <v>0.7708333000000001</v>
+      </c>
       <c r="AV113" t="inlineStr"/>
       <c r="AW113" t="inlineStr"/>
       <c r="AX113" t="inlineStr"/>
@@ -28479,8 +28905,12 @@
       <c r="AQ114" t="inlineStr"/>
       <c r="AR114" t="inlineStr"/>
       <c r="AS114" t="inlineStr"/>
-      <c r="AT114" t="inlineStr"/>
-      <c r="AU114" t="inlineStr"/>
+      <c r="AT114" t="n">
+        <v>0.9270833000000001</v>
+      </c>
+      <c r="AU114" t="n">
+        <v>0.9270833000000001</v>
+      </c>
       <c r="AV114" t="inlineStr"/>
       <c r="AW114" t="inlineStr"/>
       <c r="AX114" t="inlineStr"/>
@@ -28769,8 +29199,12 @@
       <c r="AQ115" t="inlineStr"/>
       <c r="AR115" t="inlineStr"/>
       <c r="AS115" t="inlineStr"/>
-      <c r="AT115" t="inlineStr"/>
-      <c r="AU115" t="inlineStr"/>
+      <c r="AT115" t="n">
+        <v>0.7708333000000001</v>
+      </c>
+      <c r="AU115" t="n">
+        <v>0.7708333000000001</v>
+      </c>
       <c r="AV115" t="inlineStr"/>
       <c r="AW115" t="inlineStr"/>
       <c r="AX115" t="inlineStr"/>
@@ -29073,8 +29507,12 @@
         </is>
       </c>
       <c r="AS116" t="inlineStr"/>
-      <c r="AT116" t="inlineStr"/>
-      <c r="AU116" t="inlineStr"/>
+      <c r="AT116" t="n">
+        <v>0.8541666999999999</v>
+      </c>
+      <c r="AU116" t="n">
+        <v>0.8541666999999999</v>
+      </c>
       <c r="AV116" t="inlineStr"/>
       <c r="AW116" t="inlineStr"/>
       <c r="AX116" t="inlineStr"/>
@@ -29355,8 +29793,12 @@
       <c r="AQ117" t="inlineStr"/>
       <c r="AR117" t="inlineStr"/>
       <c r="AS117" t="inlineStr"/>
-      <c r="AT117" t="inlineStr"/>
-      <c r="AU117" t="inlineStr"/>
+      <c r="AT117" t="n">
+        <v>0.8958333000000001</v>
+      </c>
+      <c r="AU117" t="n">
+        <v>0.8958333000000001</v>
+      </c>
       <c r="AV117" t="inlineStr"/>
       <c r="AW117" t="inlineStr"/>
       <c r="AX117" t="inlineStr"/>
@@ -29657,8 +30099,12 @@
         </is>
       </c>
       <c r="AS118" t="inlineStr"/>
-      <c r="AT118" t="inlineStr"/>
-      <c r="AU118" t="inlineStr"/>
+      <c r="AT118" t="n">
+        <v>0.9270833000000001</v>
+      </c>
+      <c r="AU118" t="n">
+        <v>0.9270833000000001</v>
+      </c>
       <c r="AV118" t="inlineStr"/>
       <c r="AW118" t="inlineStr"/>
       <c r="AX118" t="inlineStr"/>
@@ -29925,8 +30371,12 @@
       <c r="AQ119" t="inlineStr"/>
       <c r="AR119" t="inlineStr"/>
       <c r="AS119" t="inlineStr"/>
-      <c r="AT119" t="inlineStr"/>
-      <c r="AU119" t="inlineStr"/>
+      <c r="AT119" t="n">
+        <v>0.104166664</v>
+      </c>
+      <c r="AU119" t="n">
+        <v>0.104166664</v>
+      </c>
       <c r="AV119" t="inlineStr"/>
       <c r="AW119" t="inlineStr"/>
       <c r="AX119" t="inlineStr"/>
@@ -30145,8 +30595,12 @@
       <c r="AQ120" t="inlineStr"/>
       <c r="AR120" t="inlineStr"/>
       <c r="AS120" t="inlineStr"/>
-      <c r="AT120" t="inlineStr"/>
-      <c r="AU120" t="inlineStr"/>
+      <c r="AT120" t="n">
+        <v>0.104166664</v>
+      </c>
+      <c r="AU120" t="n">
+        <v>0.104166664</v>
+      </c>
       <c r="AV120" t="inlineStr"/>
       <c r="AW120" t="inlineStr"/>
       <c r="AX120" t="inlineStr"/>
@@ -30399,8 +30853,12 @@
         </is>
       </c>
       <c r="AS121" t="inlineStr"/>
-      <c r="AT121" t="inlineStr"/>
-      <c r="AU121" t="inlineStr"/>
+      <c r="AT121" t="n">
+        <v>0.8958333000000001</v>
+      </c>
+      <c r="AU121" t="n">
+        <v>0.8958333000000001</v>
+      </c>
       <c r="AV121" t="inlineStr"/>
       <c r="AW121" t="inlineStr"/>
       <c r="AX121" t="inlineStr"/>
@@ -30681,8 +31139,12 @@
       <c r="AQ122" t="inlineStr"/>
       <c r="AR122" t="inlineStr"/>
       <c r="AS122" t="inlineStr"/>
-      <c r="AT122" t="inlineStr"/>
-      <c r="AU122" t="inlineStr"/>
+      <c r="AT122" t="n">
+        <v>0.76388884</v>
+      </c>
+      <c r="AU122" t="n">
+        <v>0.76388884</v>
+      </c>
       <c r="AV122" t="inlineStr"/>
       <c r="AW122" t="inlineStr"/>
       <c r="AX122" t="inlineStr"/>
@@ -30883,8 +31345,12 @@
       <c r="AQ123" t="inlineStr"/>
       <c r="AR123" t="inlineStr"/>
       <c r="AS123" t="inlineStr"/>
-      <c r="AT123" t="inlineStr"/>
-      <c r="AU123" t="inlineStr"/>
+      <c r="AT123" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU123" t="n">
+        <v>0</v>
+      </c>
       <c r="AV123" t="inlineStr"/>
       <c r="AW123" t="inlineStr"/>
       <c r="AX123" t="inlineStr"/>
@@ -31057,8 +31523,12 @@
       <c r="AQ124" t="inlineStr"/>
       <c r="AR124" t="inlineStr"/>
       <c r="AS124" t="inlineStr"/>
-      <c r="AT124" t="inlineStr"/>
-      <c r="AU124" t="inlineStr"/>
+      <c r="AT124" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU124" t="n">
+        <v>0</v>
+      </c>
       <c r="AV124" t="inlineStr"/>
       <c r="AW124" t="inlineStr"/>
       <c r="AX124" t="inlineStr"/>
@@ -31293,8 +31763,12 @@
       <c r="AQ125" t="inlineStr"/>
       <c r="AR125" t="inlineStr"/>
       <c r="AS125" t="inlineStr"/>
-      <c r="AT125" t="inlineStr"/>
-      <c r="AU125" t="inlineStr"/>
+      <c r="AT125" t="n">
+        <v>0.104166664</v>
+      </c>
+      <c r="AU125" t="n">
+        <v>0.104166664</v>
+      </c>
       <c r="AV125" t="inlineStr"/>
       <c r="AW125" t="inlineStr"/>
       <c r="AX125" t="inlineStr"/>
@@ -31547,8 +32021,12 @@
       <c r="AQ126" t="inlineStr"/>
       <c r="AR126" t="inlineStr"/>
       <c r="AS126" t="inlineStr"/>
-      <c r="AT126" t="inlineStr"/>
-      <c r="AU126" t="inlineStr"/>
+      <c r="AT126" t="n">
+        <v>0.041666668</v>
+      </c>
+      <c r="AU126" t="n">
+        <v>0.041666668</v>
+      </c>
       <c r="AV126" t="inlineStr"/>
       <c r="AW126" t="inlineStr"/>
       <c r="AX126" t="inlineStr"/>
@@ -31745,8 +32223,12 @@
       <c r="AQ127" t="inlineStr"/>
       <c r="AR127" t="inlineStr"/>
       <c r="AS127" t="inlineStr"/>
-      <c r="AT127" t="inlineStr"/>
-      <c r="AU127" t="inlineStr"/>
+      <c r="AT127" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU127" t="n">
+        <v>0</v>
+      </c>
       <c r="AV127" t="inlineStr"/>
       <c r="AW127" t="inlineStr"/>
       <c r="AX127" t="inlineStr"/>
@@ -31939,8 +32421,12 @@
       <c r="AQ128" t="inlineStr"/>
       <c r="AR128" t="inlineStr"/>
       <c r="AS128" t="inlineStr"/>
-      <c r="AT128" t="inlineStr"/>
-      <c r="AU128" t="inlineStr"/>
+      <c r="AT128" t="n">
+        <v>0.14583333</v>
+      </c>
+      <c r="AU128" t="n">
+        <v>0.14583333</v>
+      </c>
       <c r="AV128" t="inlineStr">
         <is>
           <t>CEN EN 17632-1:2022, CEN EN 17632-2:2025</t>
@@ -32034,7 +32520,7 @@
         <v>3</v>
       </c>
       <c r="CD128" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129">
@@ -32149,8 +32635,12 @@
       <c r="AQ129" t="inlineStr"/>
       <c r="AR129" t="inlineStr"/>
       <c r="AS129" t="inlineStr"/>
-      <c r="AT129" t="inlineStr"/>
-      <c r="AU129" t="inlineStr"/>
+      <c r="AT129" t="n">
+        <v>0.14583333</v>
+      </c>
+      <c r="AU129" t="n">
+        <v>0.14583333</v>
+      </c>
       <c r="AV129" t="inlineStr">
         <is>
           <t>CEN EN 17632-1:2022, CEN EN 17632-2:2024</t>
@@ -32244,7 +32734,7 @@
         <v>3</v>
       </c>
       <c r="CD129" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130">
@@ -32387,8 +32877,12 @@
         </is>
       </c>
       <c r="AS130" t="inlineStr"/>
-      <c r="AT130" t="inlineStr"/>
-      <c r="AU130" t="inlineStr"/>
+      <c r="AT130" t="n">
+        <v>0.8055556</v>
+      </c>
+      <c r="AU130" t="n">
+        <v>0.8055556</v>
+      </c>
       <c r="AV130" t="inlineStr"/>
       <c r="AW130" t="inlineStr"/>
       <c r="AX130" t="inlineStr"/>
@@ -32429,12 +32923,12 @@
       <c r="BM130" t="inlineStr"/>
       <c r="BN130" t="inlineStr">
         <is>
-          <t>nbcb870bc0db648d4a0fcddfc1c38dfd5b1</t>
+          <t>n8d24cdc3698f49e1a74cb3a7ad364d77b1</t>
         </is>
       </c>
       <c r="BO130" t="inlineStr">
         <is>
-          <t>['nbcb870bc0db648d4a0fcddfc1c38dfd5b1']</t>
+          <t>['n8d24cdc3698f49e1a74cb3a7ad364d77b1']</t>
         </is>
       </c>
       <c r="BP130" t="inlineStr"/>
@@ -32653,8 +33147,12 @@
         </is>
       </c>
       <c r="AS131" t="inlineStr"/>
-      <c r="AT131" t="inlineStr"/>
-      <c r="AU131" t="inlineStr"/>
+      <c r="AT131" t="n">
+        <v>0.8159722700000001</v>
+      </c>
+      <c r="AU131" t="n">
+        <v>0.8159722700000001</v>
+      </c>
       <c r="AV131" t="inlineStr"/>
       <c r="AW131" t="inlineStr"/>
       <c r="AX131" t="inlineStr"/>
@@ -32695,12 +33193,12 @@
       <c r="BM131" t="inlineStr"/>
       <c r="BN131" t="inlineStr">
         <is>
-          <t>n731bfc8356dd4934a46218a807f66e23b1</t>
+          <t>nf04f46bae1224b61be6d1b764f6ff66db1</t>
         </is>
       </c>
       <c r="BO131" t="inlineStr">
         <is>
-          <t>['n731bfc8356dd4934a46218a807f66e23b1']</t>
+          <t>['nf04f46bae1224b61be6d1b764f6ff66db1']</t>
         </is>
       </c>
       <c r="BP131" t="inlineStr"/>
@@ -32884,8 +33382,12 @@
       <c r="AQ132" t="inlineStr"/>
       <c r="AR132" t="inlineStr"/>
       <c r="AS132" t="inlineStr"/>
-      <c r="AT132" t="inlineStr"/>
-      <c r="AU132" t="inlineStr"/>
+      <c r="AT132" t="n">
+        <v>0.104166664</v>
+      </c>
+      <c r="AU132" t="n">
+        <v>0.104166664</v>
+      </c>
       <c r="AV132" t="inlineStr"/>
       <c r="AW132" t="inlineStr"/>
       <c r="AX132" t="inlineStr"/>
@@ -33110,8 +33612,12 @@
         </is>
       </c>
       <c r="AS133" t="inlineStr"/>
-      <c r="AT133" t="inlineStr"/>
-      <c r="AU133" t="inlineStr"/>
+      <c r="AT133" t="n">
+        <v>0.8273566</v>
+      </c>
+      <c r="AU133" t="n">
+        <v>0.8273566</v>
+      </c>
       <c r="AV133" t="inlineStr">
         <is>
           <t>ISO 23386, ISO 23387, ISO 7817</t>
@@ -33189,7 +33695,7 @@
         <v>3</v>
       </c>
       <c r="CD133" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134">
@@ -33300,8 +33806,12 @@
       <c r="AQ134" t="inlineStr"/>
       <c r="AR134" t="inlineStr"/>
       <c r="AS134" t="inlineStr"/>
-      <c r="AT134" t="inlineStr"/>
-      <c r="AU134" t="inlineStr"/>
+      <c r="AT134" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU134" t="n">
+        <v>0</v>
+      </c>
       <c r="AV134" t="inlineStr"/>
       <c r="AW134" t="inlineStr"/>
       <c r="AX134" t="inlineStr"/>
@@ -33371,7 +33881,7 @@
         <v>2</v>
       </c>
       <c r="CD134" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135">
@@ -33482,8 +33992,12 @@
       <c r="AQ135" t="inlineStr"/>
       <c r="AR135" t="inlineStr"/>
       <c r="AS135" t="inlineStr"/>
-      <c r="AT135" t="inlineStr"/>
-      <c r="AU135" t="inlineStr"/>
+      <c r="AT135" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU135" t="n">
+        <v>0</v>
+      </c>
       <c r="AV135" t="inlineStr"/>
       <c r="AW135" t="inlineStr"/>
       <c r="AX135" t="inlineStr"/>
@@ -33666,9 +34180,11 @@
       <c r="AS136" t="n">
         <v>15</v>
       </c>
-      <c r="AT136" t="inlineStr"/>
+      <c r="AT136" t="n">
+        <v>0</v>
+      </c>
       <c r="AU136" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AV136" t="inlineStr"/>
       <c r="AW136" t="inlineStr"/>
@@ -33739,7 +34255,7 @@
         <v>2</v>
       </c>
       <c r="CD136" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137">
@@ -33850,8 +34366,12 @@
       <c r="AQ137" t="inlineStr"/>
       <c r="AR137" t="inlineStr"/>
       <c r="AS137" t="inlineStr"/>
-      <c r="AT137" t="inlineStr"/>
-      <c r="AU137" t="inlineStr"/>
+      <c r="AT137" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU137" t="n">
+        <v>0</v>
+      </c>
       <c r="AV137" t="inlineStr"/>
       <c r="AW137" t="inlineStr"/>
       <c r="AX137" t="inlineStr"/>
@@ -33921,7 +34441,7 @@
         <v>1</v>
       </c>
       <c r="CD137" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138">
@@ -34024,8 +34544,12 @@
       <c r="AQ138" t="inlineStr"/>
       <c r="AR138" t="inlineStr"/>
       <c r="AS138" t="inlineStr"/>
-      <c r="AT138" t="inlineStr"/>
-      <c r="AU138" t="inlineStr"/>
+      <c r="AT138" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU138" t="n">
+        <v>0</v>
+      </c>
       <c r="AV138" t="inlineStr"/>
       <c r="AW138" t="inlineStr"/>
       <c r="AX138" t="inlineStr"/>
@@ -34206,8 +34730,12 @@
       <c r="AQ139" t="inlineStr"/>
       <c r="AR139" t="inlineStr"/>
       <c r="AS139" t="inlineStr"/>
-      <c r="AT139" t="inlineStr"/>
-      <c r="AU139" t="inlineStr"/>
+      <c r="AT139" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU139" t="n">
+        <v>0</v>
+      </c>
       <c r="AV139" t="inlineStr"/>
       <c r="AW139" t="inlineStr"/>
       <c r="AX139" t="inlineStr"/>
@@ -34376,8 +34904,12 @@
       <c r="AQ140" t="inlineStr"/>
       <c r="AR140" t="inlineStr"/>
       <c r="AS140" t="inlineStr"/>
-      <c r="AT140" t="inlineStr"/>
-      <c r="AU140" t="inlineStr"/>
+      <c r="AT140" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU140" t="n">
+        <v>0</v>
+      </c>
       <c r="AV140" t="inlineStr"/>
       <c r="AW140" t="inlineStr"/>
       <c r="AX140" t="inlineStr"/>
@@ -34601,8 +35133,12 @@
       <c r="AQ141" t="inlineStr"/>
       <c r="AR141" t="inlineStr"/>
       <c r="AS141" t="inlineStr"/>
-      <c r="AT141" t="inlineStr"/>
-      <c r="AU141" t="inlineStr"/>
+      <c r="AT141" t="n">
+        <v>0.14583333</v>
+      </c>
+      <c r="AU141" t="n">
+        <v>0.14583333</v>
+      </c>
       <c r="AV141" t="inlineStr"/>
       <c r="AW141" t="inlineStr"/>
       <c r="AX141" t="inlineStr"/>
@@ -34692,7 +35228,7 @@
         <v>3</v>
       </c>
       <c r="CD141" t="n">
-        <v>1</v>
+        <v>1.014</v>
       </c>
     </row>
     <row r="142">
@@ -34791,8 +35327,12 @@
       <c r="AQ142" t="inlineStr"/>
       <c r="AR142" t="inlineStr"/>
       <c r="AS142" t="inlineStr"/>
-      <c r="AT142" t="inlineStr"/>
-      <c r="AU142" t="inlineStr"/>
+      <c r="AT142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU142" t="n">
+        <v>0</v>
+      </c>
       <c r="AV142" t="inlineStr"/>
       <c r="AW142" t="inlineStr"/>
       <c r="AX142" t="inlineStr"/>
@@ -34989,8 +35529,12 @@
       <c r="AQ143" t="inlineStr"/>
       <c r="AR143" t="inlineStr"/>
       <c r="AS143" t="inlineStr"/>
-      <c r="AT143" t="inlineStr"/>
-      <c r="AU143" t="inlineStr"/>
+      <c r="AT143" t="n">
+        <v>0.104166664</v>
+      </c>
+      <c r="AU143" t="n">
+        <v>0.104166664</v>
+      </c>
       <c r="AV143" t="inlineStr"/>
       <c r="AW143" t="inlineStr"/>
       <c r="AX143" t="inlineStr"/>
@@ -35068,7 +35612,7 @@
         <v>3</v>
       </c>
       <c r="CD143" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144">
@@ -35179,9 +35723,11 @@
       <c r="AS144" t="n">
         <v>30</v>
       </c>
-      <c r="AT144" t="inlineStr"/>
+      <c r="AT144" t="n">
+        <v>0</v>
+      </c>
       <c r="AU144" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="AV144" t="inlineStr"/>
       <c r="AW144" t="inlineStr"/>
@@ -35371,8 +35917,12 @@
       <c r="AQ145" t="inlineStr"/>
       <c r="AR145" t="inlineStr"/>
       <c r="AS145" t="inlineStr"/>
-      <c r="AT145" t="inlineStr"/>
-      <c r="AU145" t="inlineStr"/>
+      <c r="AT145" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU145" t="n">
+        <v>0</v>
+      </c>
       <c r="AV145" t="inlineStr"/>
       <c r="AW145" t="inlineStr"/>
       <c r="AX145" t="inlineStr"/>
@@ -35674,13 +36224,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1DC3F84B-675E-497E-9228-BDBA253687C6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79A15022-15DF-4C4F-B02D-F8C9F383AAE4}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56FE8BDF-1559-4E42-8D8C-FDFF2B559F6A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98B62046-A9C9-4931-9958-45DB0AC62BE6}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C106FD5E-F9B0-4363-A89A-2486B7B043A0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC7006F9-F14C-45C5-A5DC-E7A8D9514E93}"/>
 </file>
</xml_diff>

<commit_message>
Rounded the Quality score to 1 digit after period
</commit_message>
<xml_diff>
--- a/data/Ontologies_forRepo.xlsx
+++ b/data/Ontologies_forRepo.xlsx
@@ -1801,12 +1801,12 @@
       <c r="BM5" t="inlineStr"/>
       <c r="BN5" t="inlineStr">
         <is>
-          <t>n3244b1251ee04b699f21ebdd1500db17b1</t>
+          <t>n6a7d5322a38842bf86c5ad9d06b00ffcb1</t>
         </is>
       </c>
       <c r="BO5" t="inlineStr">
         <is>
-          <t>['n3244b1251ee04b699f21ebdd1500db17b1']</t>
+          <t>['n6a7d5322a38842bf86c5ad9d06b00ffcb1']</t>
         </is>
       </c>
       <c r="BP5" t="inlineStr"/>
@@ -2050,12 +2050,12 @@
       </c>
       <c r="BN6" t="inlineStr">
         <is>
-          <t>nae7ce59cd1c74adb908fa80b10955ab5b1</t>
+          <t>n279a682fe7b3414ca3dd05514f43cd8cb1</t>
         </is>
       </c>
       <c r="BO6" t="inlineStr">
         <is>
-          <t>['nae7ce59cd1c74adb908fa80b10955ab5b1']</t>
+          <t>['n279a682fe7b3414ca3dd05514f43cd8cb1']</t>
         </is>
       </c>
       <c r="BP6" t="inlineStr"/>
@@ -2099,7 +2099,7 @@
         <v>3</v>
       </c>
       <c r="CD6" t="n">
-        <v>1.239</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="7">
@@ -3256,12 +3256,12 @@
       <c r="BM11" t="inlineStr"/>
       <c r="BN11" t="inlineStr">
         <is>
-          <t>n34c3ada48c28465f83ed8415f038363bb1</t>
+          <t>n905b6ca76e544a09a9e3e6fd19847975b1</t>
         </is>
       </c>
       <c r="BO11" t="inlineStr">
         <is>
-          <t>['n34c3ada48c28465f83ed8415f038363bb1']</t>
+          <t>['n905b6ca76e544a09a9e3e6fd19847975b1']</t>
         </is>
       </c>
       <c r="BP11" t="inlineStr"/>
@@ -4398,7 +4398,7 @@
         <v>3</v>
       </c>
       <c r="CD16" t="n">
-        <v>1.986</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -4888,12 +4888,12 @@
       <c r="BM18" t="inlineStr"/>
       <c r="BN18" t="inlineStr">
         <is>
-          <t>n31739d9d92ad40e59072f273b243dbe2b8, n31739d9d92ad40e59072f273b243dbe2b9, n31739d9d92ad40e59072f273b243dbe2b10, n31739d9d92ad40e59072f273b243dbe2b11</t>
+          <t>n193fb70772a342b996e7bdd5369cf6c0b8, n193fb70772a342b996e7bdd5369cf6c0b9, n193fb70772a342b996e7bdd5369cf6c0b10, n193fb70772a342b996e7bdd5369cf6c0b11</t>
         </is>
       </c>
       <c r="BO18" t="inlineStr">
         <is>
-          <t>['n31739d9d92ad40e59072f273b243dbe2b8', 'n31739d9d92ad40e59072f273b243dbe2b9', 'n31739d9d92ad40e59072f273b243dbe2b10', 'n31739d9d92ad40e59072f273b243dbe2b11']</t>
+          <t>['n193fb70772a342b996e7bdd5369cf6c0b8', 'n193fb70772a342b996e7bdd5369cf6c0b9', 'n193fb70772a342b996e7bdd5369cf6c0b10', 'n193fb70772a342b996e7bdd5369cf6c0b11']</t>
         </is>
       </c>
       <c r="BP18" t="inlineStr"/>
@@ -5156,22 +5156,22 @@
       </c>
       <c r="BN19" t="inlineStr">
         <is>
-          <t>n44744923c071402ebde9a58be3d12dd6b7274</t>
+          <t>nfbc208f787ed40398a97a7cd1dd6f02bb7274</t>
         </is>
       </c>
       <c r="BO19" t="inlineStr">
         <is>
-          <t>['n44744923c071402ebde9a58be3d12dd6b7274']</t>
+          <t>['nfbc208f787ed40398a97a7cd1dd6f02bb7274']</t>
         </is>
       </c>
       <c r="BP19" t="inlineStr">
         <is>
-          <t>n44744923c071402ebde9a58be3d12dd6b7276</t>
+          <t>nfbc208f787ed40398a97a7cd1dd6f02bb7276</t>
         </is>
       </c>
       <c r="BQ19" t="inlineStr">
         <is>
-          <t>n44744923c071402ebde9a58be3d12dd6b7276</t>
+          <t>nfbc208f787ed40398a97a7cd1dd6f02bb7276</t>
         </is>
       </c>
       <c r="BR19" t="inlineStr">
@@ -5410,12 +5410,12 @@
       <c r="BM20" t="inlineStr"/>
       <c r="BN20" t="inlineStr">
         <is>
-          <t>n4a99d86e00f44609a5555bb477f0c721b1, n4a99d86e00f44609a5555bb477f0c721b2</t>
+          <t>n920037507b4849dd8240aa56169f3a7db1, n920037507b4849dd8240aa56169f3a7db2</t>
         </is>
       </c>
       <c r="BO20" t="inlineStr">
         <is>
-          <t>['n4a99d86e00f44609a5555bb477f0c721b1', 'n4a99d86e00f44609a5555bb477f0c721b2']</t>
+          <t>['n920037507b4849dd8240aa56169f3a7db1', 'n920037507b4849dd8240aa56169f3a7db2']</t>
         </is>
       </c>
       <c r="BP20" t="inlineStr"/>
@@ -5737,7 +5737,7 @@
         <v>3</v>
       </c>
       <c r="CD21" t="n">
-        <v>1.833</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="22">
@@ -6124,12 +6124,12 @@
       <c r="BM23" t="inlineStr"/>
       <c r="BN23" t="inlineStr">
         <is>
-          <t>n67c76c94e3a14b7098d050656db422d8b1</t>
+          <t>n0dbb84a1c7da462fba07c8020671c65ab1</t>
         </is>
       </c>
       <c r="BO23" t="inlineStr">
         <is>
-          <t>['n67c76c94e3a14b7098d050656db422d8b1']</t>
+          <t>['n0dbb84a1c7da462fba07c8020671c65ab1']</t>
         </is>
       </c>
       <c r="BP23" t="inlineStr"/>
@@ -6796,12 +6796,12 @@
       <c r="BM26" t="inlineStr"/>
       <c r="BN26" t="inlineStr">
         <is>
-          <t>nca51b53ad14c4384a9ecd0358baa5e8eb3, nca51b53ad14c4384a9ecd0358baa5e8eb4</t>
+          <t>n4af7659eea674dc4a0f2ea941a35496fb3, n4af7659eea674dc4a0f2ea941a35496fb4</t>
         </is>
       </c>
       <c r="BO26" t="inlineStr">
         <is>
-          <t>['nca51b53ad14c4384a9ecd0358baa5e8eb3', 'nca51b53ad14c4384a9ecd0358baa5e8eb4']</t>
+          <t>['n4af7659eea674dc4a0f2ea941a35496fb3', 'n4af7659eea674dc4a0f2ea941a35496fb4']</t>
         </is>
       </c>
       <c r="BP26" t="inlineStr"/>
@@ -7254,12 +7254,12 @@
       </c>
       <c r="BN28" t="inlineStr">
         <is>
-          <t>ne92fefd39a694cb3a94846113a8ffc30b1</t>
+          <t>n77b5815d578943daad838473c52485aeb1</t>
         </is>
       </c>
       <c r="BO28" t="inlineStr">
         <is>
-          <t>['ne92fefd39a694cb3a94846113a8ffc30b1']</t>
+          <t>['n77b5815d578943daad838473c52485aeb1']</t>
         </is>
       </c>
       <c r="BP28" t="inlineStr"/>
@@ -7303,7 +7303,7 @@
         <v>2</v>
       </c>
       <c r="CD28" t="n">
-        <v>1.389</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="29">
@@ -7538,12 +7538,12 @@
       <c r="BM29" t="inlineStr"/>
       <c r="BN29" t="inlineStr">
         <is>
-          <t>n3a56e66f2729490cbc26c23fa43dc5edb3, n3a56e66f2729490cbc26c23fa43dc5edb4</t>
+          <t>nb6e51031ae924e30b99e73fe1a1fdc40b3, nb6e51031ae924e30b99e73fe1a1fdc40b4</t>
         </is>
       </c>
       <c r="BO29" t="inlineStr">
         <is>
-          <t>['n3a56e66f2729490cbc26c23fa43dc5edb3', 'n3a56e66f2729490cbc26c23fa43dc5edb4']</t>
+          <t>['nb6e51031ae924e30b99e73fe1a1fdc40b3', 'nb6e51031ae924e30b99e73fe1a1fdc40b4']</t>
         </is>
       </c>
       <c r="BP29" t="inlineStr"/>
@@ -7822,12 +7822,12 @@
       <c r="BM30" t="inlineStr"/>
       <c r="BN30" t="inlineStr">
         <is>
-          <t>ne1dc41f433d441dc934dee8f4f0a064cb3, ne1dc41f433d441dc934dee8f4f0a064cb4</t>
+          <t>ne1aa0ce684f04059bdc38c9c82f71347b3, ne1aa0ce684f04059bdc38c9c82f71347b4</t>
         </is>
       </c>
       <c r="BO30" t="inlineStr">
         <is>
-          <t>['ne1dc41f433d441dc934dee8f4f0a064cb3', 'ne1dc41f433d441dc934dee8f4f0a064cb4']</t>
+          <t>['ne1aa0ce684f04059bdc38c9c82f71347b3', 'ne1aa0ce684f04059bdc38c9c82f71347b4']</t>
         </is>
       </c>
       <c r="BP30" t="inlineStr"/>
@@ -8099,12 +8099,12 @@
       <c r="BM31" t="inlineStr"/>
       <c r="BN31" t="inlineStr">
         <is>
-          <t>n44185ebbc4be42fd9f9a9a3b6c3a5c5eb1</t>
+          <t>n401ffcd421e74ebe91603b5493d9fcbeb1</t>
         </is>
       </c>
       <c r="BO31" t="inlineStr">
         <is>
-          <t>['n44185ebbc4be42fd9f9a9a3b6c3a5c5eb1']</t>
+          <t>['n401ffcd421e74ebe91603b5493d9fcbeb1']</t>
         </is>
       </c>
       <c r="BP31" t="inlineStr"/>
@@ -8148,7 +8148,7 @@
         <v>3</v>
       </c>
       <c r="CD31" t="n">
-        <v>1.81</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="32">
@@ -8368,22 +8368,22 @@
       <c r="BM32" t="inlineStr"/>
       <c r="BN32" t="inlineStr">
         <is>
-          <t>n02a4f2f658e84a55bfe7e389fc80fb4bb1</t>
+          <t>n9b6b7c172d524858a5d3724084fd915eb1</t>
         </is>
       </c>
       <c r="BO32" t="inlineStr">
         <is>
-          <t>['n02a4f2f658e84a55bfe7e389fc80fb4bb1']</t>
+          <t>['n9b6b7c172d524858a5d3724084fd915eb1']</t>
         </is>
       </c>
       <c r="BP32" t="inlineStr">
         <is>
-          <t>n02a4f2f658e84a55bfe7e389fc80fb4bb3</t>
+          <t>n9b6b7c172d524858a5d3724084fd915eb3</t>
         </is>
       </c>
       <c r="BQ32" t="inlineStr">
         <is>
-          <t>n02a4f2f658e84a55bfe7e389fc80fb4bb3</t>
+          <t>n9b6b7c172d524858a5d3724084fd915eb3</t>
         </is>
       </c>
       <c r="BR32" t="inlineStr">
@@ -8425,7 +8425,7 @@
         <v>3</v>
       </c>
       <c r="CD32" t="n">
-        <v>1.941</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="33">
@@ -8897,7 +8897,7 @@
         <v>3</v>
       </c>
       <c r="CD34" t="n">
-        <v>1.492</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="35">
@@ -9159,7 +9159,7 @@
         <v>3</v>
       </c>
       <c r="CD35" t="n">
-        <v>1.458</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="36">
@@ -9441,7 +9441,7 @@
         <v>3</v>
       </c>
       <c r="CD36" t="n">
-        <v>1.647</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="37">
@@ -9709,7 +9709,7 @@
         <v>3</v>
       </c>
       <c r="CD37" t="n">
-        <v>1.497</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="38">
@@ -9983,7 +9983,7 @@
         <v>3</v>
       </c>
       <c r="CD38" t="n">
-        <v>1.428</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="39">
@@ -10265,7 +10265,7 @@
         <v>3</v>
       </c>
       <c r="CD39" t="n">
-        <v>1.333</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="40">
@@ -10785,7 +10785,7 @@
         <v>3</v>
       </c>
       <c r="CD41" t="n">
-        <v>1.525</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="42">
@@ -11059,7 +11059,7 @@
         <v>3</v>
       </c>
       <c r="CD42" t="n">
-        <v>1.067</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="43">
@@ -11333,7 +11333,7 @@
         <v>3</v>
       </c>
       <c r="CD43" t="n">
-        <v>1.524</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="44">
@@ -12063,7 +12063,7 @@
         <v>3</v>
       </c>
       <c r="CD46" t="n">
-        <v>1.782</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="47">
@@ -12688,7 +12688,7 @@
         <v>3</v>
       </c>
       <c r="CD49" t="n">
-        <v>1.226</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="50">
@@ -12956,7 +12956,7 @@
         <v>3</v>
       </c>
       <c r="CD50" t="n">
-        <v>1.986</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51">
@@ -13191,12 +13191,12 @@
       </c>
       <c r="BN51" t="inlineStr">
         <is>
-          <t>n0f5122232f024f6f987d3ad335536392b1, https://www.researchgate.net/profile/Mathias_Bonduel</t>
+          <t>n49015c1b454e48838bcf2880c4be3fecb1, https://www.researchgate.net/profile/Mathias_Bonduel</t>
         </is>
       </c>
       <c r="BO51" t="inlineStr">
         <is>
-          <t>['n0f5122232f024f6f987d3ad335536392b1', 'https://www.researchgate.net/profile/Mathias_Bonduel']</t>
+          <t>['n49015c1b454e48838bcf2880c4be3fecb1', 'https://www.researchgate.net/profile/Mathias_Bonduel']</t>
         </is>
       </c>
       <c r="BP51" t="inlineStr"/>
@@ -15526,7 +15526,7 @@
         <v>3</v>
       </c>
       <c r="CD60" t="n">
-        <v>1.932</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="61">
@@ -16422,7 +16422,7 @@
         <v>3</v>
       </c>
       <c r="CD64" t="n">
-        <v>1.913</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="65">
@@ -16698,7 +16698,7 @@
         <v>3</v>
       </c>
       <c r="CD65" t="n">
-        <v>1.992</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66">
@@ -16968,7 +16968,7 @@
         <v>3</v>
       </c>
       <c r="CD66" t="n">
-        <v>1.886</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="67">
@@ -17553,12 +17553,12 @@
       </c>
       <c r="BP69" t="inlineStr">
         <is>
-          <t>nd6e9bf97cccd469d9294e6da77b119e5b1</t>
+          <t>ndfca450f4fdd4658814578c5166fee6bb1</t>
         </is>
       </c>
       <c r="BQ69" t="inlineStr">
         <is>
-          <t>nd6e9bf97cccd469d9294e6da77b119e5b1</t>
+          <t>ndfca450f4fdd4658814578c5166fee6bb1</t>
         </is>
       </c>
       <c r="BR69" t="inlineStr">
@@ -18561,22 +18561,22 @@
       <c r="BM73" t="inlineStr"/>
       <c r="BN73" t="inlineStr">
         <is>
-          <t>nc4d210c79b634f7a8f62a48a3e1bbf56b1</t>
+          <t>n026f0133ddbd47bfb7b225419485c1a9b1</t>
         </is>
       </c>
       <c r="BO73" t="inlineStr">
         <is>
-          <t>['nc4d210c79b634f7a8f62a48a3e1bbf56b1']</t>
+          <t>['n026f0133ddbd47bfb7b225419485c1a9b1']</t>
         </is>
       </c>
       <c r="BP73" t="inlineStr">
         <is>
-          <t>nc4d210c79b634f7a8f62a48a3e1bbf56b3</t>
+          <t>n026f0133ddbd47bfb7b225419485c1a9b3</t>
         </is>
       </c>
       <c r="BQ73" t="inlineStr">
         <is>
-          <t>nc4d210c79b634f7a8f62a48a3e1bbf56b3</t>
+          <t>n026f0133ddbd47bfb7b225419485c1a9b3</t>
         </is>
       </c>
       <c r="BR73" t="inlineStr">
@@ -18618,7 +18618,7 @@
         <v>3</v>
       </c>
       <c r="CD73" t="n">
-        <v>1.933</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="74">
@@ -19065,12 +19065,12 @@
       <c r="BM75" t="inlineStr"/>
       <c r="BN75" t="inlineStr">
         <is>
-          <t>n3d430423b1914c95b9a573defad90fbcb1, n3d430423b1914c95b9a573defad90fbcb2</t>
+          <t>nf17170b985cb4e3eb4472b6518650e83b1, nf17170b985cb4e3eb4472b6518650e83b2</t>
         </is>
       </c>
       <c r="BO75" t="inlineStr">
         <is>
-          <t>['n3d430423b1914c95b9a573defad90fbcb1', 'n3d430423b1914c95b9a573defad90fbcb2']</t>
+          <t>['nf17170b985cb4e3eb4472b6518650e83b1', 'nf17170b985cb4e3eb4472b6518650e83b2']</t>
         </is>
       </c>
       <c r="BP75" t="inlineStr"/>
@@ -19380,7 +19380,7 @@
         <v>3</v>
       </c>
       <c r="CD76" t="n">
-        <v>1.556</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="77">
@@ -19654,7 +19654,7 @@
         <v>3</v>
       </c>
       <c r="CD77" t="n">
-        <v>1.984</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78">
@@ -20134,22 +20134,22 @@
       <c r="BM79" t="inlineStr"/>
       <c r="BN79" t="inlineStr">
         <is>
-          <t>n1855b57938dd4b1e92b12a25be7ea42bb3, n1855b57938dd4b1e92b12a25be7ea42bb5</t>
+          <t>n5f0d79107b0245ffb9eb516eedb40e9eb3, n5f0d79107b0245ffb9eb516eedb40e9eb5</t>
         </is>
       </c>
       <c r="BO79" t="inlineStr">
         <is>
-          <t>['n1855b57938dd4b1e92b12a25be7ea42bb3', 'n1855b57938dd4b1e92b12a25be7ea42bb5']</t>
+          <t>['n5f0d79107b0245ffb9eb516eedb40e9eb3', 'n5f0d79107b0245ffb9eb516eedb40e9eb5']</t>
         </is>
       </c>
       <c r="BP79" t="inlineStr">
         <is>
-          <t>n1855b57938dd4b1e92b12a25be7ea42bb7</t>
+          <t>n5f0d79107b0245ffb9eb516eedb40e9eb7</t>
         </is>
       </c>
       <c r="BQ79" t="inlineStr">
         <is>
-          <t>n1855b57938dd4b1e92b12a25be7ea42bb7</t>
+          <t>n5f0d79107b0245ffb9eb516eedb40e9eb7</t>
         </is>
       </c>
       <c r="BR79" t="inlineStr">
@@ -20191,7 +20191,7 @@
         <v>3</v>
       </c>
       <c r="CD79" t="n">
-        <v>1.896</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="80">
@@ -20641,7 +20641,7 @@
         <v>3</v>
       </c>
       <c r="CD81" t="n">
-        <v>1.865</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="82">
@@ -21067,22 +21067,22 @@
       <c r="BM83" t="inlineStr"/>
       <c r="BN83" t="inlineStr">
         <is>
-          <t>ne269ecf3bfd34bc89e28c40f8506748cb3, ne269ecf3bfd34bc89e28c40f8506748cb5</t>
+          <t>n57a5a9640e114f0daea6cdab78ee6f06b3, n57a5a9640e114f0daea6cdab78ee6f06b5</t>
         </is>
       </c>
       <c r="BO83" t="inlineStr">
         <is>
-          <t>['ne269ecf3bfd34bc89e28c40f8506748cb3', 'ne269ecf3bfd34bc89e28c40f8506748cb5']</t>
+          <t>['n57a5a9640e114f0daea6cdab78ee6f06b3', 'n57a5a9640e114f0daea6cdab78ee6f06b5']</t>
         </is>
       </c>
       <c r="BP83" t="inlineStr">
         <is>
-          <t>ne269ecf3bfd34bc89e28c40f8506748cb7</t>
+          <t>n57a5a9640e114f0daea6cdab78ee6f06b7</t>
         </is>
       </c>
       <c r="BQ83" t="inlineStr">
         <is>
-          <t>ne269ecf3bfd34bc89e28c40f8506748cb7</t>
+          <t>n57a5a9640e114f0daea6cdab78ee6f06b7</t>
         </is>
       </c>
       <c r="BR83" t="inlineStr">
@@ -21124,7 +21124,7 @@
         <v>3</v>
       </c>
       <c r="CD83" t="n">
-        <v>1.815</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="84">
@@ -21404,7 +21404,7 @@
         <v>3</v>
       </c>
       <c r="CD84" t="n">
-        <v>1.179</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="85">
@@ -21656,7 +21656,7 @@
         <v>3</v>
       </c>
       <c r="CD85" t="n">
-        <v>1.933</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="86">
@@ -21865,12 +21865,12 @@
       </c>
       <c r="BN86" t="inlineStr">
         <is>
-          <t>na3f8de111d8a4b30abd84e3c819094bfb1</t>
+          <t>naf2dbc8f75b24a779a44109687c68e74b1</t>
         </is>
       </c>
       <c r="BO86" t="inlineStr">
         <is>
-          <t>['na3f8de111d8a4b30abd84e3c819094bfb1']</t>
+          <t>['naf2dbc8f75b24a779a44109687c68e74b1']</t>
         </is>
       </c>
       <c r="BP86" t="inlineStr"/>
@@ -21914,7 +21914,7 @@
         <v>3</v>
       </c>
       <c r="CD86" t="n">
-        <v>1.994</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87">
@@ -23032,7 +23032,7 @@
         <v>3</v>
       </c>
       <c r="CD91" t="n">
-        <v>1.257</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="92">
@@ -23537,7 +23537,7 @@
         <v>3</v>
       </c>
       <c r="CD93" t="n">
-        <v>1.833</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="94">
@@ -24373,7 +24373,7 @@
         <v>3</v>
       </c>
       <c r="CD97" t="n">
-        <v>1.963</v>
+        <v>2</v>
       </c>
     </row>
     <row r="98">
@@ -24578,12 +24578,12 @@
       <c r="BM98" t="inlineStr"/>
       <c r="BN98" t="inlineStr">
         <is>
-          <t>n7907b3fb6d6c4be287c978cb92b27cabb1, n7907b3fb6d6c4be287c978cb92b27cabb2</t>
+          <t>na26e13b1f1884f1cb061816f673a69b4b1, na26e13b1f1884f1cb061816f673a69b4b2</t>
         </is>
       </c>
       <c r="BO98" t="inlineStr">
         <is>
-          <t>['n7907b3fb6d6c4be287c978cb92b27cabb1', 'n7907b3fb6d6c4be287c978cb92b27cabb2']</t>
+          <t>['na26e13b1f1884f1cb061816f673a69b4b1', 'na26e13b1f1884f1cb061816f673a69b4b2']</t>
         </is>
       </c>
       <c r="BP98" t="inlineStr"/>
@@ -24627,7 +24627,7 @@
         <v>3</v>
       </c>
       <c r="CD98" t="n">
-        <v>1.947</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="99">
@@ -26065,7 +26065,7 @@
         <v>3</v>
       </c>
       <c r="CD104" t="n">
-        <v>1.462</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="105">
@@ -32923,12 +32923,12 @@
       <c r="BM130" t="inlineStr"/>
       <c r="BN130" t="inlineStr">
         <is>
-          <t>n8d24cdc3698f49e1a74cb3a7ad364d77b1</t>
+          <t>naf9f371e4cfb410d86f6001f5d7679bcb1</t>
         </is>
       </c>
       <c r="BO130" t="inlineStr">
         <is>
-          <t>['n8d24cdc3698f49e1a74cb3a7ad364d77b1']</t>
+          <t>['naf9f371e4cfb410d86f6001f5d7679bcb1']</t>
         </is>
       </c>
       <c r="BP130" t="inlineStr"/>
@@ -33193,12 +33193,12 @@
       <c r="BM131" t="inlineStr"/>
       <c r="BN131" t="inlineStr">
         <is>
-          <t>nf04f46bae1224b61be6d1b764f6ff66db1</t>
+          <t>na26a67ad03b449e5ba9f5d76cc4aa29ab1</t>
         </is>
       </c>
       <c r="BO131" t="inlineStr">
         <is>
-          <t>['nf04f46bae1224b61be6d1b764f6ff66db1']</t>
+          <t>['na26a67ad03b449e5ba9f5d76cc4aa29ab1']</t>
         </is>
       </c>
       <c r="BP131" t="inlineStr"/>
@@ -35228,7 +35228,7 @@
         <v>3</v>
       </c>
       <c r="CD141" t="n">
-        <v>1.014</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142">
@@ -36224,13 +36224,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79A15022-15DF-4C4F-B02D-F8C9F383AAE4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CA8D592-26A7-423E-AF08-9507D40F025D}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98B62046-A9C9-4931-9958-45DB0AC62BE6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{706057D7-4F23-4809-8234-2BB76B24A7BF}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC7006F9-F14C-45C5-A5DC-E7A8D9514E93}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8F566BE-512C-4487-B8CD-8154C7B2025D}"/>
 </file>
</xml_diff>

<commit_message>
FOOPs fix + Graph
- Fixed the presentation of the FOOPs scores
- Added the ontologyGraph.html from "main" to ease merging.
</commit_message>
<xml_diff>
--- a/data/Ontologies_forRepo.xlsx
+++ b/data/Ontologies_forRepo.xlsx
@@ -986,10 +986,10 @@
       <c r="AR2" t="inlineStr"/>
       <c r="AS2" t="inlineStr"/>
       <c r="AT2" t="n">
-        <v>0.6722222</v>
+        <v>0.67</v>
       </c>
       <c r="AU2" t="n">
-        <v>0.6722222</v>
+        <v>0.67</v>
       </c>
       <c r="AV2" t="inlineStr"/>
       <c r="AW2" t="inlineStr"/>
@@ -1228,10 +1228,10 @@
       <c r="AR3" t="inlineStr"/>
       <c r="AS3" t="inlineStr"/>
       <c r="AT3" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AU3" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AV3" t="inlineStr"/>
       <c r="AW3" t="inlineStr"/>
@@ -1486,10 +1486,10 @@
         <v>15</v>
       </c>
       <c r="AT4" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AU4" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AV4" t="inlineStr"/>
       <c r="AW4" t="inlineStr"/>
@@ -1756,10 +1756,10 @@
       <c r="AR5" t="inlineStr"/>
       <c r="AS5" t="inlineStr"/>
       <c r="AT5" t="n">
-        <v>0.6979166999999999</v>
+        <v>0.7</v>
       </c>
       <c r="AU5" t="n">
-        <v>0.6979166999999999</v>
+        <v>0.7</v>
       </c>
       <c r="AV5" t="inlineStr"/>
       <c r="AW5" t="inlineStr"/>
@@ -1801,12 +1801,12 @@
       <c r="BM5" t="inlineStr"/>
       <c r="BN5" t="inlineStr">
         <is>
-          <t>n6a7d5322a38842bf86c5ad9d06b00ffcb1</t>
+          <t>n15bc9c2e339a4b3ca7f4afa3c742c918b1</t>
         </is>
       </c>
       <c r="BO5" t="inlineStr">
         <is>
-          <t>['n6a7d5322a38842bf86c5ad9d06b00ffcb1']</t>
+          <t>['n15bc9c2e339a4b3ca7f4afa3c742c918b1']</t>
         </is>
       </c>
       <c r="BP5" t="inlineStr"/>
@@ -1997,10 +1997,10 @@
         <v>15</v>
       </c>
       <c r="AT6" t="n">
-        <v>0.65871125</v>
+        <v>0.66</v>
       </c>
       <c r="AU6" t="n">
-        <v>0.65871125</v>
+        <v>0.66</v>
       </c>
       <c r="AV6" t="inlineStr"/>
       <c r="AW6" t="inlineStr"/>
@@ -2050,12 +2050,12 @@
       </c>
       <c r="BN6" t="inlineStr">
         <is>
-          <t>n279a682fe7b3414ca3dd05514f43cd8cb1</t>
+          <t>n28b4a33a1a3c47afbc496e26c3cdbc21b1</t>
         </is>
       </c>
       <c r="BO6" t="inlineStr">
         <is>
-          <t>['n279a682fe7b3414ca3dd05514f43cd8cb1']</t>
+          <t>['n28b4a33a1a3c47afbc496e26c3cdbc21b1']</t>
         </is>
       </c>
       <c r="BP6" t="inlineStr"/>
@@ -2241,10 +2241,10 @@
       <c r="AR7" t="inlineStr"/>
       <c r="AS7" t="inlineStr"/>
       <c r="AT7" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AU7" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AV7" t="inlineStr"/>
       <c r="AW7" t="inlineStr"/>
@@ -3211,10 +3211,10 @@
       </c>
       <c r="AS11" t="inlineStr"/>
       <c r="AT11" t="n">
-        <v>0.6666666999999999</v>
+        <v>0.67</v>
       </c>
       <c r="AU11" t="n">
-        <v>0.6666666999999999</v>
+        <v>0.67</v>
       </c>
       <c r="AV11" t="inlineStr"/>
       <c r="AW11" t="inlineStr"/>
@@ -3256,12 +3256,12 @@
       <c r="BM11" t="inlineStr"/>
       <c r="BN11" t="inlineStr">
         <is>
-          <t>n905b6ca76e544a09a9e3e6fd19847975b1</t>
+          <t>n87b0615a1dd74723a3b1211284364afdb1</t>
         </is>
       </c>
       <c r="BO11" t="inlineStr">
         <is>
-          <t>['n905b6ca76e544a09a9e3e6fd19847975b1']</t>
+          <t>['n87b0615a1dd74723a3b1211284364afdb1']</t>
         </is>
       </c>
       <c r="BP11" t="inlineStr"/>
@@ -4035,10 +4035,10 @@
         <v>15</v>
       </c>
       <c r="AT15" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AU15" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AV15" t="inlineStr"/>
       <c r="AW15" t="inlineStr"/>
@@ -4296,10 +4296,10 @@
       <c r="AR16" t="inlineStr"/>
       <c r="AS16" t="inlineStr"/>
       <c r="AT16" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AU16" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AV16" t="inlineStr"/>
       <c r="AW16" t="inlineStr"/>
@@ -4577,10 +4577,10 @@
       </c>
       <c r="AS17" t="inlineStr"/>
       <c r="AT17" t="n">
-        <v>0.8611111</v>
+        <v>0.86</v>
       </c>
       <c r="AU17" t="n">
-        <v>0.8611111</v>
+        <v>0.86</v>
       </c>
       <c r="AV17" t="inlineStr">
         <is>
@@ -4843,10 +4843,10 @@
       </c>
       <c r="AS18" t="inlineStr"/>
       <c r="AT18" t="n">
-        <v>0.6597222700000001</v>
+        <v>0.66</v>
       </c>
       <c r="AU18" t="n">
-        <v>0.6597222700000001</v>
+        <v>0.66</v>
       </c>
       <c r="AV18" t="inlineStr"/>
       <c r="AW18" t="inlineStr"/>
@@ -4888,12 +4888,12 @@
       <c r="BM18" t="inlineStr"/>
       <c r="BN18" t="inlineStr">
         <is>
-          <t>n193fb70772a342b996e7bdd5369cf6c0b8, n193fb70772a342b996e7bdd5369cf6c0b9, n193fb70772a342b996e7bdd5369cf6c0b10, n193fb70772a342b996e7bdd5369cf6c0b11</t>
+          <t>nb2f1c618ad41435cbfd118dd348a826bb8, nb2f1c618ad41435cbfd118dd348a826bb9, nb2f1c618ad41435cbfd118dd348a826bb10, nb2f1c618ad41435cbfd118dd348a826bb11</t>
         </is>
       </c>
       <c r="BO18" t="inlineStr">
         <is>
-          <t>['n193fb70772a342b996e7bdd5369cf6c0b8', 'n193fb70772a342b996e7bdd5369cf6c0b9', 'n193fb70772a342b996e7bdd5369cf6c0b10', 'n193fb70772a342b996e7bdd5369cf6c0b11']</t>
+          <t>['nb2f1c618ad41435cbfd118dd348a826bb8', 'nb2f1c618ad41435cbfd118dd348a826bb9', 'nb2f1c618ad41435cbfd118dd348a826bb10', 'nb2f1c618ad41435cbfd118dd348a826bb11']</t>
         </is>
       </c>
       <c r="BP18" t="inlineStr"/>
@@ -5156,22 +5156,22 @@
       </c>
       <c r="BN19" t="inlineStr">
         <is>
-          <t>nfbc208f787ed40398a97a7cd1dd6f02bb7274</t>
+          <t>nc689fbfbb68c48a4bb850489dc06615db7274</t>
         </is>
       </c>
       <c r="BO19" t="inlineStr">
         <is>
-          <t>['nfbc208f787ed40398a97a7cd1dd6f02bb7274']</t>
+          <t>['nc689fbfbb68c48a4bb850489dc06615db7274']</t>
         </is>
       </c>
       <c r="BP19" t="inlineStr">
         <is>
-          <t>nfbc208f787ed40398a97a7cd1dd6f02bb7276</t>
+          <t>nc689fbfbb68c48a4bb850489dc06615db7276</t>
         </is>
       </c>
       <c r="BQ19" t="inlineStr">
         <is>
-          <t>nfbc208f787ed40398a97a7cd1dd6f02bb7276</t>
+          <t>nc689fbfbb68c48a4bb850489dc06615db7276</t>
         </is>
       </c>
       <c r="BR19" t="inlineStr">
@@ -5365,10 +5365,10 @@
       <c r="AR20" t="inlineStr"/>
       <c r="AS20" t="inlineStr"/>
       <c r="AT20" t="n">
-        <v>0.7395833000000001</v>
+        <v>0.74</v>
       </c>
       <c r="AU20" t="n">
-        <v>0.7395833000000001</v>
+        <v>0.74</v>
       </c>
       <c r="AV20" t="inlineStr"/>
       <c r="AW20" t="inlineStr"/>
@@ -5410,12 +5410,12 @@
       <c r="BM20" t="inlineStr"/>
       <c r="BN20" t="inlineStr">
         <is>
-          <t>n920037507b4849dd8240aa56169f3a7db1, n920037507b4849dd8240aa56169f3a7db2</t>
+          <t>nd5a555793efd425088f30c9880618a8cb1, nd5a555793efd425088f30c9880618a8cb2</t>
         </is>
       </c>
       <c r="BO20" t="inlineStr">
         <is>
-          <t>['n920037507b4849dd8240aa56169f3a7db1', 'n920037507b4849dd8240aa56169f3a7db2']</t>
+          <t>['nd5a555793efd425088f30c9880618a8cb1', 'nd5a555793efd425088f30c9880618a8cb2']</t>
         </is>
       </c>
       <c r="BP20" t="inlineStr"/>
@@ -5627,10 +5627,10 @@
         <v>15</v>
       </c>
       <c r="AT21" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AU21" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AV21" t="inlineStr"/>
       <c r="AW21" t="inlineStr"/>
@@ -6087,10 +6087,10 @@
       <c r="AR23" t="inlineStr"/>
       <c r="AS23" t="inlineStr"/>
       <c r="AT23" t="n">
-        <v>0.8125</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="AU23" t="n">
-        <v>0.8125</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="AV23" t="inlineStr"/>
       <c r="AW23" t="inlineStr"/>
@@ -6124,12 +6124,12 @@
       <c r="BM23" t="inlineStr"/>
       <c r="BN23" t="inlineStr">
         <is>
-          <t>n0dbb84a1c7da462fba07c8020671c65ab1</t>
+          <t>nc2db33f02b224b7f9d088f8361346b1cb1</t>
         </is>
       </c>
       <c r="BO23" t="inlineStr">
         <is>
-          <t>['n0dbb84a1c7da462fba07c8020671c65ab1']</t>
+          <t>['nc2db33f02b224b7f9d088f8361346b1cb1']</t>
         </is>
       </c>
       <c r="BP23" t="inlineStr"/>
@@ -6743,10 +6743,10 @@
       </c>
       <c r="AS26" t="inlineStr"/>
       <c r="AT26" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AU26" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AV26" t="inlineStr"/>
       <c r="AW26" t="inlineStr"/>
@@ -6796,12 +6796,12 @@
       <c r="BM26" t="inlineStr"/>
       <c r="BN26" t="inlineStr">
         <is>
-          <t>n4af7659eea674dc4a0f2ea941a35496fb3, n4af7659eea674dc4a0f2ea941a35496fb4</t>
+          <t>nccc3d14c88044a58812e3f139ad2d1aab3, nccc3d14c88044a58812e3f139ad2d1aab4</t>
         </is>
       </c>
       <c r="BO26" t="inlineStr">
         <is>
-          <t>['n4af7659eea674dc4a0f2ea941a35496fb3', 'n4af7659eea674dc4a0f2ea941a35496fb4']</t>
+          <t>['nccc3d14c88044a58812e3f139ad2d1aab3', 'nccc3d14c88044a58812e3f139ad2d1aab4']</t>
         </is>
       </c>
       <c r="BP26" t="inlineStr"/>
@@ -7201,10 +7201,10 @@
       <c r="AR28" t="inlineStr"/>
       <c r="AS28" t="inlineStr"/>
       <c r="AT28" t="n">
-        <v>0.7973485</v>
+        <v>0.8</v>
       </c>
       <c r="AU28" t="n">
-        <v>0.7973485</v>
+        <v>0.8</v>
       </c>
       <c r="AV28" t="inlineStr"/>
       <c r="AW28" t="inlineStr"/>
@@ -7254,12 +7254,12 @@
       </c>
       <c r="BN28" t="inlineStr">
         <is>
-          <t>n77b5815d578943daad838473c52485aeb1</t>
+          <t>n79619e692a814d5e933caf3da7bcd356b1</t>
         </is>
       </c>
       <c r="BO28" t="inlineStr">
         <is>
-          <t>['n77b5815d578943daad838473c52485aeb1']</t>
+          <t>['n79619e692a814d5e933caf3da7bcd356b1']</t>
         </is>
       </c>
       <c r="BP28" t="inlineStr"/>
@@ -7485,10 +7485,10 @@
       </c>
       <c r="AS29" t="inlineStr"/>
       <c r="AT29" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AU29" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AV29" t="inlineStr"/>
       <c r="AW29" t="inlineStr"/>
@@ -7538,12 +7538,12 @@
       <c r="BM29" t="inlineStr"/>
       <c r="BN29" t="inlineStr">
         <is>
-          <t>nb6e51031ae924e30b99e73fe1a1fdc40b3, nb6e51031ae924e30b99e73fe1a1fdc40b4</t>
+          <t>nc94a92cd905f440fbc2cdaeeb2cf0484b3, nc94a92cd905f440fbc2cdaeeb2cf0484b4</t>
         </is>
       </c>
       <c r="BO29" t="inlineStr">
         <is>
-          <t>['nb6e51031ae924e30b99e73fe1a1fdc40b3', 'nb6e51031ae924e30b99e73fe1a1fdc40b4']</t>
+          <t>['nc94a92cd905f440fbc2cdaeeb2cf0484b3', 'nc94a92cd905f440fbc2cdaeeb2cf0484b4']</t>
         </is>
       </c>
       <c r="BP29" t="inlineStr"/>
@@ -7769,10 +7769,10 @@
       </c>
       <c r="AS30" t="inlineStr"/>
       <c r="AT30" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AU30" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AV30" t="inlineStr"/>
       <c r="AW30" t="inlineStr"/>
@@ -7822,12 +7822,12 @@
       <c r="BM30" t="inlineStr"/>
       <c r="BN30" t="inlineStr">
         <is>
-          <t>ne1aa0ce684f04059bdc38c9c82f71347b3, ne1aa0ce684f04059bdc38c9c82f71347b4</t>
+          <t>nc16b2a79767847d8866a556bc24c1d01b3, nc16b2a79767847d8866a556bc24c1d01b4</t>
         </is>
       </c>
       <c r="BO30" t="inlineStr">
         <is>
-          <t>['ne1aa0ce684f04059bdc38c9c82f71347b3', 'ne1aa0ce684f04059bdc38c9c82f71347b4']</t>
+          <t>['nc16b2a79767847d8866a556bc24c1d01b3', 'nc16b2a79767847d8866a556bc24c1d01b4']</t>
         </is>
       </c>
       <c r="BP30" t="inlineStr"/>
@@ -8046,10 +8046,10 @@
       </c>
       <c r="AS31" t="inlineStr"/>
       <c r="AT31" t="n">
-        <v>0.8125</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="AU31" t="n">
-        <v>0.8125</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="AV31" t="inlineStr"/>
       <c r="AW31" t="inlineStr"/>
@@ -8099,12 +8099,12 @@
       <c r="BM31" t="inlineStr"/>
       <c r="BN31" t="inlineStr">
         <is>
-          <t>n401ffcd421e74ebe91603b5493d9fcbeb1</t>
+          <t>ndb4e37ff2156491cb7d019ac2fa42cc3b1</t>
         </is>
       </c>
       <c r="BO31" t="inlineStr">
         <is>
-          <t>['n401ffcd421e74ebe91603b5493d9fcbeb1']</t>
+          <t>['ndb4e37ff2156491cb7d019ac2fa42cc3b1']</t>
         </is>
       </c>
       <c r="BP31" t="inlineStr"/>
@@ -8323,10 +8323,10 @@
       <c r="AR32" t="inlineStr"/>
       <c r="AS32" t="inlineStr"/>
       <c r="AT32" t="n">
-        <v>0.7892157400000001</v>
+        <v>0.79</v>
       </c>
       <c r="AU32" t="n">
-        <v>0.7892157400000001</v>
+        <v>0.79</v>
       </c>
       <c r="AV32" t="inlineStr"/>
       <c r="AW32" t="inlineStr"/>
@@ -8368,22 +8368,22 @@
       <c r="BM32" t="inlineStr"/>
       <c r="BN32" t="inlineStr">
         <is>
-          <t>n9b6b7c172d524858a5d3724084fd915eb1</t>
+          <t>n989d0ef5426148a1aa32c442a6c82e99b1</t>
         </is>
       </c>
       <c r="BO32" t="inlineStr">
         <is>
-          <t>['n9b6b7c172d524858a5d3724084fd915eb1']</t>
+          <t>['n989d0ef5426148a1aa32c442a6c82e99b1']</t>
         </is>
       </c>
       <c r="BP32" t="inlineStr">
         <is>
-          <t>n9b6b7c172d524858a5d3724084fd915eb3</t>
+          <t>n989d0ef5426148a1aa32c442a6c82e99b3</t>
         </is>
       </c>
       <c r="BQ32" t="inlineStr">
         <is>
-          <t>n9b6b7c172d524858a5d3724084fd915eb3</t>
+          <t>n989d0ef5426148a1aa32c442a6c82e99b3</t>
         </is>
       </c>
       <c r="BR32" t="inlineStr">
@@ -9599,10 +9599,10 @@
       <c r="AR37" t="inlineStr"/>
       <c r="AS37" t="inlineStr"/>
       <c r="AT37" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AU37" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AV37" t="inlineStr"/>
       <c r="AW37" t="inlineStr"/>
@@ -9881,10 +9881,10 @@
       </c>
       <c r="AS38" t="inlineStr"/>
       <c r="AT38" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AU38" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AV38" t="inlineStr"/>
       <c r="AW38" t="inlineStr"/>
@@ -10155,10 +10155,10 @@
       </c>
       <c r="AS39" t="inlineStr"/>
       <c r="AT39" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AU39" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AV39" t="inlineStr">
         <is>
@@ -10407,10 +10407,10 @@
       <c r="AR40" t="inlineStr"/>
       <c r="AS40" t="inlineStr"/>
       <c r="AT40" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AU40" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AV40" t="inlineStr"/>
       <c r="AW40" t="inlineStr"/>
@@ -10683,10 +10683,10 @@
       </c>
       <c r="AS41" t="inlineStr"/>
       <c r="AT41" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AU41" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AV41" t="inlineStr"/>
       <c r="AW41" t="inlineStr"/>
@@ -10949,10 +10949,10 @@
       <c r="AR42" t="inlineStr"/>
       <c r="AS42" t="inlineStr"/>
       <c r="AT42" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AU42" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AV42" t="inlineStr"/>
       <c r="AW42" t="inlineStr"/>
@@ -11231,10 +11231,10 @@
       </c>
       <c r="AS43" t="inlineStr"/>
       <c r="AT43" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AU43" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AV43" t="inlineStr"/>
       <c r="AW43" t="inlineStr"/>
@@ -11467,10 +11467,10 @@
       <c r="AR44" t="inlineStr"/>
       <c r="AS44" t="inlineStr"/>
       <c r="AT44" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AU44" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AV44" t="inlineStr"/>
       <c r="AW44" t="inlineStr"/>
@@ -11707,10 +11707,10 @@
       </c>
       <c r="AS45" t="inlineStr"/>
       <c r="AT45" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AU45" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AV45" t="inlineStr"/>
       <c r="AW45" t="inlineStr"/>
@@ -11961,10 +11961,10 @@
       </c>
       <c r="AS46" t="inlineStr"/>
       <c r="AT46" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AU46" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AV46" t="inlineStr"/>
       <c r="AW46" t="inlineStr"/>
@@ -12594,10 +12594,10 @@
       <c r="AR49" t="inlineStr"/>
       <c r="AS49" t="inlineStr"/>
       <c r="AT49" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AU49" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AV49" t="inlineStr"/>
       <c r="AW49" t="inlineStr"/>
@@ -12854,10 +12854,10 @@
       <c r="AR50" t="inlineStr"/>
       <c r="AS50" t="inlineStr"/>
       <c r="AT50" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AU50" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AV50" t="inlineStr">
         <is>
@@ -13138,10 +13138,10 @@
       </c>
       <c r="AS51" t="inlineStr"/>
       <c r="AT51" t="n">
-        <v>0.8611111</v>
+        <v>0.86</v>
       </c>
       <c r="AU51" t="n">
-        <v>0.8611111</v>
+        <v>0.86</v>
       </c>
       <c r="AV51" t="inlineStr"/>
       <c r="AW51" t="inlineStr"/>
@@ -13191,12 +13191,12 @@
       </c>
       <c r="BN51" t="inlineStr">
         <is>
-          <t>n49015c1b454e48838bcf2880c4be3fecb1, https://www.researchgate.net/profile/Mathias_Bonduel</t>
+          <t>n9f5dcdd845534f4b987d4cba50f885bfb1, https://www.researchgate.net/profile/Mathias_Bonduel</t>
         </is>
       </c>
       <c r="BO51" t="inlineStr">
         <is>
-          <t>['n49015c1b454e48838bcf2880c4be3fecb1', 'https://www.researchgate.net/profile/Mathias_Bonduel']</t>
+          <t>['n9f5dcdd845534f4b987d4cba50f885bfb1', 'https://www.researchgate.net/profile/Mathias_Bonduel']</t>
         </is>
       </c>
       <c r="BP51" t="inlineStr"/>
@@ -13400,10 +13400,10 @@
       <c r="AR52" t="inlineStr"/>
       <c r="AS52" t="inlineStr"/>
       <c r="AT52" t="n">
-        <v>0.72222215</v>
+        <v>0.72</v>
       </c>
       <c r="AU52" t="n">
-        <v>0.72222215</v>
+        <v>0.72</v>
       </c>
       <c r="AV52" t="inlineStr"/>
       <c r="AW52" t="inlineStr"/>
@@ -13662,10 +13662,10 @@
       </c>
       <c r="AS53" t="inlineStr"/>
       <c r="AT53" t="n">
-        <v>0.1875</v>
+        <v>0.19</v>
       </c>
       <c r="AU53" t="n">
-        <v>0.1875</v>
+        <v>0.19</v>
       </c>
       <c r="AV53" t="inlineStr"/>
       <c r="AW53" t="inlineStr"/>
@@ -13916,10 +13916,10 @@
       <c r="AR54" t="inlineStr"/>
       <c r="AS54" t="inlineStr"/>
       <c r="AT54" t="n">
-        <v>0.6388889</v>
+        <v>0.64</v>
       </c>
       <c r="AU54" t="n">
-        <v>0.6388889</v>
+        <v>0.64</v>
       </c>
       <c r="AV54" t="inlineStr"/>
       <c r="AW54" t="inlineStr"/>
@@ -14168,10 +14168,10 @@
       <c r="AR55" t="inlineStr"/>
       <c r="AS55" t="inlineStr"/>
       <c r="AT55" t="n">
-        <v>0.68402785</v>
+        <v>0.68</v>
       </c>
       <c r="AU55" t="n">
-        <v>0.68402785</v>
+        <v>0.68</v>
       </c>
       <c r="AV55" t="inlineStr"/>
       <c r="AW55" t="inlineStr"/>
@@ -14699,10 +14699,10 @@
       <c r="AR57" t="inlineStr"/>
       <c r="AS57" t="inlineStr"/>
       <c r="AT57" t="n">
-        <v>0.6770833000000001</v>
+        <v>0.68</v>
       </c>
       <c r="AU57" t="n">
-        <v>0.6770833000000001</v>
+        <v>0.68</v>
       </c>
       <c r="AV57" t="inlineStr"/>
       <c r="AW57" t="inlineStr"/>
@@ -15173,10 +15173,10 @@
       </c>
       <c r="AS59" t="inlineStr"/>
       <c r="AT59" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AU59" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AV59" t="inlineStr"/>
       <c r="AW59" t="inlineStr"/>
@@ -15428,10 +15428,10 @@
       <c r="AR60" t="inlineStr"/>
       <c r="AS60" t="inlineStr"/>
       <c r="AT60" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AU60" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AV60" t="inlineStr"/>
       <c r="AW60" t="inlineStr"/>
@@ -15868,10 +15868,10 @@
       <c r="AR62" t="inlineStr"/>
       <c r="AS62" t="inlineStr"/>
       <c r="AT62" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AU62" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AV62" t="inlineStr"/>
       <c r="AW62" t="inlineStr"/>
@@ -16320,10 +16320,10 @@
       <c r="AR64" t="inlineStr"/>
       <c r="AS64" t="inlineStr"/>
       <c r="AT64" t="n">
-        <v>0.3784722</v>
+        <v>0.38</v>
       </c>
       <c r="AU64" t="n">
-        <v>0.3784722</v>
+        <v>0.38</v>
       </c>
       <c r="AV64" t="inlineStr"/>
       <c r="AW64" t="inlineStr"/>
@@ -16604,10 +16604,10 @@
       </c>
       <c r="AS65" t="inlineStr"/>
       <c r="AT65" t="n">
-        <v>0.81218195</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="AU65" t="n">
-        <v>0.81218195</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="AV65" t="inlineStr"/>
       <c r="AW65" t="inlineStr"/>
@@ -16866,10 +16866,10 @@
       <c r="AR66" t="inlineStr"/>
       <c r="AS66" t="inlineStr"/>
       <c r="AT66" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AU66" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AV66" t="inlineStr"/>
       <c r="AW66" t="inlineStr"/>
@@ -17490,10 +17490,10 @@
       </c>
       <c r="AS69" t="inlineStr"/>
       <c r="AT69" t="n">
-        <v>0.8993056</v>
+        <v>0.9</v>
       </c>
       <c r="AU69" t="n">
-        <v>0.8993056</v>
+        <v>0.9</v>
       </c>
       <c r="AV69" t="inlineStr">
         <is>
@@ -17553,12 +17553,12 @@
       </c>
       <c r="BP69" t="inlineStr">
         <is>
-          <t>ndfca450f4fdd4658814578c5166fee6bb1</t>
+          <t>nf21d15b0c1d74ea2be6f2121e229069db1</t>
         </is>
       </c>
       <c r="BQ69" t="inlineStr">
         <is>
-          <t>ndfca450f4fdd4658814578c5166fee6bb1</t>
+          <t>nf21d15b0c1d74ea2be6f2121e229069db1</t>
         </is>
       </c>
       <c r="BR69" t="inlineStr">
@@ -17976,10 +17976,10 @@
       </c>
       <c r="AS71" t="inlineStr"/>
       <c r="AT71" t="n">
-        <v>0.7361111</v>
+        <v>0.74</v>
       </c>
       <c r="AU71" t="n">
-        <v>0.7361111</v>
+        <v>0.74</v>
       </c>
       <c r="AV71" t="inlineStr"/>
       <c r="AW71" t="inlineStr"/>
@@ -18240,10 +18240,10 @@
         <v>0</v>
       </c>
       <c r="AT72" t="n">
-        <v>0.0625</v>
+        <v>0.06</v>
       </c>
       <c r="AU72" t="n">
-        <v>0.0625</v>
+        <v>0.06</v>
       </c>
       <c r="AV72" t="inlineStr">
         <is>
@@ -18508,10 +18508,10 @@
       <c r="AR73" t="inlineStr"/>
       <c r="AS73" t="inlineStr"/>
       <c r="AT73" t="n">
-        <v>0.0625</v>
+        <v>0.06</v>
       </c>
       <c r="AU73" t="n">
-        <v>0.0625</v>
+        <v>0.06</v>
       </c>
       <c r="AV73" t="inlineStr">
         <is>
@@ -18561,22 +18561,22 @@
       <c r="BM73" t="inlineStr"/>
       <c r="BN73" t="inlineStr">
         <is>
-          <t>n026f0133ddbd47bfb7b225419485c1a9b1</t>
+          <t>n5fd7d7a83c45457ea66451a105083985b1</t>
         </is>
       </c>
       <c r="BO73" t="inlineStr">
         <is>
-          <t>['n026f0133ddbd47bfb7b225419485c1a9b1']</t>
+          <t>['n5fd7d7a83c45457ea66451a105083985b1']</t>
         </is>
       </c>
       <c r="BP73" t="inlineStr">
         <is>
-          <t>n026f0133ddbd47bfb7b225419485c1a9b3</t>
+          <t>n5fd7d7a83c45457ea66451a105083985b3</t>
         </is>
       </c>
       <c r="BQ73" t="inlineStr">
         <is>
-          <t>n026f0133ddbd47bfb7b225419485c1a9b3</t>
+          <t>n5fd7d7a83c45457ea66451a105083985b3</t>
         </is>
       </c>
       <c r="BR73" t="inlineStr">
@@ -18764,10 +18764,10 @@
       </c>
       <c r="AS74" t="inlineStr"/>
       <c r="AT74" t="n">
-        <v>0.56815</v>
+        <v>0.57</v>
       </c>
       <c r="AU74" t="n">
-        <v>0.56815</v>
+        <v>0.57</v>
       </c>
       <c r="AV74" t="inlineStr"/>
       <c r="AW74" t="inlineStr"/>
@@ -19020,10 +19020,10 @@
       <c r="AR75" t="inlineStr"/>
       <c r="AS75" t="inlineStr"/>
       <c r="AT75" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AU75" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AV75" t="inlineStr"/>
       <c r="AW75" t="inlineStr"/>
@@ -19065,12 +19065,12 @@
       <c r="BM75" t="inlineStr"/>
       <c r="BN75" t="inlineStr">
         <is>
-          <t>nf17170b985cb4e3eb4472b6518650e83b1, nf17170b985cb4e3eb4472b6518650e83b2</t>
+          <t>n8012851f050e4f3eb5c9827a0dc99bd6b1, n8012851f050e4f3eb5c9827a0dc99bd6b2</t>
         </is>
       </c>
       <c r="BO75" t="inlineStr">
         <is>
-          <t>['nf17170b985cb4e3eb4472b6518650e83b1', 'nf17170b985cb4e3eb4472b6518650e83b2']</t>
+          <t>['n8012851f050e4f3eb5c9827a0dc99bd6b1', 'n8012851f050e4f3eb5c9827a0dc99bd6b2']</t>
         </is>
       </c>
       <c r="BP75" t="inlineStr"/>
@@ -19270,10 +19270,10 @@
         <v>15</v>
       </c>
       <c r="AT76" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AU76" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AV76" t="inlineStr"/>
       <c r="AW76" t="inlineStr"/>
@@ -19552,10 +19552,10 @@
       </c>
       <c r="AS77" t="inlineStr"/>
       <c r="AT77" t="n">
-        <v>0.72023803</v>
+        <v>0.72</v>
       </c>
       <c r="AU77" t="n">
-        <v>0.72023803</v>
+        <v>0.72</v>
       </c>
       <c r="AV77" t="inlineStr"/>
       <c r="AW77" t="inlineStr"/>
@@ -19824,10 +19824,10 @@
       </c>
       <c r="AS78" t="inlineStr"/>
       <c r="AT78" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AU78" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AV78" t="inlineStr"/>
       <c r="AW78" t="inlineStr"/>
@@ -20097,10 +20097,10 @@
       <c r="AR79" t="inlineStr"/>
       <c r="AS79" t="inlineStr"/>
       <c r="AT79" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AU79" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AV79" t="inlineStr"/>
       <c r="AW79" t="inlineStr"/>
@@ -20134,22 +20134,22 @@
       <c r="BM79" t="inlineStr"/>
       <c r="BN79" t="inlineStr">
         <is>
-          <t>n5f0d79107b0245ffb9eb516eedb40e9eb3, n5f0d79107b0245ffb9eb516eedb40e9eb5</t>
+          <t>n17e582eed7f74fd68f9a257592435f12b3, n17e582eed7f74fd68f9a257592435f12b5</t>
         </is>
       </c>
       <c r="BO79" t="inlineStr">
         <is>
-          <t>['n5f0d79107b0245ffb9eb516eedb40e9eb3', 'n5f0d79107b0245ffb9eb516eedb40e9eb5']</t>
+          <t>['n17e582eed7f74fd68f9a257592435f12b3', 'n17e582eed7f74fd68f9a257592435f12b5']</t>
         </is>
       </c>
       <c r="BP79" t="inlineStr">
         <is>
-          <t>n5f0d79107b0245ffb9eb516eedb40e9eb7</t>
+          <t>n17e582eed7f74fd68f9a257592435f12b7</t>
         </is>
       </c>
       <c r="BQ79" t="inlineStr">
         <is>
-          <t>n5f0d79107b0245ffb9eb516eedb40e9eb7</t>
+          <t>n17e582eed7f74fd68f9a257592435f12b7</t>
         </is>
       </c>
       <c r="BR79" t="inlineStr">
@@ -20295,10 +20295,10 @@
       <c r="AR80" t="inlineStr"/>
       <c r="AS80" t="inlineStr"/>
       <c r="AT80" t="n">
-        <v>0.041666668</v>
+        <v>0.04</v>
       </c>
       <c r="AU80" t="n">
-        <v>0.041666668</v>
+        <v>0.04</v>
       </c>
       <c r="AV80" t="inlineStr"/>
       <c r="AW80" t="inlineStr"/>
@@ -20539,10 +20539,10 @@
       </c>
       <c r="AS81" t="inlineStr"/>
       <c r="AT81" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AU81" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AV81" t="inlineStr"/>
       <c r="AW81" t="inlineStr"/>
@@ -21014,10 +21014,10 @@
       <c r="AR83" t="inlineStr"/>
       <c r="AS83" t="inlineStr"/>
       <c r="AT83" t="n">
-        <v>0.87082696</v>
+        <v>0.87</v>
       </c>
       <c r="AU83" t="n">
-        <v>0.87082696</v>
+        <v>0.87</v>
       </c>
       <c r="AV83" t="inlineStr">
         <is>
@@ -21067,22 +21067,22 @@
       <c r="BM83" t="inlineStr"/>
       <c r="BN83" t="inlineStr">
         <is>
-          <t>n57a5a9640e114f0daea6cdab78ee6f06b3, n57a5a9640e114f0daea6cdab78ee6f06b5</t>
+          <t>n4f44a599c41e46038cdd6a513c8cfb9cb3, n4f44a599c41e46038cdd6a513c8cfb9cb5</t>
         </is>
       </c>
       <c r="BO83" t="inlineStr">
         <is>
-          <t>['n57a5a9640e114f0daea6cdab78ee6f06b3', 'n57a5a9640e114f0daea6cdab78ee6f06b5']</t>
+          <t>['n4f44a599c41e46038cdd6a513c8cfb9cb3', 'n4f44a599c41e46038cdd6a513c8cfb9cb5']</t>
         </is>
       </c>
       <c r="BP83" t="inlineStr">
         <is>
-          <t>n57a5a9640e114f0daea6cdab78ee6f06b7</t>
+          <t>n4f44a599c41e46038cdd6a513c8cfb9cb7</t>
         </is>
       </c>
       <c r="BQ83" t="inlineStr">
         <is>
-          <t>n57a5a9640e114f0daea6cdab78ee6f06b7</t>
+          <t>n4f44a599c41e46038cdd6a513c8cfb9cb7</t>
         </is>
       </c>
       <c r="BR83" t="inlineStr">
@@ -21294,10 +21294,10 @@
       </c>
       <c r="AS84" t="inlineStr"/>
       <c r="AT84" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AU84" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AV84" t="inlineStr"/>
       <c r="AW84" t="inlineStr"/>
@@ -21562,10 +21562,10 @@
       <c r="AR85" t="inlineStr"/>
       <c r="AS85" t="inlineStr"/>
       <c r="AT85" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AU85" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AV85" t="inlineStr"/>
       <c r="AW85" t="inlineStr"/>
@@ -21820,10 +21820,10 @@
       <c r="AR86" t="inlineStr"/>
       <c r="AS86" t="inlineStr"/>
       <c r="AT86" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AU86" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AV86" t="inlineStr"/>
       <c r="AW86" t="inlineStr"/>
@@ -21865,12 +21865,12 @@
       </c>
       <c r="BN86" t="inlineStr">
         <is>
-          <t>naf2dbc8f75b24a779a44109687c68e74b1</t>
+          <t>nc9db8e5cf4f74d15bc6a2a2730a05b57b1</t>
         </is>
       </c>
       <c r="BO86" t="inlineStr">
         <is>
-          <t>['naf2dbc8f75b24a779a44109687c68e74b1']</t>
+          <t>['nc9db8e5cf4f74d15bc6a2a2730a05b57b1']</t>
         </is>
       </c>
       <c r="BP86" t="inlineStr"/>
@@ -22238,10 +22238,10 @@
       <c r="AR88" t="inlineStr"/>
       <c r="AS88" t="inlineStr"/>
       <c r="AT88" t="n">
-        <v>0.20833333</v>
+        <v>0.21</v>
       </c>
       <c r="AU88" t="n">
-        <v>0.20833333</v>
+        <v>0.21</v>
       </c>
       <c r="AV88" t="inlineStr">
         <is>
@@ -22468,10 +22468,10 @@
       </c>
       <c r="AS89" t="inlineStr"/>
       <c r="AT89" t="n">
-        <v>0.20833333</v>
+        <v>0.21</v>
       </c>
       <c r="AU89" t="n">
-        <v>0.20833333</v>
+        <v>0.21</v>
       </c>
       <c r="AV89" t="inlineStr">
         <is>
@@ -22682,10 +22682,10 @@
       <c r="AR90" t="inlineStr"/>
       <c r="AS90" t="inlineStr"/>
       <c r="AT90" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AU90" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AV90" t="inlineStr"/>
       <c r="AW90" t="inlineStr"/>
@@ -22938,10 +22938,10 @@
       </c>
       <c r="AS91" t="inlineStr"/>
       <c r="AT91" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AU91" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AV91" t="inlineStr"/>
       <c r="AW91" t="inlineStr"/>
@@ -23180,10 +23180,10 @@
       <c r="AR92" t="inlineStr"/>
       <c r="AS92" t="inlineStr"/>
       <c r="AT92" t="n">
-        <v>0.6527777299999999</v>
+        <v>0.65</v>
       </c>
       <c r="AU92" t="n">
-        <v>0.6527777299999999</v>
+        <v>0.65</v>
       </c>
       <c r="AV92" t="inlineStr"/>
       <c r="AW92" t="inlineStr"/>
@@ -23443,10 +23443,10 @@
       </c>
       <c r="AS93" t="inlineStr"/>
       <c r="AT93" t="n">
-        <v>0.7708333000000001</v>
+        <v>0.77</v>
       </c>
       <c r="AU93" t="n">
-        <v>0.7708333000000001</v>
+        <v>0.77</v>
       </c>
       <c r="AV93" t="inlineStr"/>
       <c r="AW93" t="inlineStr"/>
@@ -24263,10 +24263,10 @@
       <c r="AR97" t="inlineStr"/>
       <c r="AS97" t="inlineStr"/>
       <c r="AT97" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AU97" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AV97" t="inlineStr"/>
       <c r="AW97" t="inlineStr"/>
@@ -24533,10 +24533,10 @@
       <c r="AR98" t="inlineStr"/>
       <c r="AS98" t="inlineStr"/>
       <c r="AT98" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AU98" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AV98" t="inlineStr"/>
       <c r="AW98" t="inlineStr"/>
@@ -24578,12 +24578,12 @@
       <c r="BM98" t="inlineStr"/>
       <c r="BN98" t="inlineStr">
         <is>
-          <t>na26e13b1f1884f1cb061816f673a69b4b1, na26e13b1f1884f1cb061816f673a69b4b2</t>
+          <t>ne4084765d65c46d0b2f3dbddfe1e749bb1, ne4084765d65c46d0b2f3dbddfe1e749bb2</t>
         </is>
       </c>
       <c r="BO98" t="inlineStr">
         <is>
-          <t>['na26e13b1f1884f1cb061816f673a69b4b1', 'na26e13b1f1884f1cb061816f673a69b4b2']</t>
+          <t>['ne4084765d65c46d0b2f3dbddfe1e749bb1', 'ne4084765d65c46d0b2f3dbddfe1e749bb2']</t>
         </is>
       </c>
       <c r="BP98" t="inlineStr"/>
@@ -24789,10 +24789,10 @@
       <c r="AR99" t="inlineStr"/>
       <c r="AS99" t="inlineStr"/>
       <c r="AT99" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AU99" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AV99" t="inlineStr"/>
       <c r="AW99" t="inlineStr"/>
@@ -25053,10 +25053,10 @@
       <c r="AR100" t="inlineStr"/>
       <c r="AS100" t="inlineStr"/>
       <c r="AT100" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AU100" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AV100" t="inlineStr"/>
       <c r="AW100" t="inlineStr"/>
@@ -25513,10 +25513,10 @@
       <c r="AR102" t="inlineStr"/>
       <c r="AS102" t="inlineStr"/>
       <c r="AT102" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AU102" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AV102" t="inlineStr"/>
       <c r="AW102" t="inlineStr"/>
@@ -25955,10 +25955,10 @@
       <c r="AR104" t="inlineStr"/>
       <c r="AS104" t="inlineStr"/>
       <c r="AT104" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AU104" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AV104" t="inlineStr"/>
       <c r="AW104" t="inlineStr"/>
@@ -26235,10 +26235,10 @@
       </c>
       <c r="AS105" t="inlineStr"/>
       <c r="AT105" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AU105" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AV105" t="inlineStr"/>
       <c r="AW105" t="inlineStr"/>
@@ -26517,10 +26517,10 @@
       <c r="AR106" t="inlineStr"/>
       <c r="AS106" t="inlineStr"/>
       <c r="AT106" t="n">
-        <v>0.9270833000000001</v>
+        <v>0.93</v>
       </c>
       <c r="AU106" t="n">
-        <v>0.9270833000000001</v>
+        <v>0.93</v>
       </c>
       <c r="AV106" t="inlineStr"/>
       <c r="AW106" t="inlineStr"/>
@@ -26803,10 +26803,10 @@
       <c r="AR107" t="inlineStr"/>
       <c r="AS107" t="inlineStr"/>
       <c r="AT107" t="n">
-        <v>0.7708333000000001</v>
+        <v>0.77</v>
       </c>
       <c r="AU107" t="n">
-        <v>0.7708333000000001</v>
+        <v>0.77</v>
       </c>
       <c r="AV107" t="inlineStr"/>
       <c r="AW107" t="inlineStr"/>
@@ -27105,10 +27105,10 @@
       </c>
       <c r="AS108" t="inlineStr"/>
       <c r="AT108" t="n">
-        <v>0.8541666999999999</v>
+        <v>0.85</v>
       </c>
       <c r="AU108" t="n">
-        <v>0.8541666999999999</v>
+        <v>0.85</v>
       </c>
       <c r="AV108" t="inlineStr">
         <is>
@@ -27415,10 +27415,10 @@
       </c>
       <c r="AS109" t="inlineStr"/>
       <c r="AT109" t="n">
-        <v>0.8958333000000001</v>
+        <v>0.9</v>
       </c>
       <c r="AU109" t="n">
-        <v>0.8958333000000001</v>
+        <v>0.9</v>
       </c>
       <c r="AV109" t="inlineStr"/>
       <c r="AW109" t="inlineStr"/>
@@ -27719,10 +27719,10 @@
       <c r="AR110" t="inlineStr"/>
       <c r="AS110" t="inlineStr"/>
       <c r="AT110" t="n">
-        <v>0.8958333000000001</v>
+        <v>0.9</v>
       </c>
       <c r="AU110" t="n">
-        <v>0.8958333000000001</v>
+        <v>0.9</v>
       </c>
       <c r="AV110" t="inlineStr"/>
       <c r="AW110" t="inlineStr"/>
@@ -28020,10 +28020,10 @@
       <c r="AR111" t="inlineStr"/>
       <c r="AS111" t="inlineStr"/>
       <c r="AT111" t="n">
-        <v>0.8958333000000001</v>
+        <v>0.9</v>
       </c>
       <c r="AU111" t="n">
-        <v>0.8958333000000001</v>
+        <v>0.9</v>
       </c>
       <c r="AV111" t="inlineStr"/>
       <c r="AW111" t="inlineStr"/>
@@ -28314,10 +28314,10 @@
       <c r="AR112" t="inlineStr"/>
       <c r="AS112" t="inlineStr"/>
       <c r="AT112" t="n">
-        <v>0.8958333000000001</v>
+        <v>0.9</v>
       </c>
       <c r="AU112" t="n">
-        <v>0.8958333000000001</v>
+        <v>0.9</v>
       </c>
       <c r="AV112" t="inlineStr"/>
       <c r="AW112" t="inlineStr"/>
@@ -28608,10 +28608,10 @@
       <c r="AR113" t="inlineStr"/>
       <c r="AS113" t="inlineStr"/>
       <c r="AT113" t="n">
-        <v>0.7708333000000001</v>
+        <v>0.77</v>
       </c>
       <c r="AU113" t="n">
-        <v>0.7708333000000001</v>
+        <v>0.77</v>
       </c>
       <c r="AV113" t="inlineStr"/>
       <c r="AW113" t="inlineStr"/>
@@ -28906,10 +28906,10 @@
       <c r="AR114" t="inlineStr"/>
       <c r="AS114" t="inlineStr"/>
       <c r="AT114" t="n">
-        <v>0.9270833000000001</v>
+        <v>0.93</v>
       </c>
       <c r="AU114" t="n">
-        <v>0.9270833000000001</v>
+        <v>0.93</v>
       </c>
       <c r="AV114" t="inlineStr"/>
       <c r="AW114" t="inlineStr"/>
@@ -29200,10 +29200,10 @@
       <c r="AR115" t="inlineStr"/>
       <c r="AS115" t="inlineStr"/>
       <c r="AT115" t="n">
-        <v>0.7708333000000001</v>
+        <v>0.77</v>
       </c>
       <c r="AU115" t="n">
-        <v>0.7708333000000001</v>
+        <v>0.77</v>
       </c>
       <c r="AV115" t="inlineStr"/>
       <c r="AW115" t="inlineStr"/>
@@ -29508,10 +29508,10 @@
       </c>
       <c r="AS116" t="inlineStr"/>
       <c r="AT116" t="n">
-        <v>0.8541666999999999</v>
+        <v>0.85</v>
       </c>
       <c r="AU116" t="n">
-        <v>0.8541666999999999</v>
+        <v>0.85</v>
       </c>
       <c r="AV116" t="inlineStr"/>
       <c r="AW116" t="inlineStr"/>
@@ -29794,10 +29794,10 @@
       <c r="AR117" t="inlineStr"/>
       <c r="AS117" t="inlineStr"/>
       <c r="AT117" t="n">
-        <v>0.8958333000000001</v>
+        <v>0.9</v>
       </c>
       <c r="AU117" t="n">
-        <v>0.8958333000000001</v>
+        <v>0.9</v>
       </c>
       <c r="AV117" t="inlineStr"/>
       <c r="AW117" t="inlineStr"/>
@@ -30100,10 +30100,10 @@
       </c>
       <c r="AS118" t="inlineStr"/>
       <c r="AT118" t="n">
-        <v>0.9270833000000001</v>
+        <v>0.93</v>
       </c>
       <c r="AU118" t="n">
-        <v>0.9270833000000001</v>
+        <v>0.93</v>
       </c>
       <c r="AV118" t="inlineStr"/>
       <c r="AW118" t="inlineStr"/>
@@ -30372,10 +30372,10 @@
       <c r="AR119" t="inlineStr"/>
       <c r="AS119" t="inlineStr"/>
       <c r="AT119" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AU119" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AV119" t="inlineStr"/>
       <c r="AW119" t="inlineStr"/>
@@ -30596,10 +30596,10 @@
       <c r="AR120" t="inlineStr"/>
       <c r="AS120" t="inlineStr"/>
       <c r="AT120" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AU120" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AV120" t="inlineStr"/>
       <c r="AW120" t="inlineStr"/>
@@ -30854,10 +30854,10 @@
       </c>
       <c r="AS121" t="inlineStr"/>
       <c r="AT121" t="n">
-        <v>0.8958333000000001</v>
+        <v>0.9</v>
       </c>
       <c r="AU121" t="n">
-        <v>0.8958333000000001</v>
+        <v>0.9</v>
       </c>
       <c r="AV121" t="inlineStr"/>
       <c r="AW121" t="inlineStr"/>
@@ -31140,10 +31140,10 @@
       <c r="AR122" t="inlineStr"/>
       <c r="AS122" t="inlineStr"/>
       <c r="AT122" t="n">
-        <v>0.76388884</v>
+        <v>0.76</v>
       </c>
       <c r="AU122" t="n">
-        <v>0.76388884</v>
+        <v>0.76</v>
       </c>
       <c r="AV122" t="inlineStr"/>
       <c r="AW122" t="inlineStr"/>
@@ -31764,10 +31764,10 @@
       <c r="AR125" t="inlineStr"/>
       <c r="AS125" t="inlineStr"/>
       <c r="AT125" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AU125" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AV125" t="inlineStr"/>
       <c r="AW125" t="inlineStr"/>
@@ -32022,10 +32022,10 @@
       <c r="AR126" t="inlineStr"/>
       <c r="AS126" t="inlineStr"/>
       <c r="AT126" t="n">
-        <v>0.041666668</v>
+        <v>0.04</v>
       </c>
       <c r="AU126" t="n">
-        <v>0.041666668</v>
+        <v>0.04</v>
       </c>
       <c r="AV126" t="inlineStr"/>
       <c r="AW126" t="inlineStr"/>
@@ -32422,10 +32422,10 @@
       <c r="AR128" t="inlineStr"/>
       <c r="AS128" t="inlineStr"/>
       <c r="AT128" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AU128" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AV128" t="inlineStr">
         <is>
@@ -32636,10 +32636,10 @@
       <c r="AR129" t="inlineStr"/>
       <c r="AS129" t="inlineStr"/>
       <c r="AT129" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AU129" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AV129" t="inlineStr">
         <is>
@@ -32878,10 +32878,10 @@
       </c>
       <c r="AS130" t="inlineStr"/>
       <c r="AT130" t="n">
-        <v>0.8055556</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="AU130" t="n">
-        <v>0.8055556</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="AV130" t="inlineStr"/>
       <c r="AW130" t="inlineStr"/>
@@ -32923,12 +32923,12 @@
       <c r="BM130" t="inlineStr"/>
       <c r="BN130" t="inlineStr">
         <is>
-          <t>naf9f371e4cfb410d86f6001f5d7679bcb1</t>
+          <t>ne934ef65e9a04967be7a00061d311175b1</t>
         </is>
       </c>
       <c r="BO130" t="inlineStr">
         <is>
-          <t>['naf9f371e4cfb410d86f6001f5d7679bcb1']</t>
+          <t>['ne934ef65e9a04967be7a00061d311175b1']</t>
         </is>
       </c>
       <c r="BP130" t="inlineStr"/>
@@ -33148,10 +33148,10 @@
       </c>
       <c r="AS131" t="inlineStr"/>
       <c r="AT131" t="n">
-        <v>0.8159722700000001</v>
+        <v>0.82</v>
       </c>
       <c r="AU131" t="n">
-        <v>0.8159722700000001</v>
+        <v>0.82</v>
       </c>
       <c r="AV131" t="inlineStr"/>
       <c r="AW131" t="inlineStr"/>
@@ -33193,12 +33193,12 @@
       <c r="BM131" t="inlineStr"/>
       <c r="BN131" t="inlineStr">
         <is>
-          <t>na26a67ad03b449e5ba9f5d76cc4aa29ab1</t>
+          <t>n0dd39a8a3e6b4f8498432d75a3bf4671b1</t>
         </is>
       </c>
       <c r="BO131" t="inlineStr">
         <is>
-          <t>['na26a67ad03b449e5ba9f5d76cc4aa29ab1']</t>
+          <t>['n0dd39a8a3e6b4f8498432d75a3bf4671b1']</t>
         </is>
       </c>
       <c r="BP131" t="inlineStr"/>
@@ -33383,10 +33383,10 @@
       <c r="AR132" t="inlineStr"/>
       <c r="AS132" t="inlineStr"/>
       <c r="AT132" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AU132" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AV132" t="inlineStr"/>
       <c r="AW132" t="inlineStr"/>
@@ -33613,10 +33613,10 @@
       </c>
       <c r="AS133" t="inlineStr"/>
       <c r="AT133" t="n">
-        <v>0.8273566</v>
+        <v>0.83</v>
       </c>
       <c r="AU133" t="n">
-        <v>0.8273566</v>
+        <v>0.83</v>
       </c>
       <c r="AV133" t="inlineStr">
         <is>
@@ -35134,10 +35134,10 @@
       <c r="AR141" t="inlineStr"/>
       <c r="AS141" t="inlineStr"/>
       <c r="AT141" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AU141" t="n">
-        <v>0.14583333</v>
+        <v>0.15</v>
       </c>
       <c r="AV141" t="inlineStr"/>
       <c r="AW141" t="inlineStr"/>
@@ -35530,10 +35530,10 @@
       <c r="AR143" t="inlineStr"/>
       <c r="AS143" t="inlineStr"/>
       <c r="AT143" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AU143" t="n">
-        <v>0.104166664</v>
+        <v>0.1</v>
       </c>
       <c r="AV143" t="inlineStr"/>
       <c r="AW143" t="inlineStr"/>
@@ -36224,13 +36224,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CA8D592-26A7-423E-AF08-9507D40F025D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC0D7783-3091-4DD8-9EAA-97FE4E5E148A}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{706057D7-4F23-4809-8234-2BB76B24A7BF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FD687FE-FDC9-406F-90D2-C888CCCF4DDD}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8F566BE-512C-4487-B8CD-8154C7B2025D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30552C15-C933-4D4B-BBB0-77A2566C923E}"/>
 </file>
</xml_diff>

<commit_message>
New ontologies -> update of Ontologies_forRepo
</commit_message>
<xml_diff>
--- a/data/Ontologies_forRepo.xlsx
+++ b/data/Ontologies_forRepo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CD144"/>
+  <dimension ref="A1:CD145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -986,10 +986,10 @@
       <c r="AR2" t="inlineStr"/>
       <c r="AS2" t="inlineStr"/>
       <c r="AT2" t="n">
-        <v>0.04</v>
+        <v>0.63</v>
       </c>
       <c r="AU2" t="n">
-        <v>0.04</v>
+        <v>0.63</v>
       </c>
       <c r="AV2" t="inlineStr"/>
       <c r="AW2" t="inlineStr"/>
@@ -1228,10 +1228,10 @@
       <c r="AR3" t="inlineStr"/>
       <c r="AS3" t="inlineStr"/>
       <c r="AT3" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AU3" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AV3" t="inlineStr"/>
       <c r="AW3" t="inlineStr"/>
@@ -1756,10 +1756,10 @@
       <c r="AR5" t="inlineStr"/>
       <c r="AS5" t="inlineStr"/>
       <c r="AT5" t="n">
-        <v>0.04</v>
+        <v>0.7</v>
       </c>
       <c r="AU5" t="n">
-        <v>0.04</v>
+        <v>0.7</v>
       </c>
       <c r="AV5" t="inlineStr"/>
       <c r="AW5" t="inlineStr"/>
@@ -1801,12 +1801,12 @@
       <c r="BM5" t="inlineStr"/>
       <c r="BN5" t="inlineStr">
         <is>
-          <t>n81c1fb85bc794fb1a2bd2c0f0fd42b3ab1</t>
+          <t>naa3575725204497f99bf31ac508efb34b1</t>
         </is>
       </c>
       <c r="BO5" t="inlineStr">
         <is>
-          <t>['n81c1fb85bc794fb1a2bd2c0f0fd42b3ab1']</t>
+          <t>['naa3575725204497f99bf31ac508efb34b1']</t>
         </is>
       </c>
       <c r="BP5" t="inlineStr"/>
@@ -1997,10 +1997,10 @@
         <v>15</v>
       </c>
       <c r="AT6" t="n">
-        <v>0.04</v>
+        <v>0.66</v>
       </c>
       <c r="AU6" t="n">
-        <v>0.04</v>
+        <v>0.66</v>
       </c>
       <c r="AV6" t="inlineStr"/>
       <c r="AW6" t="inlineStr"/>
@@ -2050,12 +2050,12 @@
       </c>
       <c r="BN6" t="inlineStr">
         <is>
-          <t>n0d091193132244879d0a82a9e28ec796b1</t>
+          <t>nc75ef802e5dc4d48a7e3f58125b37752b1</t>
         </is>
       </c>
       <c r="BO6" t="inlineStr">
         <is>
-          <t>['n0d091193132244879d0a82a9e28ec796b1']</t>
+          <t>['nc75ef802e5dc4d48a7e3f58125b37752b1']</t>
         </is>
       </c>
       <c r="BP6" t="inlineStr"/>
@@ -3201,20 +3201,20 @@
       </c>
       <c r="AQ11" t="inlineStr">
         <is>
-          <t>contax, dtc, facility, fmo, hbpo, hmo</t>
+          <t>contax, dtc, facility, fmo, hbpo, hmo, rdo</t>
         </is>
       </c>
       <c r="AR11" t="inlineStr">
         <is>
-          <t>contax, dtc, facility, fmo, hbpo, hmo</t>
+          <t>contax, dtc, facility, fmo, hbpo, hmo, rdo</t>
         </is>
       </c>
       <c r="AS11" t="inlineStr"/>
       <c r="AT11" t="n">
-        <v>0.65</v>
+        <v>0.67</v>
       </c>
       <c r="AU11" t="n">
-        <v>0.65</v>
+        <v>0.67</v>
       </c>
       <c r="AV11" t="inlineStr"/>
       <c r="AW11" t="inlineStr"/>
@@ -3256,12 +3256,12 @@
       <c r="BM11" t="inlineStr"/>
       <c r="BN11" t="inlineStr">
         <is>
-          <t>nd0bd47af5e7c4466aacedcb3fb04f854b1</t>
+          <t>n72429165a43b4919a763188dc2ed3925b1</t>
         </is>
       </c>
       <c r="BO11" t="inlineStr">
         <is>
-          <t>['nd0bd47af5e7c4466aacedcb3fb04f854b1']</t>
+          <t>['n72429165a43b4919a763188dc2ed3925b1']</t>
         </is>
       </c>
       <c r="BP11" t="inlineStr"/>
@@ -4296,10 +4296,10 @@
       <c r="AR16" t="inlineStr"/>
       <c r="AS16" t="inlineStr"/>
       <c r="AT16" t="n">
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="AU16" t="n">
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="AV16" t="inlineStr"/>
       <c r="AW16" t="inlineStr"/>
@@ -4577,10 +4577,10 @@
       </c>
       <c r="AS17" t="inlineStr"/>
       <c r="AT17" t="n">
-        <v>0.04</v>
+        <v>0.86</v>
       </c>
       <c r="AU17" t="n">
-        <v>0.04</v>
+        <v>0.86</v>
       </c>
       <c r="AV17" t="inlineStr">
         <is>
@@ -4843,10 +4843,10 @@
       </c>
       <c r="AS18" t="inlineStr"/>
       <c r="AT18" t="n">
-        <v>0.04</v>
+        <v>0.66</v>
       </c>
       <c r="AU18" t="n">
-        <v>0.04</v>
+        <v>0.66</v>
       </c>
       <c r="AV18" t="inlineStr"/>
       <c r="AW18" t="inlineStr"/>
@@ -4888,12 +4888,12 @@
       <c r="BM18" t="inlineStr"/>
       <c r="BN18" t="inlineStr">
         <is>
-          <t>n5a4e53b53f974c4bb4c0fbf11b251b96b8, n5a4e53b53f974c4bb4c0fbf11b251b96b9, n5a4e53b53f974c4bb4c0fbf11b251b96b10, n5a4e53b53f974c4bb4c0fbf11b251b96b11</t>
+          <t>n9a427eb68b884f0fb6ae2e96f19f4451b8, n9a427eb68b884f0fb6ae2e96f19f4451b9, n9a427eb68b884f0fb6ae2e96f19f4451b10, n9a427eb68b884f0fb6ae2e96f19f4451b11</t>
         </is>
       </c>
       <c r="BO18" t="inlineStr">
         <is>
-          <t>['n5a4e53b53f974c4bb4c0fbf11b251b96b8', 'n5a4e53b53f974c4bb4c0fbf11b251b96b9', 'n5a4e53b53f974c4bb4c0fbf11b251b96b10', 'n5a4e53b53f974c4bb4c0fbf11b251b96b11']</t>
+          <t>['n9a427eb68b884f0fb6ae2e96f19f4451b8', 'n9a427eb68b884f0fb6ae2e96f19f4451b9', 'n9a427eb68b884f0fb6ae2e96f19f4451b10', 'n9a427eb68b884f0fb6ae2e96f19f4451b11']</t>
         </is>
       </c>
       <c r="BP18" t="inlineStr"/>
@@ -5156,22 +5156,22 @@
       </c>
       <c r="BN19" t="inlineStr">
         <is>
-          <t>n91951ac3f34d45c9b5eadd848ddacedbb7274</t>
+          <t>nc840e02d5877443989198ba7db658004b7274</t>
         </is>
       </c>
       <c r="BO19" t="inlineStr">
         <is>
-          <t>['n91951ac3f34d45c9b5eadd848ddacedbb7274']</t>
+          <t>['nc840e02d5877443989198ba7db658004b7274']</t>
         </is>
       </c>
       <c r="BP19" t="inlineStr">
         <is>
-          <t>n91951ac3f34d45c9b5eadd848ddacedbb7276</t>
+          <t>nc840e02d5877443989198ba7db658004b7276</t>
         </is>
       </c>
       <c r="BQ19" t="inlineStr">
         <is>
-          <t>n91951ac3f34d45c9b5eadd848ddacedbb7276</t>
+          <t>nc840e02d5877443989198ba7db658004b7276</t>
         </is>
       </c>
       <c r="BR19" t="inlineStr">
@@ -5365,10 +5365,10 @@
       <c r="AR20" t="inlineStr"/>
       <c r="AS20" t="inlineStr"/>
       <c r="AT20" t="n">
-        <v>0.04</v>
+        <v>0.74</v>
       </c>
       <c r="AU20" t="n">
-        <v>0.04</v>
+        <v>0.74</v>
       </c>
       <c r="AV20" t="inlineStr"/>
       <c r="AW20" t="inlineStr"/>
@@ -5410,12 +5410,12 @@
       <c r="BM20" t="inlineStr"/>
       <c r="BN20" t="inlineStr">
         <is>
-          <t>n00ff620de57b4c20a8658601fa3b9103b1, n00ff620de57b4c20a8658601fa3b9103b2</t>
+          <t>ncb6ecf054fee4fda92cd8730bc630390b1, ncb6ecf054fee4fda92cd8730bc630390b2</t>
         </is>
       </c>
       <c r="BO20" t="inlineStr">
         <is>
-          <t>['n00ff620de57b4c20a8658601fa3b9103b1', 'n00ff620de57b4c20a8658601fa3b9103b2']</t>
+          <t>['ncb6ecf054fee4fda92cd8730bc630390b1', 'ncb6ecf054fee4fda92cd8730bc630390b2']</t>
         </is>
       </c>
       <c r="BP20" t="inlineStr"/>
@@ -6087,10 +6087,10 @@
       <c r="AR23" t="inlineStr"/>
       <c r="AS23" t="inlineStr"/>
       <c r="AT23" t="n">
-        <v>0.04</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="AU23" t="n">
-        <v>0.04</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="AV23" t="inlineStr"/>
       <c r="AW23" t="inlineStr"/>
@@ -6124,12 +6124,12 @@
       <c r="BM23" t="inlineStr"/>
       <c r="BN23" t="inlineStr">
         <is>
-          <t>n3876f6cd37854dba89851dcd5f6d2aacb1</t>
+          <t>nb1d5f29cffec4b75a6362a242835b597b1</t>
         </is>
       </c>
       <c r="BO23" t="inlineStr">
         <is>
-          <t>['n3876f6cd37854dba89851dcd5f6d2aacb1']</t>
+          <t>['nb1d5f29cffec4b75a6362a242835b597b1']</t>
         </is>
       </c>
       <c r="BP23" t="inlineStr"/>
@@ -6743,10 +6743,10 @@
       </c>
       <c r="AS26" t="inlineStr"/>
       <c r="AT26" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AU26" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AV26" t="inlineStr"/>
       <c r="AW26" t="inlineStr"/>
@@ -6796,12 +6796,12 @@
       <c r="BM26" t="inlineStr"/>
       <c r="BN26" t="inlineStr">
         <is>
-          <t>nf19c1b72e8444096900979fbdafd1447b3, nf19c1b72e8444096900979fbdafd1447b4</t>
+          <t>nee403343d03e4a29bea709f4679251f1b3, nee403343d03e4a29bea709f4679251f1b4</t>
         </is>
       </c>
       <c r="BO26" t="inlineStr">
         <is>
-          <t>['nf19c1b72e8444096900979fbdafd1447b3', 'nf19c1b72e8444096900979fbdafd1447b4']</t>
+          <t>['nee403343d03e4a29bea709f4679251f1b3', 'nee403343d03e4a29bea709f4679251f1b4']</t>
         </is>
       </c>
       <c r="BP26" t="inlineStr"/>
@@ -7201,10 +7201,10 @@
       <c r="AR28" t="inlineStr"/>
       <c r="AS28" t="inlineStr"/>
       <c r="AT28" t="n">
-        <v>0.04</v>
+        <v>0.8</v>
       </c>
       <c r="AU28" t="n">
-        <v>0.04</v>
+        <v>0.8</v>
       </c>
       <c r="AV28" t="inlineStr"/>
       <c r="AW28" t="inlineStr"/>
@@ -7254,12 +7254,12 @@
       </c>
       <c r="BN28" t="inlineStr">
         <is>
-          <t>ne82515fa19334711a69efe259980677fb1</t>
+          <t>n40d87f2956d3464faca8e7210457fe85b1</t>
         </is>
       </c>
       <c r="BO28" t="inlineStr">
         <is>
-          <t>['ne82515fa19334711a69efe259980677fb1']</t>
+          <t>['n40d87f2956d3464faca8e7210457fe85b1']</t>
         </is>
       </c>
       <c r="BP28" t="inlineStr"/>
@@ -7485,10 +7485,10 @@
       </c>
       <c r="AS29" t="inlineStr"/>
       <c r="AT29" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AU29" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AV29" t="inlineStr"/>
       <c r="AW29" t="inlineStr"/>
@@ -7538,12 +7538,12 @@
       <c r="BM29" t="inlineStr"/>
       <c r="BN29" t="inlineStr">
         <is>
-          <t>n946f289d9fa64409b6f907d0589c1b37b3, n946f289d9fa64409b6f907d0589c1b37b4</t>
+          <t>nee37fd230dc9476da5f27343bbb846ceb3, nee37fd230dc9476da5f27343bbb846ceb4</t>
         </is>
       </c>
       <c r="BO29" t="inlineStr">
         <is>
-          <t>['n946f289d9fa64409b6f907d0589c1b37b3', 'n946f289d9fa64409b6f907d0589c1b37b4']</t>
+          <t>['nee37fd230dc9476da5f27343bbb846ceb3', 'nee37fd230dc9476da5f27343bbb846ceb4']</t>
         </is>
       </c>
       <c r="BP29" t="inlineStr"/>
@@ -7769,10 +7769,10 @@
       </c>
       <c r="AS30" t="inlineStr"/>
       <c r="AT30" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AU30" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AV30" t="inlineStr"/>
       <c r="AW30" t="inlineStr"/>
@@ -7822,12 +7822,12 @@
       <c r="BM30" t="inlineStr"/>
       <c r="BN30" t="inlineStr">
         <is>
-          <t>n0b978a5aaebe40c78eefc8ec2788558ab3, n0b978a5aaebe40c78eefc8ec2788558ab4</t>
+          <t>n528b0a2ec09f4001bf201ca376d90b6fb3, n528b0a2ec09f4001bf201ca376d90b6fb4</t>
         </is>
       </c>
       <c r="BO30" t="inlineStr">
         <is>
-          <t>['n0b978a5aaebe40c78eefc8ec2788558ab3', 'n0b978a5aaebe40c78eefc8ec2788558ab4']</t>
+          <t>['n528b0a2ec09f4001bf201ca376d90b6fb3', 'n528b0a2ec09f4001bf201ca376d90b6fb4']</t>
         </is>
       </c>
       <c r="BP30" t="inlineStr"/>
@@ -8046,10 +8046,10 @@
       </c>
       <c r="AS31" t="inlineStr"/>
       <c r="AT31" t="n">
-        <v>0.04</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="AU31" t="n">
-        <v>0.04</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="AV31" t="inlineStr"/>
       <c r="AW31" t="inlineStr"/>
@@ -8099,12 +8099,12 @@
       <c r="BM31" t="inlineStr"/>
       <c r="BN31" t="inlineStr">
         <is>
-          <t>nc7f2d50f26b344c788295c2b2276737ab1</t>
+          <t>n75b77a0c456b4ce4a2b6d44c45bf6fc2b1</t>
         </is>
       </c>
       <c r="BO31" t="inlineStr">
         <is>
-          <t>['nc7f2d50f26b344c788295c2b2276737ab1']</t>
+          <t>['n75b77a0c456b4ce4a2b6d44c45bf6fc2b1']</t>
         </is>
       </c>
       <c r="BP31" t="inlineStr"/>
@@ -8323,10 +8323,10 @@
       <c r="AR32" t="inlineStr"/>
       <c r="AS32" t="inlineStr"/>
       <c r="AT32" t="n">
-        <v>0.04</v>
+        <v>0.79</v>
       </c>
       <c r="AU32" t="n">
-        <v>0.04</v>
+        <v>0.79</v>
       </c>
       <c r="AV32" t="inlineStr"/>
       <c r="AW32" t="inlineStr"/>
@@ -8368,22 +8368,22 @@
       <c r="BM32" t="inlineStr"/>
       <c r="BN32" t="inlineStr">
         <is>
-          <t>n1796c93f31974dcd9cfc5638e185f8e7b1</t>
+          <t>naeb95d73e3484ab2bc430d97e4424b0eb1</t>
         </is>
       </c>
       <c r="BO32" t="inlineStr">
         <is>
-          <t>['n1796c93f31974dcd9cfc5638e185f8e7b1']</t>
+          <t>['naeb95d73e3484ab2bc430d97e4424b0eb1']</t>
         </is>
       </c>
       <c r="BP32" t="inlineStr">
         <is>
-          <t>n1796c93f31974dcd9cfc5638e185f8e7b3</t>
+          <t>naeb95d73e3484ab2bc430d97e4424b0eb3</t>
         </is>
       </c>
       <c r="BQ32" t="inlineStr">
         <is>
-          <t>n1796c93f31974dcd9cfc5638e185f8e7b3</t>
+          <t>naeb95d73e3484ab2bc430d97e4424b0eb3</t>
         </is>
       </c>
       <c r="BR32" t="inlineStr">
@@ -8825,10 +8825,10 @@
       </c>
       <c r="AS34" t="inlineStr"/>
       <c r="AT34" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="AU34" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="AV34" t="inlineStr"/>
       <c r="AW34" t="inlineStr"/>
@@ -9087,10 +9087,10 @@
       </c>
       <c r="AS35" t="inlineStr"/>
       <c r="AT35" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="AU35" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="AV35" t="inlineStr"/>
       <c r="AW35" t="inlineStr"/>
@@ -9361,10 +9361,10 @@
       </c>
       <c r="AS36" t="inlineStr"/>
       <c r="AT36" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="AU36" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="AV36" t="inlineStr">
         <is>
@@ -9629,10 +9629,10 @@
       <c r="AR37" t="inlineStr"/>
       <c r="AS37" t="inlineStr"/>
       <c r="AT37" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AU37" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AV37" t="inlineStr"/>
       <c r="AW37" t="inlineStr"/>
@@ -9911,10 +9911,10 @@
       </c>
       <c r="AS38" t="inlineStr"/>
       <c r="AT38" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AU38" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AV38" t="inlineStr"/>
       <c r="AW38" t="inlineStr"/>
@@ -10185,10 +10185,10 @@
       </c>
       <c r="AS39" t="inlineStr"/>
       <c r="AT39" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AU39" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AV39" t="inlineStr">
         <is>
@@ -10437,10 +10437,10 @@
       <c r="AR40" t="inlineStr"/>
       <c r="AS40" t="inlineStr"/>
       <c r="AT40" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AU40" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AV40" t="inlineStr"/>
       <c r="AW40" t="inlineStr"/>
@@ -10713,10 +10713,10 @@
       </c>
       <c r="AS41" t="inlineStr"/>
       <c r="AT41" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AU41" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AV41" t="inlineStr"/>
       <c r="AW41" t="inlineStr"/>
@@ -10979,10 +10979,10 @@
       <c r="AR42" t="inlineStr"/>
       <c r="AS42" t="inlineStr"/>
       <c r="AT42" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AU42" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AV42" t="inlineStr"/>
       <c r="AW42" t="inlineStr"/>
@@ -11261,10 +11261,10 @@
       </c>
       <c r="AS43" t="inlineStr"/>
       <c r="AT43" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AU43" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AV43" t="inlineStr"/>
       <c r="AW43" t="inlineStr"/>
@@ -11497,10 +11497,10 @@
       <c r="AR44" t="inlineStr"/>
       <c r="AS44" t="inlineStr"/>
       <c r="AT44" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AU44" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AV44" t="inlineStr"/>
       <c r="AW44" t="inlineStr"/>
@@ -11737,10 +11737,10 @@
       </c>
       <c r="AS45" t="inlineStr"/>
       <c r="AT45" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AU45" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AV45" t="inlineStr"/>
       <c r="AW45" t="inlineStr"/>
@@ -11991,10 +11991,10 @@
       </c>
       <c r="AS46" t="inlineStr"/>
       <c r="AT46" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AU46" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="AV46" t="inlineStr"/>
       <c r="AW46" t="inlineStr"/>
@@ -13158,20 +13158,20 @@
       </c>
       <c r="AQ51" t="inlineStr">
         <is>
-          <t>aoi, contax, cto, fmo, hmo</t>
+          <t>aoi, contax, cto, fmo, hmo, rdo</t>
         </is>
       </c>
       <c r="AR51" t="inlineStr">
         <is>
-          <t>aoi, contax, cto, fmo, hmo</t>
+          <t>aoi, contax, cto, fmo, hmo, rdo</t>
         </is>
       </c>
       <c r="AS51" t="inlineStr"/>
       <c r="AT51" t="n">
-        <v>0.04</v>
+        <v>0.86</v>
       </c>
       <c r="AU51" t="n">
-        <v>0.04</v>
+        <v>0.86</v>
       </c>
       <c r="AV51" t="inlineStr"/>
       <c r="AW51" t="inlineStr"/>
@@ -13221,12 +13221,12 @@
       </c>
       <c r="BN51" t="inlineStr">
         <is>
-          <t>n256aa1983fc74e34b54e0bca922c8324b1, https://www.researchgate.net/profile/Mathias_Bonduel</t>
+          <t>n8988c478d0574088a599efd11381e1dbb1, https://www.researchgate.net/profile/Mathias_Bonduel</t>
         </is>
       </c>
       <c r="BO51" t="inlineStr">
         <is>
-          <t>['n256aa1983fc74e34b54e0bca922c8324b1', 'https://www.researchgate.net/profile/Mathias_Bonduel']</t>
+          <t>['n8988c478d0574088a599efd11381e1dbb1', 'https://www.researchgate.net/profile/Mathias_Bonduel']</t>
         </is>
       </c>
       <c r="BP51" t="inlineStr"/>
@@ -13430,10 +13430,10 @@
       <c r="AR52" t="inlineStr"/>
       <c r="AS52" t="inlineStr"/>
       <c r="AT52" t="n">
-        <v>0.04</v>
+        <v>0.72</v>
       </c>
       <c r="AU52" t="n">
-        <v>0.04</v>
+        <v>0.72</v>
       </c>
       <c r="AV52" t="inlineStr"/>
       <c r="AW52" t="inlineStr"/>
@@ -13946,10 +13946,10 @@
       <c r="AR54" t="inlineStr"/>
       <c r="AS54" t="inlineStr"/>
       <c r="AT54" t="n">
-        <v>0.53</v>
+        <v>0.64</v>
       </c>
       <c r="AU54" t="n">
-        <v>0.53</v>
+        <v>0.64</v>
       </c>
       <c r="AV54" t="inlineStr"/>
       <c r="AW54" t="inlineStr"/>
@@ -14198,10 +14198,10 @@
       <c r="AR55" t="inlineStr"/>
       <c r="AS55" t="inlineStr"/>
       <c r="AT55" t="n">
-        <v>0.04</v>
+        <v>0.68</v>
       </c>
       <c r="AU55" t="n">
-        <v>0.04</v>
+        <v>0.68</v>
       </c>
       <c r="AV55" t="inlineStr"/>
       <c r="AW55" t="inlineStr"/>
@@ -15458,10 +15458,10 @@
       <c r="AR60" t="inlineStr"/>
       <c r="AS60" t="inlineStr"/>
       <c r="AT60" t="n">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="AU60" t="n">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="AV60" t="inlineStr"/>
       <c r="AW60" t="inlineStr"/>
@@ -15898,10 +15898,10 @@
       <c r="AR62" t="inlineStr"/>
       <c r="AS62" t="inlineStr"/>
       <c r="AT62" t="n">
-        <v>0.15</v>
+        <v>0.08</v>
       </c>
       <c r="AU62" t="n">
-        <v>0.15</v>
+        <v>0.08</v>
       </c>
       <c r="AV62" t="inlineStr"/>
       <c r="AW62" t="inlineStr"/>
@@ -17605,12 +17605,12 @@
       </c>
       <c r="BP69" t="inlineStr">
         <is>
-          <t>n73008469406e431a8e9f1f427528e081b1</t>
+          <t>nb6c1030bc15140b7bd8315f7f6f94786b1</t>
         </is>
       </c>
       <c r="BQ69" t="inlineStr">
         <is>
-          <t>n73008469406e431a8e9f1f427528e081b1</t>
+          <t>nb6c1030bc15140b7bd8315f7f6f94786b1</t>
         </is>
       </c>
       <c r="BR69" t="inlineStr">
@@ -18635,22 +18635,22 @@
       <c r="BM73" t="inlineStr"/>
       <c r="BN73" t="inlineStr">
         <is>
-          <t>ne166b15af3114df2941d5735e52ac17cb1</t>
+          <t>n322a3f8a18eb426d92e8d3ef551d0041b1</t>
         </is>
       </c>
       <c r="BO73" t="inlineStr">
         <is>
-          <t>['ne166b15af3114df2941d5735e52ac17cb1']</t>
+          <t>['n322a3f8a18eb426d92e8d3ef551d0041b1']</t>
         </is>
       </c>
       <c r="BP73" t="inlineStr">
         <is>
-          <t>ne166b15af3114df2941d5735e52ac17cb3</t>
+          <t>n322a3f8a18eb426d92e8d3ef551d0041b3</t>
         </is>
       </c>
       <c r="BQ73" t="inlineStr">
         <is>
-          <t>ne166b15af3114df2941d5735e52ac17cb3</t>
+          <t>n322a3f8a18eb426d92e8d3ef551d0041b3</t>
         </is>
       </c>
       <c r="BR73" t="inlineStr">
@@ -19139,12 +19139,12 @@
       <c r="BM75" t="inlineStr"/>
       <c r="BN75" t="inlineStr">
         <is>
-          <t>n1fc0ae429aec4e4492fd225212dfaee9b1, n1fc0ae429aec4e4492fd225212dfaee9b2</t>
+          <t>n369e74fd059b47afb4c6368aef845a00b1, n369e74fd059b47afb4c6368aef845a00b2</t>
         </is>
       </c>
       <c r="BO75" t="inlineStr">
         <is>
-          <t>['n1fc0ae429aec4e4492fd225212dfaee9b1', 'n1fc0ae429aec4e4492fd225212dfaee9b2']</t>
+          <t>['n369e74fd059b47afb4c6368aef845a00b1', 'n369e74fd059b47afb4c6368aef845a00b2']</t>
         </is>
       </c>
       <c r="BP75" t="inlineStr"/>
@@ -20208,22 +20208,22 @@
       <c r="BM79" t="inlineStr"/>
       <c r="BN79" t="inlineStr">
         <is>
-          <t>nc847728842c3437796451e6cf952805ab3, nc847728842c3437796451e6cf952805ab5</t>
+          <t>ncaed24a5ea4d44998ff20c016f30195bb3, ncaed24a5ea4d44998ff20c016f30195bb5</t>
         </is>
       </c>
       <c r="BO79" t="inlineStr">
         <is>
-          <t>['nc847728842c3437796451e6cf952805ab3', 'nc847728842c3437796451e6cf952805ab5']</t>
+          <t>['ncaed24a5ea4d44998ff20c016f30195bb3', 'ncaed24a5ea4d44998ff20c016f30195bb5']</t>
         </is>
       </c>
       <c r="BP79" t="inlineStr">
         <is>
-          <t>nc847728842c3437796451e6cf952805ab7</t>
+          <t>ncaed24a5ea4d44998ff20c016f30195bb7</t>
         </is>
       </c>
       <c r="BQ79" t="inlineStr">
         <is>
-          <t>nc847728842c3437796451e6cf952805ab7</t>
+          <t>ncaed24a5ea4d44998ff20c016f30195bb7</t>
         </is>
       </c>
       <c r="BR79" t="inlineStr">
@@ -21149,22 +21149,22 @@
       <c r="BM83" t="inlineStr"/>
       <c r="BN83" t="inlineStr">
         <is>
-          <t>na308a401dd8246698d1dd76a69e08237b3, na308a401dd8246698d1dd76a69e08237b5</t>
+          <t>nbc624cf109b04f1da74ad7cf69c51c79b3, nbc624cf109b04f1da74ad7cf69c51c79b5</t>
         </is>
       </c>
       <c r="BO83" t="inlineStr">
         <is>
-          <t>['na308a401dd8246698d1dd76a69e08237b3', 'na308a401dd8246698d1dd76a69e08237b5']</t>
+          <t>['nbc624cf109b04f1da74ad7cf69c51c79b3', 'nbc624cf109b04f1da74ad7cf69c51c79b5']</t>
         </is>
       </c>
       <c r="BP83" t="inlineStr">
         <is>
-          <t>na308a401dd8246698d1dd76a69e08237b7</t>
+          <t>nbc624cf109b04f1da74ad7cf69c51c79b7</t>
         </is>
       </c>
       <c r="BQ83" t="inlineStr">
         <is>
-          <t>na308a401dd8246698d1dd76a69e08237b7</t>
+          <t>nbc624cf109b04f1da74ad7cf69c51c79b7</t>
         </is>
       </c>
       <c r="BR83" t="inlineStr">
@@ -21947,12 +21947,12 @@
       </c>
       <c r="BN86" t="inlineStr">
         <is>
-          <t>nd91e0dd233d748ff9d0e66f8f15c7d32b1</t>
+          <t>nc3430a98e20a4a29b29fc799547c2b0cb1</t>
         </is>
       </c>
       <c r="BO86" t="inlineStr">
         <is>
-          <t>['nd91e0dd233d748ff9d0e66f8f15c7d32b1']</t>
+          <t>['nc3430a98e20a4a29b29fc799547c2b0cb1']</t>
         </is>
       </c>
       <c r="BP86" t="inlineStr"/>
@@ -24478,12 +24478,12 @@
       <c r="BM97" t="inlineStr"/>
       <c r="BN97" t="inlineStr">
         <is>
-          <t>n9ba7776daae74af7a43db8f9490bac1ab1, n9ba7776daae74af7a43db8f9490bac1ab2</t>
+          <t>n87bac52c16bb47d08a97ec8b5a5f5bc8b1, n87bac52c16bb47d08a97ec8b5a5f5bc8b2</t>
         </is>
       </c>
       <c r="BO97" t="inlineStr">
         <is>
-          <t>['n9ba7776daae74af7a43db8f9490bac1ab1', 'n9ba7776daae74af7a43db8f9490bac1ab2']</t>
+          <t>['n87bac52c16bb47d08a97ec8b5a5f5bc8b1', 'n87bac52c16bb47d08a97ec8b5a5f5bc8b2']</t>
         </is>
       </c>
       <c r="BP97" t="inlineStr"/>
@@ -26644,10 +26644,10 @@
       <c r="AR106" t="inlineStr"/>
       <c r="AS106" t="inlineStr"/>
       <c r="AT106" t="n">
-        <v>0.93</v>
+        <v>0.89</v>
       </c>
       <c r="AU106" t="n">
-        <v>0.93</v>
+        <v>0.89</v>
       </c>
       <c r="AV106" t="inlineStr"/>
       <c r="AW106" t="inlineStr"/>
@@ -29920,12 +29920,8 @@
       <c r="AQ117" t="inlineStr"/>
       <c r="AR117" t="inlineStr"/>
       <c r="AS117" t="inlineStr"/>
-      <c r="AT117" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="AU117" t="n">
-        <v>0.9</v>
-      </c>
+      <c r="AT117" t="inlineStr"/>
+      <c r="AU117" t="inlineStr"/>
       <c r="AV117" t="inlineStr"/>
       <c r="AW117" t="inlineStr"/>
       <c r="AX117" t="inlineStr"/>
@@ -30723,10 +30719,10 @@
       <c r="AR120" t="inlineStr"/>
       <c r="AS120" t="inlineStr"/>
       <c r="AT120" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="AU120" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="AV120" t="inlineStr"/>
       <c r="AW120" t="inlineStr"/>
@@ -32858,12 +32854,12 @@
       <c r="BM129" t="inlineStr"/>
       <c r="BN129" t="inlineStr">
         <is>
-          <t>nc89c61f8f25f4907b5a7d0060c5a373eb1</t>
+          <t>n278c491c2734435291fb311446c9dd86b1</t>
         </is>
       </c>
       <c r="BO129" t="inlineStr">
         <is>
-          <t>['nc89c61f8f25f4907b5a7d0060c5a373eb1']</t>
+          <t>['n278c491c2734435291fb311446c9dd86b1']</t>
         </is>
       </c>
       <c r="BP129" t="inlineStr"/>
@@ -33128,12 +33124,12 @@
       <c r="BM130" t="inlineStr"/>
       <c r="BN130" t="inlineStr">
         <is>
-          <t>n8ab0ee428f9f4bb8a7d0506919637400b1</t>
+          <t>nb9de99644e1a4ab0a595df488e393c0bb1</t>
         </is>
       </c>
       <c r="BO130" t="inlineStr">
         <is>
-          <t>['n8ab0ee428f9f4bb8a7d0506919637400b1']</t>
+          <t>['nb9de99644e1a4ab0a595df488e393c0bb1']</t>
         </is>
       </c>
       <c r="BP130" t="inlineStr"/>
@@ -33649,22 +33645,22 @@
       </c>
       <c r="BN132" t="inlineStr">
         <is>
-          <t>n061ec797826f4bfdbc7ac7d7d80d8732b1, n061ec797826f4bfdbc7ac7d7d80d8732b3, n061ec797826f4bfdbc7ac7d7d80d8732b5, n061ec797826f4bfdbc7ac7d7d80d8732b7</t>
+          <t>n34dc5491c0c54188a2ce0a6a1f24326db1, n34dc5491c0c54188a2ce0a6a1f24326db3, n34dc5491c0c54188a2ce0a6a1f24326db5, n34dc5491c0c54188a2ce0a6a1f24326db7</t>
         </is>
       </c>
       <c r="BO132" t="inlineStr">
         <is>
-          <t>['n061ec797826f4bfdbc7ac7d7d80d8732b1', 'n061ec797826f4bfdbc7ac7d7d80d8732b3', 'n061ec797826f4bfdbc7ac7d7d80d8732b5', 'n061ec797826f4bfdbc7ac7d7d80d8732b7']</t>
+          <t>['n34dc5491c0c54188a2ce0a6a1f24326db1', 'n34dc5491c0c54188a2ce0a6a1f24326db3', 'n34dc5491c0c54188a2ce0a6a1f24326db5', 'n34dc5491c0c54188a2ce0a6a1f24326db7']</t>
         </is>
       </c>
       <c r="BP132" t="inlineStr">
         <is>
-          <t>n061ec797826f4bfdbc7ac7d7d80d8732b9</t>
+          <t>n34dc5491c0c54188a2ce0a6a1f24326db9</t>
         </is>
       </c>
       <c r="BQ132" t="inlineStr">
         <is>
-          <t>n061ec797826f4bfdbc7ac7d7d80d8732b9</t>
+          <t>n34dc5491c0c54188a2ce0a6a1f24326db9</t>
         </is>
       </c>
       <c r="BR132" t="inlineStr">
@@ -36274,6 +36270,278 @@
       </c>
       <c r="CD144" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>https://w3id.org/rdo#</t>
+        </is>
+      </c>
+      <c r="B145" t="b">
+        <v>1</v>
+      </c>
+      <c r="C145" t="inlineStr"/>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>rdo</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>rdo</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>rdo</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>Roof Damage Ontology</t>
+        </is>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>Roof Damage Ontology</t>
+        </is>
+      </c>
+      <c r="I145" t="inlineStr">
+        <is>
+          <t>Roof Damage Ontology</t>
+        </is>
+      </c>
+      <c r="J145" t="inlineStr">
+        <is>
+          <t>This ontology provides a semantic framework for representing roof condition inspection information, including roofs and roof pitches, inspections, orthophotos, and image-derived defect observations. It is designed to support structured documentation, querying, and interoperability within digital twin–based workflows for roof condition monitoring and maintenance, particularly in the context of existing and heritage buildings.</t>
+        </is>
+      </c>
+      <c r="K145" t="inlineStr">
+        <is>
+          <t>This ontology provides a semantic framework for representing roof condition inspection information, including roofs and roof pitches, inspections, orthophotos, and image-derived defect observations. It is designed to support structured documentation, querying, and interoperability within digital twin–based workflows for roof condition monitoring and maintenance, particularly in the context of existing and heritage buildings.</t>
+        </is>
+      </c>
+      <c r="L145" t="inlineStr">
+        <is>
+          <t>This ontology provides a semantic framework for representing roof condition inspection information, including roofs and roof pitches, inspections, orthophotos, and image-derived defect observations. It is designed to support structured documentation, querying, and interoperability within digital twin–based workflows for roof condition monitoring and maintenance, particularly in the context of existing and heritage buildings.</t>
+        </is>
+      </c>
+      <c r="M145" t="n">
+        <v>2026</v>
+      </c>
+      <c r="N145" t="inlineStr">
+        <is>
+          <t>2026-02-06</t>
+        </is>
+      </c>
+      <c r="O145" t="inlineStr"/>
+      <c r="P145" t="inlineStr"/>
+      <c r="Q145" t="inlineStr">
+        <is>
+          <t>2026-02-06</t>
+        </is>
+      </c>
+      <c r="R145" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC BY 4.0 </t>
+        </is>
+      </c>
+      <c r="S145" t="inlineStr">
+        <is>
+          <t>https://creativecommons.org/licenses/by/4.0/</t>
+        </is>
+      </c>
+      <c r="T145" t="inlineStr">
+        <is>
+          <t>https://creativecommons.org/licenses/by/4.0/</t>
+        </is>
+      </c>
+      <c r="U145" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="V145" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
+      <c r="W145" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
+      <c r="X145" t="inlineStr">
+        <is>
+          <t>dot, beo</t>
+        </is>
+      </c>
+      <c r="Y145" t="inlineStr">
+        <is>
+          <t>beo, dot</t>
+        </is>
+      </c>
+      <c r="Z145" t="inlineStr">
+        <is>
+          <t>beo, dot</t>
+        </is>
+      </c>
+      <c r="AA145" t="inlineStr">
+        <is>
+          <t>foaf, dcterms</t>
+        </is>
+      </c>
+      <c r="AB145" t="inlineStr">
+        <is>
+          <t>dc, dcterms, vann, schema, foaf, pi</t>
+        </is>
+      </c>
+      <c r="AC145" t="inlineStr">
+        <is>
+          <t>dc, dcterms, vann, schema, foaf, pi</t>
+        </is>
+      </c>
+      <c r="AD145" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE145" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF145" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG145" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH145" t="inlineStr"/>
+      <c r="AI145" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ145" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK145" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL145" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM145" t="n">
+        <v>79.40000000000001</v>
+      </c>
+      <c r="AN145" t="inlineStr"/>
+      <c r="AO145" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP145" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ145" t="inlineStr"/>
+      <c r="AR145" t="inlineStr"/>
+      <c r="AS145" t="inlineStr"/>
+      <c r="AT145" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="AU145" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="AV145" t="inlineStr"/>
+      <c r="AW145" t="inlineStr"/>
+      <c r="AX145" t="inlineStr"/>
+      <c r="AY145" t="b">
+        <v>0</v>
+      </c>
+      <c r="AZ145" t="inlineStr"/>
+      <c r="BA145" t="b">
+        <v>0</v>
+      </c>
+      <c r="BB145" t="inlineStr"/>
+      <c r="BC145" t="inlineStr"/>
+      <c r="BD145" t="inlineStr"/>
+      <c r="BE145" t="inlineStr"/>
+      <c r="BF145" t="inlineStr"/>
+      <c r="BG145" t="inlineStr"/>
+      <c r="BH145" t="inlineStr">
+        <is>
+          <t>Quality</t>
+        </is>
+      </c>
+      <c r="BI145" t="inlineStr"/>
+      <c r="BJ145" t="inlineStr">
+        <is>
+          <t>Quality</t>
+        </is>
+      </c>
+      <c r="BK145" t="inlineStr">
+        <is>
+          <t>Safety</t>
+        </is>
+      </c>
+      <c r="BL145" t="inlineStr"/>
+      <c r="BM145" t="inlineStr">
+        <is>
+          <t>Safety</t>
+        </is>
+      </c>
+      <c r="BN145" t="inlineStr">
+        <is>
+          <t>Frederic Bosche, University of Edinburgh, Jiajun Li, University of Edinburgh</t>
+        </is>
+      </c>
+      <c r="BO145" t="inlineStr">
+        <is>
+          <t>['Frederic Bosche, University of Edinburgh', 'Jiajun Li, University of Edinburgh']</t>
+        </is>
+      </c>
+      <c r="BP145" t="inlineStr">
+        <is>
+          <t>Cyberbuild, University of Edinburgh</t>
+        </is>
+      </c>
+      <c r="BQ145" t="inlineStr">
+        <is>
+          <t>Cyberbuild, University of Edinburgh</t>
+        </is>
+      </c>
+      <c r="BR145" t="inlineStr">
+        <is>
+          <t>{owl: http://www.w3.org/2002/07/owl#}, {rdf: http://www.w3.org/1999/02/22-rdf-syntax-ns#}, {xsd: http://www.w3.org/2001/XMLSchema#}, {rdfs: http://www.w3.org/2000/01/rdf-schema#}, {None: http://lcweb.loc.gov/catdir/cpso/lcco/}, {None: http://lcweb.loc.gov/standards/iso639-2/}, {None: http://purl.org/dc/aboutdcmi#}, {None: http://purl.org/dc/dcam/}, {None: http://purl.org/dc/dcmitype/}, {dc: http://purl.org/dc/elements/1.1/}, {dcterms: http://purl.org/dc/terms/}, {None: http://purl.org/spar/}, {vann: http://purl.org/vocab/vann/}, {schema: http://schema.org/#}, {None: http://webprotege.stanford.edu/}, {None: http://www.getty.edu/research/tools/vocabulary/tgn/}, {None: http://www.iana.org/assignments/media-types/}, {None: http://www.ietf.org/rfc/}, {None: http://www.nlm.nih.gov/mesh/}, {None: http://www.oclc.org/dewey/}, {None: http://www.sil.org/iso639-3/}, {None: http://www.udcc.org/}, {None: http://www.w3.org/TR/}, {None: http://wwwcf.nlm.nih.gov/class/}, {foaf: http://xmlns.com/foaf/0.1/}, {pi: https://pi.pauwel.be/voc/}, {beo: https://pi.pauwel.be/voc/buildingelement#}, {dot: https://w3id.org/dot#}, {None: https://www.dublincore.org/specifications/dublin-core/dcmi-box/}, {None: https://www.dublincore.org/specifications/dublin-core/dcmi-period/}, {None: https://www.dublincore.org/specifications/dublin-core/dcmi-point/}, {None: https://www.iso.org/obp/ui/#}</t>
+        </is>
+      </c>
+      <c r="BS145" t="n">
+        <v>38</v>
+      </c>
+      <c r="BT145" t="n">
+        <v>38</v>
+      </c>
+      <c r="BU145" t="n">
+        <v>31</v>
+      </c>
+      <c r="BV145" t="n">
+        <v>31</v>
+      </c>
+      <c r="BW145" t="n">
+        <v>11</v>
+      </c>
+      <c r="BX145" t="n">
+        <v>11</v>
+      </c>
+      <c r="BY145" t="b">
+        <v>1</v>
+      </c>
+      <c r="BZ145" t="b">
+        <v>1</v>
+      </c>
+      <c r="CA145" t="b">
+        <v>0</v>
+      </c>
+      <c r="CB145" t="n">
+        <v>2</v>
+      </c>
+      <c r="CC145" t="n">
+        <v>2</v>
+      </c>
+      <c r="CD145" t="n">
+        <v>1.8</v>
       </c>
     </row>
   </sheetData>
@@ -36505,13 +36773,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D6D156-9A71-4D0D-8DA3-DC2EB8492A46}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A1A2FC8-8B41-498F-B6B0-90893F088D3F}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18D1B2F6-9009-4F71-A0D9-2DB6E1869A69}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA3049ED-834F-48B6-BF51-A5106EC2732B}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC3806F6-5A8F-4142-AC58-B0E4B4378BA9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{575C3B20-B428-4B0C-9F1A-789C1C8844F0}"/>
 </file>
</xml_diff>